<commit_message>
searching for an approach
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>floor</t>
   </si>
@@ -136,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -166,6 +166,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1725,11 +1728,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC207"/>
+  <dimension ref="A1:AF207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S190" sqref="S190"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U198" sqref="U198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1744,7 @@
     <col min="6" max="7" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,11 +1781,14 @@
       <c r="T1" s="6"/>
       <c r="U1" s="7"/>
       <c r="V1" s="8"/>
-      <c r="W1" s="7"/>
+      <c r="W1" s="6"/>
       <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -1807,11 +1813,14 @@
       <c r="T2" s="6"/>
       <c r="U2" s="7"/>
       <c r="V2" s="8"/>
-      <c r="W2" s="7"/>
+      <c r="W2" s="6"/>
       <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>199</v>
       </c>
@@ -1836,11 +1845,14 @@
       <c r="T3" s="6"/>
       <c r="U3" s="7"/>
       <c r="V3" s="8"/>
-      <c r="W3" s="7"/>
+      <c r="W3" s="6"/>
       <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>198</v>
       </c>
@@ -1865,11 +1877,14 @@
       <c r="T4" s="6"/>
       <c r="U4" s="7"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="7"/>
+      <c r="W4" s="6"/>
       <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>197</v>
       </c>
@@ -1894,11 +1909,14 @@
       <c r="T5" s="6"/>
       <c r="U5" s="7"/>
       <c r="V5" s="8"/>
-      <c r="W5" s="7"/>
+      <c r="W5" s="6"/>
       <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>196</v>
       </c>
@@ -1923,11 +1941,14 @@
       <c r="T6" s="6"/>
       <c r="U6" s="7"/>
       <c r="V6" s="8"/>
-      <c r="W6" s="7"/>
+      <c r="W6" s="6"/>
       <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>195</v>
       </c>
@@ -1952,11 +1973,14 @@
       <c r="T7" s="6"/>
       <c r="U7" s="7"/>
       <c r="V7" s="8"/>
-      <c r="W7" s="7"/>
+      <c r="W7" s="6"/>
       <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>194</v>
       </c>
@@ -1981,11 +2005,14 @@
       <c r="T8" s="6"/>
       <c r="U8" s="7"/>
       <c r="V8" s="8"/>
-      <c r="W8" s="7"/>
+      <c r="W8" s="6"/>
       <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>193</v>
       </c>
@@ -2010,11 +2037,14 @@
       <c r="T9" s="6"/>
       <c r="U9" s="7"/>
       <c r="V9" s="8"/>
-      <c r="W9" s="7"/>
+      <c r="W9" s="6"/>
       <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>192</v>
       </c>
@@ -2039,11 +2069,14 @@
       <c r="T10" s="6"/>
       <c r="U10" s="7"/>
       <c r="V10" s="8"/>
-      <c r="W10" s="7"/>
+      <c r="W10" s="6"/>
       <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>191</v>
       </c>
@@ -2068,11 +2101,14 @@
       <c r="T11" s="6"/>
       <c r="U11" s="7"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="7"/>
+      <c r="W11" s="6"/>
       <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>190</v>
       </c>
@@ -2097,11 +2133,14 @@
       <c r="T12" s="6"/>
       <c r="U12" s="7"/>
       <c r="V12" s="8"/>
-      <c r="W12" s="7"/>
+      <c r="W12" s="6"/>
       <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>189</v>
       </c>
@@ -2126,11 +2165,14 @@
       <c r="T13" s="6"/>
       <c r="U13" s="7"/>
       <c r="V13" s="8"/>
-      <c r="W13" s="7"/>
+      <c r="W13" s="6"/>
       <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>188</v>
       </c>
@@ -2155,11 +2197,14 @@
       <c r="T14" s="6"/>
       <c r="U14" s="7"/>
       <c r="V14" s="8"/>
-      <c r="W14" s="7"/>
+      <c r="W14" s="6"/>
       <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>187</v>
       </c>
@@ -2184,11 +2229,14 @@
       <c r="T15" s="6"/>
       <c r="U15" s="7"/>
       <c r="V15" s="8"/>
-      <c r="W15" s="7"/>
+      <c r="W15" s="6"/>
       <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>186</v>
       </c>
@@ -2213,11 +2261,14 @@
       <c r="T16" s="6"/>
       <c r="U16" s="7"/>
       <c r="V16" s="8"/>
-      <c r="W16" s="7"/>
+      <c r="W16" s="6"/>
       <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>185</v>
       </c>
@@ -2242,11 +2293,14 @@
       <c r="T17" s="6"/>
       <c r="U17" s="7"/>
       <c r="V17" s="8"/>
-      <c r="W17" s="7"/>
+      <c r="W17" s="6"/>
       <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>184</v>
       </c>
@@ -2271,11 +2325,14 @@
       <c r="T18" s="6"/>
       <c r="U18" s="7"/>
       <c r="V18" s="8"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="6"/>
       <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>183</v>
       </c>
@@ -2300,11 +2357,14 @@
       <c r="T19" s="6"/>
       <c r="U19" s="7"/>
       <c r="V19" s="8"/>
-      <c r="W19" s="7"/>
+      <c r="W19" s="6"/>
       <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>182</v>
       </c>
@@ -2329,11 +2389,14 @@
       <c r="T20" s="6"/>
       <c r="U20" s="7"/>
       <c r="V20" s="8"/>
-      <c r="W20" s="7"/>
+      <c r="W20" s="6"/>
       <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>181</v>
       </c>
@@ -2358,11 +2421,14 @@
       <c r="T21" s="6"/>
       <c r="U21" s="7"/>
       <c r="V21" s="8"/>
-      <c r="W21" s="7"/>
+      <c r="W21" s="6"/>
       <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>180</v>
       </c>
@@ -2387,11 +2453,14 @@
       <c r="T22" s="6"/>
       <c r="U22" s="7"/>
       <c r="V22" s="8"/>
-      <c r="W22" s="7"/>
+      <c r="W22" s="6"/>
       <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>179</v>
       </c>
@@ -2416,11 +2485,14 @@
       <c r="T23" s="6"/>
       <c r="U23" s="7"/>
       <c r="V23" s="8"/>
-      <c r="W23" s="7"/>
+      <c r="W23" s="6"/>
       <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>178</v>
       </c>
@@ -2445,11 +2517,14 @@
       <c r="T24" s="6"/>
       <c r="U24" s="7"/>
       <c r="V24" s="8"/>
-      <c r="W24" s="7"/>
+      <c r="W24" s="6"/>
       <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>177</v>
       </c>
@@ -2474,11 +2549,14 @@
       <c r="T25" s="6"/>
       <c r="U25" s="7"/>
       <c r="V25" s="8"/>
-      <c r="W25" s="7"/>
+      <c r="W25" s="6"/>
       <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>176</v>
       </c>
@@ -2503,11 +2581,14 @@
       <c r="T26" s="6"/>
       <c r="U26" s="7"/>
       <c r="V26" s="8"/>
-      <c r="W26" s="7"/>
+      <c r="W26" s="6"/>
       <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>175</v>
       </c>
@@ -2532,11 +2613,14 @@
       <c r="T27" s="6"/>
       <c r="U27" s="7"/>
       <c r="V27" s="8"/>
-      <c r="W27" s="7"/>
+      <c r="W27" s="6"/>
       <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>174</v>
       </c>
@@ -2561,11 +2645,14 @@
       <c r="T28" s="6"/>
       <c r="U28" s="7"/>
       <c r="V28" s="8"/>
-      <c r="W28" s="7"/>
+      <c r="W28" s="6"/>
       <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>173</v>
       </c>
@@ -2590,11 +2677,14 @@
       <c r="T29" s="6"/>
       <c r="U29" s="7"/>
       <c r="V29" s="8"/>
-      <c r="W29" s="7"/>
+      <c r="W29" s="6"/>
       <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>172</v>
       </c>
@@ -2619,11 +2709,14 @@
       <c r="T30" s="6"/>
       <c r="U30" s="7"/>
       <c r="V30" s="8"/>
-      <c r="W30" s="7"/>
+      <c r="W30" s="6"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>171</v>
       </c>
@@ -2648,11 +2741,14 @@
       <c r="T31" s="6"/>
       <c r="U31" s="7"/>
       <c r="V31" s="8"/>
-      <c r="W31" s="7"/>
+      <c r="W31" s="6"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>170</v>
       </c>
@@ -2677,11 +2773,14 @@
       <c r="T32" s="6"/>
       <c r="U32" s="7"/>
       <c r="V32" s="8"/>
-      <c r="W32" s="7"/>
+      <c r="W32" s="6"/>
       <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>169</v>
       </c>
@@ -2706,11 +2805,14 @@
       <c r="T33" s="6"/>
       <c r="U33" s="7"/>
       <c r="V33" s="8"/>
-      <c r="W33" s="7"/>
+      <c r="W33" s="6"/>
       <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>168</v>
       </c>
@@ -2735,11 +2837,14 @@
       <c r="T34" s="6"/>
       <c r="U34" s="7"/>
       <c r="V34" s="8"/>
-      <c r="W34" s="7"/>
+      <c r="W34" s="6"/>
       <c r="X34" s="7"/>
-      <c r="Y34" s="7"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>167</v>
       </c>
@@ -2764,11 +2869,14 @@
       <c r="T35" s="6"/>
       <c r="U35" s="7"/>
       <c r="V35" s="8"/>
-      <c r="W35" s="7"/>
+      <c r="W35" s="6"/>
       <c r="X35" s="7"/>
-      <c r="Y35" s="7"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>166</v>
       </c>
@@ -2793,11 +2901,14 @@
       <c r="T36" s="6"/>
       <c r="U36" s="7"/>
       <c r="V36" s="8"/>
-      <c r="W36" s="7"/>
+      <c r="W36" s="6"/>
       <c r="X36" s="7"/>
-      <c r="Y36" s="7"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>165</v>
       </c>
@@ -2822,11 +2933,14 @@
       <c r="T37" s="6"/>
       <c r="U37" s="7"/>
       <c r="V37" s="8"/>
-      <c r="W37" s="7"/>
+      <c r="W37" s="6"/>
       <c r="X37" s="7"/>
-      <c r="Y37" s="7"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>164</v>
       </c>
@@ -2851,11 +2965,14 @@
       <c r="T38" s="6"/>
       <c r="U38" s="7"/>
       <c r="V38" s="8"/>
-      <c r="W38" s="7"/>
+      <c r="W38" s="6"/>
       <c r="X38" s="7"/>
-      <c r="Y38" s="7"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>163</v>
       </c>
@@ -2880,11 +2997,14 @@
       <c r="T39" s="6"/>
       <c r="U39" s="7"/>
       <c r="V39" s="8"/>
-      <c r="W39" s="7"/>
+      <c r="W39" s="6"/>
       <c r="X39" s="7"/>
-      <c r="Y39" s="7"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>162</v>
       </c>
@@ -2909,11 +3029,14 @@
       <c r="T40" s="6"/>
       <c r="U40" s="7"/>
       <c r="V40" s="8"/>
-      <c r="W40" s="7"/>
+      <c r="W40" s="6"/>
       <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="7"/>
+      <c r="AB40" s="7"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>161</v>
       </c>
@@ -2938,11 +3061,14 @@
       <c r="T41" s="6"/>
       <c r="U41" s="7"/>
       <c r="V41" s="8"/>
-      <c r="W41" s="7"/>
+      <c r="W41" s="6"/>
       <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="7"/>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>160</v>
       </c>
@@ -2967,11 +3093,14 @@
       <c r="T42" s="6"/>
       <c r="U42" s="7"/>
       <c r="V42" s="8"/>
-      <c r="W42" s="7"/>
+      <c r="W42" s="6"/>
       <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="7"/>
+      <c r="AA42" s="7"/>
+      <c r="AB42" s="7"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>159</v>
       </c>
@@ -2996,11 +3125,14 @@
       <c r="T43" s="6"/>
       <c r="U43" s="7"/>
       <c r="V43" s="8"/>
-      <c r="W43" s="7"/>
+      <c r="W43" s="6"/>
       <c r="X43" s="7"/>
-      <c r="Y43" s="7"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y43" s="8"/>
+      <c r="Z43" s="7"/>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>158</v>
       </c>
@@ -3025,11 +3157,14 @@
       <c r="T44" s="6"/>
       <c r="U44" s="7"/>
       <c r="V44" s="8"/>
-      <c r="W44" s="7"/>
+      <c r="W44" s="6"/>
       <c r="X44" s="7"/>
-      <c r="Y44" s="7"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="7"/>
+      <c r="AA44" s="7"/>
+      <c r="AB44" s="7"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>157</v>
       </c>
@@ -3054,11 +3189,14 @@
       <c r="T45" s="6"/>
       <c r="U45" s="7"/>
       <c r="V45" s="8"/>
-      <c r="W45" s="7"/>
+      <c r="W45" s="6"/>
       <c r="X45" s="7"/>
-      <c r="Y45" s="7"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y45" s="8"/>
+      <c r="Z45" s="7"/>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>156</v>
       </c>
@@ -3083,11 +3221,14 @@
       <c r="T46" s="6"/>
       <c r="U46" s="7"/>
       <c r="V46" s="8"/>
-      <c r="W46" s="7"/>
+      <c r="W46" s="6"/>
       <c r="X46" s="7"/>
-      <c r="Y46" s="7"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="7"/>
+      <c r="AB46" s="7"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>155</v>
       </c>
@@ -3112,11 +3253,14 @@
       <c r="T47" s="6"/>
       <c r="U47" s="7"/>
       <c r="V47" s="8"/>
-      <c r="W47" s="7"/>
+      <c r="W47" s="6"/>
       <c r="X47" s="7"/>
-      <c r="Y47" s="7"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y47" s="8"/>
+      <c r="Z47" s="7"/>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7"/>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>154</v>
       </c>
@@ -3141,11 +3285,14 @@
       <c r="T48" s="6"/>
       <c r="U48" s="7"/>
       <c r="V48" s="8"/>
-      <c r="W48" s="7"/>
+      <c r="W48" s="6"/>
       <c r="X48" s="7"/>
-      <c r="Y48" s="7"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="7"/>
+      <c r="AB48" s="7"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>153</v>
       </c>
@@ -3170,11 +3317,14 @@
       <c r="T49" s="6"/>
       <c r="U49" s="7"/>
       <c r="V49" s="8"/>
-      <c r="W49" s="7"/>
+      <c r="W49" s="6"/>
       <c r="X49" s="7"/>
-      <c r="Y49" s="7"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y49" s="8"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>152</v>
       </c>
@@ -3199,11 +3349,14 @@
       <c r="T50" s="6"/>
       <c r="U50" s="7"/>
       <c r="V50" s="8"/>
-      <c r="W50" s="7"/>
+      <c r="W50" s="6"/>
       <c r="X50" s="7"/>
-      <c r="Y50" s="7"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y50" s="8"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>151</v>
       </c>
@@ -3228,11 +3381,14 @@
       <c r="T51" s="6"/>
       <c r="U51" s="7"/>
       <c r="V51" s="8"/>
-      <c r="W51" s="7"/>
+      <c r="W51" s="6"/>
       <c r="X51" s="7"/>
-      <c r="Y51" s="7"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y51" s="8"/>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>150</v>
       </c>
@@ -3257,11 +3413,14 @@
       <c r="T52" s="6"/>
       <c r="U52" s="7"/>
       <c r="V52" s="8"/>
-      <c r="W52" s="7"/>
+      <c r="W52" s="6"/>
       <c r="X52" s="7"/>
-      <c r="Y52" s="7"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="7"/>
+      <c r="AB52" s="7"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>149</v>
       </c>
@@ -3286,11 +3445,14 @@
       <c r="T53" s="6"/>
       <c r="U53" s="7"/>
       <c r="V53" s="8"/>
-      <c r="W53" s="7"/>
+      <c r="W53" s="6"/>
       <c r="X53" s="7"/>
-      <c r="Y53" s="7"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y53" s="8"/>
+      <c r="Z53" s="7"/>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>148</v>
       </c>
@@ -3315,11 +3477,14 @@
       <c r="T54" s="6"/>
       <c r="U54" s="7"/>
       <c r="V54" s="8"/>
-      <c r="W54" s="7"/>
+      <c r="W54" s="6"/>
       <c r="X54" s="7"/>
-      <c r="Y54" s="7"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y54" s="8"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>147</v>
       </c>
@@ -3344,11 +3509,14 @@
       <c r="T55" s="6"/>
       <c r="U55" s="7"/>
       <c r="V55" s="8"/>
-      <c r="W55" s="7"/>
+      <c r="W55" s="6"/>
       <c r="X55" s="7"/>
-      <c r="Y55" s="7"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="7"/>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>146</v>
       </c>
@@ -3373,11 +3541,14 @@
       <c r="T56" s="6"/>
       <c r="U56" s="7"/>
       <c r="V56" s="8"/>
-      <c r="W56" s="7"/>
+      <c r="W56" s="6"/>
       <c r="X56" s="7"/>
-      <c r="Y56" s="7"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y56" s="8"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>145</v>
       </c>
@@ -3402,11 +3573,14 @@
       <c r="T57" s="6"/>
       <c r="U57" s="7"/>
       <c r="V57" s="8"/>
-      <c r="W57" s="7"/>
+      <c r="W57" s="6"/>
       <c r="X57" s="7"/>
-      <c r="Y57" s="7"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y57" s="8"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>144</v>
       </c>
@@ -3431,11 +3605,14 @@
       <c r="T58" s="6"/>
       <c r="U58" s="7"/>
       <c r="V58" s="8"/>
-      <c r="W58" s="7"/>
+      <c r="W58" s="6"/>
       <c r="X58" s="7"/>
-      <c r="Y58" s="7"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="7"/>
+      <c r="AB58" s="7"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>143</v>
       </c>
@@ -3460,11 +3637,14 @@
       <c r="T59" s="6"/>
       <c r="U59" s="7"/>
       <c r="V59" s="8"/>
-      <c r="W59" s="7"/>
+      <c r="W59" s="6"/>
       <c r="X59" s="7"/>
-      <c r="Y59" s="7"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y59" s="8"/>
+      <c r="Z59" s="7"/>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7"/>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>142</v>
       </c>
@@ -3489,11 +3669,14 @@
       <c r="T60" s="6"/>
       <c r="U60" s="7"/>
       <c r="V60" s="8"/>
-      <c r="W60" s="7"/>
+      <c r="W60" s="6"/>
       <c r="X60" s="7"/>
-      <c r="Y60" s="7"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y60" s="8"/>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="7"/>
+      <c r="AB60" s="7"/>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>141</v>
       </c>
@@ -3518,11 +3701,14 @@
       <c r="T61" s="6"/>
       <c r="U61" s="7"/>
       <c r="V61" s="8"/>
-      <c r="W61" s="7"/>
+      <c r="W61" s="6"/>
       <c r="X61" s="7"/>
-      <c r="Y61" s="7"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y61" s="8"/>
+      <c r="Z61" s="7"/>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7"/>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>140</v>
       </c>
@@ -3547,11 +3733,14 @@
       <c r="T62" s="6"/>
       <c r="U62" s="7"/>
       <c r="V62" s="8"/>
-      <c r="W62" s="7"/>
+      <c r="W62" s="6"/>
       <c r="X62" s="7"/>
-      <c r="Y62" s="7"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y62" s="8"/>
+      <c r="Z62" s="7"/>
+      <c r="AA62" s="7"/>
+      <c r="AB62" s="7"/>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>139</v>
       </c>
@@ -3576,11 +3765,14 @@
       <c r="T63" s="6"/>
       <c r="U63" s="7"/>
       <c r="V63" s="8"/>
-      <c r="W63" s="7"/>
+      <c r="W63" s="6"/>
       <c r="X63" s="7"/>
-      <c r="Y63" s="7"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y63" s="8"/>
+      <c r="Z63" s="7"/>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7"/>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>138</v>
       </c>
@@ -3605,11 +3797,14 @@
       <c r="T64" s="6"/>
       <c r="U64" s="7"/>
       <c r="V64" s="8"/>
-      <c r="W64" s="7"/>
+      <c r="W64" s="6"/>
       <c r="X64" s="7"/>
-      <c r="Y64" s="7"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y64" s="8"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="7"/>
+      <c r="AB64" s="7"/>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>137</v>
       </c>
@@ -3634,11 +3829,14 @@
       <c r="T65" s="6"/>
       <c r="U65" s="7"/>
       <c r="V65" s="8"/>
-      <c r="W65" s="7"/>
+      <c r="W65" s="6"/>
       <c r="X65" s="7"/>
-      <c r="Y65" s="7"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y65" s="8"/>
+      <c r="Z65" s="7"/>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7"/>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>136</v>
       </c>
@@ -3663,11 +3861,14 @@
       <c r="T66" s="6"/>
       <c r="U66" s="7"/>
       <c r="V66" s="8"/>
-      <c r="W66" s="7"/>
+      <c r="W66" s="6"/>
       <c r="X66" s="7"/>
-      <c r="Y66" s="7"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y66" s="8"/>
+      <c r="Z66" s="7"/>
+      <c r="AA66" s="7"/>
+      <c r="AB66" s="7"/>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>135</v>
       </c>
@@ -3692,11 +3893,14 @@
       <c r="T67" s="6"/>
       <c r="U67" s="7"/>
       <c r="V67" s="8"/>
-      <c r="W67" s="7"/>
+      <c r="W67" s="6"/>
       <c r="X67" s="7"/>
-      <c r="Y67" s="7"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y67" s="8"/>
+      <c r="Z67" s="7"/>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7"/>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>134</v>
       </c>
@@ -3721,11 +3925,14 @@
       <c r="T68" s="6"/>
       <c r="U68" s="7"/>
       <c r="V68" s="8"/>
-      <c r="W68" s="7"/>
+      <c r="W68" s="6"/>
       <c r="X68" s="7"/>
-      <c r="Y68" s="7"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y68" s="8"/>
+      <c r="Z68" s="7"/>
+      <c r="AA68" s="7"/>
+      <c r="AB68" s="7"/>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>133</v>
       </c>
@@ -3750,11 +3957,14 @@
       <c r="T69" s="6"/>
       <c r="U69" s="7"/>
       <c r="V69" s="8"/>
-      <c r="W69" s="7"/>
+      <c r="W69" s="6"/>
       <c r="X69" s="7"/>
-      <c r="Y69" s="7"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y69" s="8"/>
+      <c r="Z69" s="7"/>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7"/>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>132</v>
       </c>
@@ -3779,11 +3989,14 @@
       <c r="T70" s="6"/>
       <c r="U70" s="7"/>
       <c r="V70" s="8"/>
-      <c r="W70" s="7"/>
+      <c r="W70" s="6"/>
       <c r="X70" s="7"/>
-      <c r="Y70" s="7"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y70" s="8"/>
+      <c r="Z70" s="7"/>
+      <c r="AA70" s="7"/>
+      <c r="AB70" s="7"/>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>131</v>
       </c>
@@ -3808,11 +4021,14 @@
       <c r="T71" s="6"/>
       <c r="U71" s="7"/>
       <c r="V71" s="8"/>
-      <c r="W71" s="7"/>
+      <c r="W71" s="6"/>
       <c r="X71" s="7"/>
-      <c r="Y71" s="7"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y71" s="8"/>
+      <c r="Z71" s="7"/>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7"/>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>130</v>
       </c>
@@ -3837,11 +4053,14 @@
       <c r="T72" s="6"/>
       <c r="U72" s="7"/>
       <c r="V72" s="8"/>
-      <c r="W72" s="7"/>
+      <c r="W72" s="6"/>
       <c r="X72" s="7"/>
-      <c r="Y72" s="7"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="7"/>
+      <c r="AA72" s="7"/>
+      <c r="AB72" s="7"/>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>129</v>
       </c>
@@ -3866,11 +4085,14 @@
       <c r="T73" s="6"/>
       <c r="U73" s="7"/>
       <c r="V73" s="8"/>
-      <c r="W73" s="7"/>
+      <c r="W73" s="6"/>
       <c r="X73" s="7"/>
-      <c r="Y73" s="7"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="7"/>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7"/>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>128</v>
       </c>
@@ -3895,11 +4117,14 @@
       <c r="T74" s="6"/>
       <c r="U74" s="7"/>
       <c r="V74" s="8"/>
-      <c r="W74" s="7"/>
+      <c r="W74" s="6"/>
       <c r="X74" s="7"/>
-      <c r="Y74" s="7"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="7"/>
+      <c r="AA74" s="7"/>
+      <c r="AB74" s="7"/>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>127</v>
       </c>
@@ -3924,11 +4149,14 @@
       <c r="T75" s="6"/>
       <c r="U75" s="7"/>
       <c r="V75" s="8"/>
-      <c r="W75" s="7"/>
+      <c r="W75" s="6"/>
       <c r="X75" s="7"/>
-      <c r="Y75" s="7"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y75" s="8"/>
+      <c r="Z75" s="7"/>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7"/>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>126</v>
       </c>
@@ -3953,11 +4181,14 @@
       <c r="T76" s="6"/>
       <c r="U76" s="7"/>
       <c r="V76" s="8"/>
-      <c r="W76" s="7"/>
+      <c r="W76" s="6"/>
       <c r="X76" s="7"/>
-      <c r="Y76" s="7"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y76" s="8"/>
+      <c r="Z76" s="7"/>
+      <c r="AA76" s="7"/>
+      <c r="AB76" s="7"/>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>125</v>
       </c>
@@ -3982,11 +4213,14 @@
       <c r="T77" s="6"/>
       <c r="U77" s="7"/>
       <c r="V77" s="8"/>
-      <c r="W77" s="7"/>
+      <c r="W77" s="6"/>
       <c r="X77" s="7"/>
-      <c r="Y77" s="7"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y77" s="8"/>
+      <c r="Z77" s="7"/>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7"/>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>124</v>
       </c>
@@ -4011,11 +4245,14 @@
       <c r="T78" s="6"/>
       <c r="U78" s="7"/>
       <c r="V78" s="8"/>
-      <c r="W78" s="7"/>
+      <c r="W78" s="6"/>
       <c r="X78" s="7"/>
-      <c r="Y78" s="7"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y78" s="8"/>
+      <c r="Z78" s="7"/>
+      <c r="AA78" s="7"/>
+      <c r="AB78" s="7"/>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>123</v>
       </c>
@@ -4040,11 +4277,14 @@
       <c r="T79" s="6"/>
       <c r="U79" s="7"/>
       <c r="V79" s="8"/>
-      <c r="W79" s="7"/>
+      <c r="W79" s="6"/>
       <c r="X79" s="7"/>
-      <c r="Y79" s="7"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y79" s="8"/>
+      <c r="Z79" s="7"/>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7"/>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>122</v>
       </c>
@@ -4069,11 +4309,14 @@
       <c r="T80" s="6"/>
       <c r="U80" s="7"/>
       <c r="V80" s="8"/>
-      <c r="W80" s="7"/>
+      <c r="W80" s="6"/>
       <c r="X80" s="7"/>
-      <c r="Y80" s="7"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y80" s="8"/>
+      <c r="Z80" s="7"/>
+      <c r="AA80" s="7"/>
+      <c r="AB80" s="7"/>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>121</v>
       </c>
@@ -4098,11 +4341,14 @@
       <c r="T81" s="6"/>
       <c r="U81" s="7"/>
       <c r="V81" s="8"/>
-      <c r="W81" s="7"/>
+      <c r="W81" s="6"/>
       <c r="X81" s="7"/>
-      <c r="Y81" s="7"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y81" s="8"/>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7"/>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>120</v>
       </c>
@@ -4127,11 +4373,14 @@
       <c r="T82" s="6"/>
       <c r="U82" s="7"/>
       <c r="V82" s="8"/>
-      <c r="W82" s="7"/>
+      <c r="W82" s="6"/>
       <c r="X82" s="7"/>
-      <c r="Y82" s="7"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y82" s="8"/>
+      <c r="Z82" s="7"/>
+      <c r="AA82" s="7"/>
+      <c r="AB82" s="7"/>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>119</v>
       </c>
@@ -4156,11 +4405,14 @@
       <c r="T83" s="6"/>
       <c r="U83" s="7"/>
       <c r="V83" s="8"/>
-      <c r="W83" s="7"/>
+      <c r="W83" s="6"/>
       <c r="X83" s="7"/>
-      <c r="Y83" s="7"/>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y83" s="8"/>
+      <c r="Z83" s="7"/>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7"/>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>118</v>
       </c>
@@ -4185,11 +4437,14 @@
       <c r="T84" s="6"/>
       <c r="U84" s="7"/>
       <c r="V84" s="8"/>
-      <c r="W84" s="7"/>
+      <c r="W84" s="6"/>
       <c r="X84" s="7"/>
-      <c r="Y84" s="7"/>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y84" s="8"/>
+      <c r="Z84" s="7"/>
+      <c r="AA84" s="7"/>
+      <c r="AB84" s="7"/>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>117</v>
       </c>
@@ -4214,11 +4469,14 @@
       <c r="T85" s="6"/>
       <c r="U85" s="7"/>
       <c r="V85" s="8"/>
-      <c r="W85" s="7"/>
+      <c r="W85" s="6"/>
       <c r="X85" s="7"/>
-      <c r="Y85" s="7"/>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y85" s="8"/>
+      <c r="Z85" s="7"/>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7"/>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>116</v>
       </c>
@@ -4243,11 +4501,14 @@
       <c r="T86" s="6"/>
       <c r="U86" s="7"/>
       <c r="V86" s="8"/>
-      <c r="W86" s="7"/>
+      <c r="W86" s="6"/>
       <c r="X86" s="7"/>
-      <c r="Y86" s="7"/>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y86" s="8"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="7"/>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>115</v>
       </c>
@@ -4272,11 +4533,14 @@
       <c r="T87" s="6"/>
       <c r="U87" s="7"/>
       <c r="V87" s="8"/>
-      <c r="W87" s="7"/>
+      <c r="W87" s="6"/>
       <c r="X87" s="7"/>
-      <c r="Y87" s="7"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y87" s="8"/>
+      <c r="Z87" s="7"/>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7"/>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>114</v>
       </c>
@@ -4301,11 +4565,14 @@
       <c r="T88" s="6"/>
       <c r="U88" s="7"/>
       <c r="V88" s="8"/>
-      <c r="W88" s="7"/>
+      <c r="W88" s="6"/>
       <c r="X88" s="7"/>
-      <c r="Y88" s="7"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y88" s="8"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="7"/>
+      <c r="AB88" s="7"/>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>113</v>
       </c>
@@ -4330,11 +4597,14 @@
       <c r="T89" s="6"/>
       <c r="U89" s="7"/>
       <c r="V89" s="8"/>
-      <c r="W89" s="7"/>
+      <c r="W89" s="6"/>
       <c r="X89" s="7"/>
-      <c r="Y89" s="7"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y89" s="8"/>
+      <c r="Z89" s="7"/>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7"/>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>112</v>
       </c>
@@ -4359,11 +4629,14 @@
       <c r="T90" s="6"/>
       <c r="U90" s="7"/>
       <c r="V90" s="8"/>
-      <c r="W90" s="7"/>
+      <c r="W90" s="6"/>
       <c r="X90" s="7"/>
-      <c r="Y90" s="7"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y90" s="8"/>
+      <c r="Z90" s="7"/>
+      <c r="AA90" s="7"/>
+      <c r="AB90" s="7"/>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>111</v>
       </c>
@@ -4388,11 +4661,14 @@
       <c r="T91" s="6"/>
       <c r="U91" s="7"/>
       <c r="V91" s="8"/>
-      <c r="W91" s="7"/>
+      <c r="W91" s="6"/>
       <c r="X91" s="7"/>
-      <c r="Y91" s="7"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y91" s="8"/>
+      <c r="Z91" s="7"/>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7"/>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>110</v>
       </c>
@@ -4417,11 +4693,14 @@
       <c r="T92" s="6"/>
       <c r="U92" s="7"/>
       <c r="V92" s="8"/>
-      <c r="W92" s="7"/>
+      <c r="W92" s="6"/>
       <c r="X92" s="7"/>
-      <c r="Y92" s="7"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y92" s="8"/>
+      <c r="Z92" s="7"/>
+      <c r="AA92" s="7"/>
+      <c r="AB92" s="7"/>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>109</v>
       </c>
@@ -4446,11 +4725,14 @@
       <c r="T93" s="6"/>
       <c r="U93" s="7"/>
       <c r="V93" s="8"/>
-      <c r="W93" s="7"/>
+      <c r="W93" s="6"/>
       <c r="X93" s="7"/>
-      <c r="Y93" s="7"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y93" s="8"/>
+      <c r="Z93" s="7"/>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7"/>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>108</v>
       </c>
@@ -4475,11 +4757,14 @@
       <c r="T94" s="6"/>
       <c r="U94" s="7"/>
       <c r="V94" s="8"/>
-      <c r="W94" s="7"/>
+      <c r="W94" s="6"/>
       <c r="X94" s="7"/>
-      <c r="Y94" s="7"/>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y94" s="8"/>
+      <c r="Z94" s="7"/>
+      <c r="AA94" s="7"/>
+      <c r="AB94" s="7"/>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>107</v>
       </c>
@@ -4504,11 +4789,14 @@
       <c r="T95" s="6"/>
       <c r="U95" s="7"/>
       <c r="V95" s="8"/>
-      <c r="W95" s="7"/>
+      <c r="W95" s="6"/>
       <c r="X95" s="7"/>
-      <c r="Y95" s="7"/>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y95" s="8"/>
+      <c r="Z95" s="7"/>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7"/>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>106</v>
       </c>
@@ -4533,11 +4821,14 @@
       <c r="T96" s="6"/>
       <c r="U96" s="7"/>
       <c r="V96" s="8"/>
-      <c r="W96" s="7"/>
+      <c r="W96" s="6"/>
       <c r="X96" s="7"/>
-      <c r="Y96" s="7"/>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y96" s="8"/>
+      <c r="Z96" s="7"/>
+      <c r="AA96" s="7"/>
+      <c r="AB96" s="7"/>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>105</v>
       </c>
@@ -4562,11 +4853,14 @@
       <c r="T97" s="6"/>
       <c r="U97" s="7"/>
       <c r="V97" s="8"/>
-      <c r="W97" s="7"/>
+      <c r="W97" s="6"/>
       <c r="X97" s="7"/>
-      <c r="Y97" s="7"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y97" s="8"/>
+      <c r="Z97" s="7"/>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7"/>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>104</v>
       </c>
@@ -4591,11 +4885,14 @@
       <c r="T98" s="6"/>
       <c r="U98" s="7"/>
       <c r="V98" s="8"/>
-      <c r="W98" s="7"/>
+      <c r="W98" s="6"/>
       <c r="X98" s="7"/>
-      <c r="Y98" s="7"/>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y98" s="8"/>
+      <c r="Z98" s="7"/>
+      <c r="AA98" s="7"/>
+      <c r="AB98" s="7"/>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>103</v>
       </c>
@@ -4620,11 +4917,14 @@
       <c r="T99" s="6"/>
       <c r="U99" s="7"/>
       <c r="V99" s="8"/>
-      <c r="W99" s="7"/>
+      <c r="W99" s="6"/>
       <c r="X99" s="7"/>
-      <c r="Y99" s="7"/>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y99" s="8"/>
+      <c r="Z99" s="7"/>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7"/>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>102</v>
       </c>
@@ -4649,11 +4949,14 @@
       <c r="T100" s="6"/>
       <c r="U100" s="7"/>
       <c r="V100" s="8"/>
-      <c r="W100" s="7"/>
+      <c r="W100" s="6"/>
       <c r="X100" s="7"/>
-      <c r="Y100" s="7"/>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y100" s="8"/>
+      <c r="Z100" s="7"/>
+      <c r="AA100" s="7"/>
+      <c r="AB100" s="7"/>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>101</v>
       </c>
@@ -4678,11 +4981,14 @@
       <c r="T101" s="6"/>
       <c r="U101" s="7"/>
       <c r="V101" s="8"/>
-      <c r="W101" s="7"/>
+      <c r="W101" s="6"/>
       <c r="X101" s="7"/>
-      <c r="Y101" s="7"/>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y101" s="8"/>
+      <c r="Z101" s="7"/>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7"/>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4707,11 +5013,14 @@
       <c r="T102" s="6"/>
       <c r="U102" s="7"/>
       <c r="V102" s="8"/>
-      <c r="W102" s="7"/>
+      <c r="W102" s="6"/>
       <c r="X102" s="7"/>
-      <c r="Y102" s="7"/>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y102" s="8"/>
+      <c r="Z102" s="7"/>
+      <c r="AA102" s="7"/>
+      <c r="AB102" s="7"/>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>99</v>
       </c>
@@ -4736,11 +5045,14 @@
       <c r="T103" s="6"/>
       <c r="U103" s="7"/>
       <c r="V103" s="8"/>
-      <c r="W103" s="7"/>
+      <c r="W103" s="6"/>
       <c r="X103" s="7"/>
-      <c r="Y103" s="7"/>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y103" s="8"/>
+      <c r="Z103" s="7"/>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7"/>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>98</v>
       </c>
@@ -4765,11 +5077,14 @@
       <c r="T104" s="6"/>
       <c r="U104" s="7"/>
       <c r="V104" s="8"/>
-      <c r="W104" s="7"/>
+      <c r="W104" s="6"/>
       <c r="X104" s="7"/>
-      <c r="Y104" s="7"/>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y104" s="8"/>
+      <c r="Z104" s="7"/>
+      <c r="AA104" s="7"/>
+      <c r="AB104" s="7"/>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>97</v>
       </c>
@@ -4794,11 +5109,14 @@
       <c r="T105" s="6"/>
       <c r="U105" s="7"/>
       <c r="V105" s="8"/>
-      <c r="W105" s="7"/>
+      <c r="W105" s="6"/>
       <c r="X105" s="7"/>
-      <c r="Y105" s="7"/>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y105" s="8"/>
+      <c r="Z105" s="7"/>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7"/>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>96</v>
       </c>
@@ -4823,11 +5141,14 @@
       <c r="T106" s="6"/>
       <c r="U106" s="7"/>
       <c r="V106" s="8"/>
-      <c r="W106" s="7"/>
+      <c r="W106" s="6"/>
       <c r="X106" s="7"/>
-      <c r="Y106" s="7"/>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y106" s="8"/>
+      <c r="Z106" s="7"/>
+      <c r="AA106" s="7"/>
+      <c r="AB106" s="7"/>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>95</v>
       </c>
@@ -4852,11 +5173,14 @@
       <c r="T107" s="6"/>
       <c r="U107" s="7"/>
       <c r="V107" s="8"/>
-      <c r="W107" s="7"/>
+      <c r="W107" s="6"/>
       <c r="X107" s="7"/>
-      <c r="Y107" s="7"/>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y107" s="8"/>
+      <c r="Z107" s="7"/>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7"/>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>94</v>
       </c>
@@ -4881,11 +5205,14 @@
       <c r="T108" s="6"/>
       <c r="U108" s="7"/>
       <c r="V108" s="8"/>
-      <c r="W108" s="7"/>
+      <c r="W108" s="6"/>
       <c r="X108" s="7"/>
-      <c r="Y108" s="7"/>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y108" s="8"/>
+      <c r="Z108" s="7"/>
+      <c r="AA108" s="7"/>
+      <c r="AB108" s="7"/>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>93</v>
       </c>
@@ -4910,11 +5237,14 @@
       <c r="T109" s="6"/>
       <c r="U109" s="7"/>
       <c r="V109" s="8"/>
-      <c r="W109" s="7"/>
+      <c r="W109" s="6"/>
       <c r="X109" s="7"/>
-      <c r="Y109" s="7"/>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y109" s="8"/>
+      <c r="Z109" s="7"/>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7"/>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>92</v>
       </c>
@@ -4939,11 +5269,14 @@
       <c r="T110" s="6"/>
       <c r="U110" s="7"/>
       <c r="V110" s="8"/>
-      <c r="W110" s="7"/>
+      <c r="W110" s="6"/>
       <c r="X110" s="7"/>
-      <c r="Y110" s="7"/>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y110" s="8"/>
+      <c r="Z110" s="7"/>
+      <c r="AA110" s="7"/>
+      <c r="AB110" s="7"/>
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>91</v>
       </c>
@@ -4968,11 +5301,14 @@
       <c r="T111" s="6"/>
       <c r="U111" s="7"/>
       <c r="V111" s="8"/>
-      <c r="W111" s="7"/>
+      <c r="W111" s="6"/>
       <c r="X111" s="7"/>
-      <c r="Y111" s="7"/>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y111" s="8"/>
+      <c r="Z111" s="7"/>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7"/>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>90</v>
       </c>
@@ -4997,11 +5333,14 @@
       <c r="T112" s="6"/>
       <c r="U112" s="7"/>
       <c r="V112" s="8"/>
-      <c r="W112" s="7"/>
+      <c r="W112" s="6"/>
       <c r="X112" s="7"/>
-      <c r="Y112" s="7"/>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y112" s="8"/>
+      <c r="Z112" s="7"/>
+      <c r="AA112" s="7"/>
+      <c r="AB112" s="7"/>
+    </row>
+    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>89</v>
       </c>
@@ -5026,11 +5365,14 @@
       <c r="T113" s="6"/>
       <c r="U113" s="7"/>
       <c r="V113" s="8"/>
-      <c r="W113" s="7"/>
+      <c r="W113" s="6"/>
       <c r="X113" s="7"/>
-      <c r="Y113" s="7"/>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y113" s="8"/>
+      <c r="Z113" s="7"/>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7"/>
+    </row>
+    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>88</v>
       </c>
@@ -5055,11 +5397,14 @@
       <c r="T114" s="6"/>
       <c r="U114" s="7"/>
       <c r="V114" s="8"/>
-      <c r="W114" s="7"/>
+      <c r="W114" s="6"/>
       <c r="X114" s="7"/>
-      <c r="Y114" s="7"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y114" s="8"/>
+      <c r="Z114" s="7"/>
+      <c r="AA114" s="7"/>
+      <c r="AB114" s="7"/>
+    </row>
+    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>87</v>
       </c>
@@ -5084,11 +5429,14 @@
       <c r="T115" s="6"/>
       <c r="U115" s="7"/>
       <c r="V115" s="8"/>
-      <c r="W115" s="7"/>
+      <c r="W115" s="6"/>
       <c r="X115" s="7"/>
-      <c r="Y115" s="7"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y115" s="8"/>
+      <c r="Z115" s="7"/>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7"/>
+    </row>
+    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>86</v>
       </c>
@@ -5113,11 +5461,14 @@
       <c r="T116" s="6"/>
       <c r="U116" s="7"/>
       <c r="V116" s="8"/>
-      <c r="W116" s="7"/>
+      <c r="W116" s="6"/>
       <c r="X116" s="7"/>
-      <c r="Y116" s="7"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y116" s="8"/>
+      <c r="Z116" s="7"/>
+      <c r="AA116" s="7"/>
+      <c r="AB116" s="7"/>
+    </row>
+    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>85</v>
       </c>
@@ -5142,11 +5493,14 @@
       <c r="T117" s="6"/>
       <c r="U117" s="7"/>
       <c r="V117" s="8"/>
-      <c r="W117" s="7"/>
+      <c r="W117" s="6"/>
       <c r="X117" s="7"/>
-      <c r="Y117" s="7"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y117" s="8"/>
+      <c r="Z117" s="7"/>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7"/>
+    </row>
+    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>84</v>
       </c>
@@ -5171,11 +5525,14 @@
       <c r="T118" s="6"/>
       <c r="U118" s="7"/>
       <c r="V118" s="8"/>
-      <c r="W118" s="7"/>
+      <c r="W118" s="6"/>
       <c r="X118" s="7"/>
-      <c r="Y118" s="7"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y118" s="8"/>
+      <c r="Z118" s="7"/>
+      <c r="AA118" s="7"/>
+      <c r="AB118" s="7"/>
+    </row>
+    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>83</v>
       </c>
@@ -5200,11 +5557,14 @@
       <c r="T119" s="6"/>
       <c r="U119" s="7"/>
       <c r="V119" s="8"/>
-      <c r="W119" s="7"/>
+      <c r="W119" s="6"/>
       <c r="X119" s="7"/>
-      <c r="Y119" s="7"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y119" s="8"/>
+      <c r="Z119" s="7"/>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7"/>
+    </row>
+    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>82</v>
       </c>
@@ -5229,11 +5589,14 @@
       <c r="T120" s="6"/>
       <c r="U120" s="7"/>
       <c r="V120" s="8"/>
-      <c r="W120" s="7"/>
+      <c r="W120" s="6"/>
       <c r="X120" s="7"/>
-      <c r="Y120" s="7"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y120" s="8"/>
+      <c r="Z120" s="7"/>
+      <c r="AA120" s="7"/>
+      <c r="AB120" s="7"/>
+    </row>
+    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>81</v>
       </c>
@@ -5258,11 +5621,14 @@
       <c r="T121" s="6"/>
       <c r="U121" s="7"/>
       <c r="V121" s="8"/>
-      <c r="W121" s="7"/>
+      <c r="W121" s="6"/>
       <c r="X121" s="7"/>
-      <c r="Y121" s="7"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y121" s="8"/>
+      <c r="Z121" s="7"/>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7"/>
+    </row>
+    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>80</v>
       </c>
@@ -5287,11 +5653,14 @@
       <c r="T122" s="6"/>
       <c r="U122" s="7"/>
       <c r="V122" s="8"/>
-      <c r="W122" s="7"/>
+      <c r="W122" s="6"/>
       <c r="X122" s="7"/>
-      <c r="Y122" s="7"/>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y122" s="8"/>
+      <c r="Z122" s="7"/>
+      <c r="AA122" s="7"/>
+      <c r="AB122" s="7"/>
+    </row>
+    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>79</v>
       </c>
@@ -5316,11 +5685,14 @@
       <c r="T123" s="6"/>
       <c r="U123" s="7"/>
       <c r="V123" s="8"/>
-      <c r="W123" s="7"/>
+      <c r="W123" s="6"/>
       <c r="X123" s="7"/>
-      <c r="Y123" s="7"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y123" s="8"/>
+      <c r="Z123" s="7"/>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7"/>
+    </row>
+    <row r="124" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>78</v>
       </c>
@@ -5345,11 +5717,14 @@
       <c r="T124" s="6"/>
       <c r="U124" s="7"/>
       <c r="V124" s="8"/>
-      <c r="W124" s="7"/>
+      <c r="W124" s="6"/>
       <c r="X124" s="7"/>
-      <c r="Y124" s="7"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y124" s="8"/>
+      <c r="Z124" s="7"/>
+      <c r="AA124" s="7"/>
+      <c r="AB124" s="7"/>
+    </row>
+    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>77</v>
       </c>
@@ -5374,11 +5749,14 @@
       <c r="T125" s="6"/>
       <c r="U125" s="7"/>
       <c r="V125" s="8"/>
-      <c r="W125" s="7"/>
+      <c r="W125" s="6"/>
       <c r="X125" s="7"/>
-      <c r="Y125" s="7"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y125" s="8"/>
+      <c r="Z125" s="7"/>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7"/>
+    </row>
+    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>76</v>
       </c>
@@ -5403,11 +5781,14 @@
       <c r="T126" s="6"/>
       <c r="U126" s="7"/>
       <c r="V126" s="8"/>
-      <c r="W126" s="7"/>
+      <c r="W126" s="6"/>
       <c r="X126" s="7"/>
-      <c r="Y126" s="7"/>
-    </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y126" s="8"/>
+      <c r="Z126" s="7"/>
+      <c r="AA126" s="7"/>
+      <c r="AB126" s="7"/>
+    </row>
+    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>75</v>
       </c>
@@ -5432,11 +5813,14 @@
       <c r="T127" s="6"/>
       <c r="U127" s="7"/>
       <c r="V127" s="8"/>
-      <c r="W127" s="7"/>
+      <c r="W127" s="6"/>
       <c r="X127" s="7"/>
-      <c r="Y127" s="7"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y127" s="8"/>
+      <c r="Z127" s="7"/>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7"/>
+    </row>
+    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>74</v>
       </c>
@@ -5461,11 +5845,14 @@
       <c r="T128" s="6"/>
       <c r="U128" s="7"/>
       <c r="V128" s="8"/>
-      <c r="W128" s="7"/>
+      <c r="W128" s="6"/>
       <c r="X128" s="7"/>
-      <c r="Y128" s="7"/>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y128" s="8"/>
+      <c r="Z128" s="7"/>
+      <c r="AA128" s="7"/>
+      <c r="AB128" s="7"/>
+    </row>
+    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>73</v>
       </c>
@@ -5490,11 +5877,14 @@
       <c r="T129" s="6"/>
       <c r="U129" s="7"/>
       <c r="V129" s="8"/>
-      <c r="W129" s="7"/>
+      <c r="W129" s="6"/>
       <c r="X129" s="7"/>
-      <c r="Y129" s="7"/>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y129" s="8"/>
+      <c r="Z129" s="7"/>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7"/>
+    </row>
+    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>72</v>
       </c>
@@ -5519,11 +5909,14 @@
       <c r="T130" s="6"/>
       <c r="U130" s="7"/>
       <c r="V130" s="8"/>
-      <c r="W130" s="7"/>
+      <c r="W130" s="6"/>
       <c r="X130" s="7"/>
-      <c r="Y130" s="7"/>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y130" s="8"/>
+      <c r="Z130" s="7"/>
+      <c r="AA130" s="7"/>
+      <c r="AB130" s="7"/>
+    </row>
+    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>71</v>
       </c>
@@ -5548,11 +5941,14 @@
       <c r="T131" s="6"/>
       <c r="U131" s="7"/>
       <c r="V131" s="8"/>
-      <c r="W131" s="7"/>
+      <c r="W131" s="6"/>
       <c r="X131" s="7"/>
-      <c r="Y131" s="7"/>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y131" s="8"/>
+      <c r="Z131" s="7"/>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7"/>
+    </row>
+    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>70</v>
       </c>
@@ -5577,11 +5973,14 @@
       <c r="T132" s="6"/>
       <c r="U132" s="7"/>
       <c r="V132" s="8"/>
-      <c r="W132" s="7"/>
+      <c r="W132" s="6"/>
       <c r="X132" s="7"/>
-      <c r="Y132" s="7"/>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y132" s="8"/>
+      <c r="Z132" s="7"/>
+      <c r="AA132" s="7"/>
+      <c r="AB132" s="7"/>
+    </row>
+    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>69</v>
       </c>
@@ -5606,11 +6005,14 @@
       <c r="T133" s="6"/>
       <c r="U133" s="7"/>
       <c r="V133" s="8"/>
-      <c r="W133" s="7"/>
+      <c r="W133" s="6"/>
       <c r="X133" s="7"/>
-      <c r="Y133" s="7"/>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y133" s="8"/>
+      <c r="Z133" s="7"/>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7"/>
+    </row>
+    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>68</v>
       </c>
@@ -5635,11 +6037,14 @@
       <c r="T134" s="6"/>
       <c r="U134" s="7"/>
       <c r="V134" s="8"/>
-      <c r="W134" s="7"/>
+      <c r="W134" s="6"/>
       <c r="X134" s="7"/>
-      <c r="Y134" s="7"/>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y134" s="8"/>
+      <c r="Z134" s="7"/>
+      <c r="AA134" s="7"/>
+      <c r="AB134" s="7"/>
+    </row>
+    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>67</v>
       </c>
@@ -5664,11 +6069,14 @@
       <c r="T135" s="6"/>
       <c r="U135" s="7"/>
       <c r="V135" s="8"/>
-      <c r="W135" s="7"/>
+      <c r="W135" s="6"/>
       <c r="X135" s="7"/>
-      <c r="Y135" s="7"/>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y135" s="8"/>
+      <c r="Z135" s="7"/>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7"/>
+    </row>
+    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>66</v>
       </c>
@@ -5693,11 +6101,14 @@
       <c r="T136" s="6"/>
       <c r="U136" s="7"/>
       <c r="V136" s="8"/>
-      <c r="W136" s="7"/>
+      <c r="W136" s="6"/>
       <c r="X136" s="7"/>
-      <c r="Y136" s="7"/>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y136" s="8"/>
+      <c r="Z136" s="7"/>
+      <c r="AA136" s="7"/>
+      <c r="AB136" s="7"/>
+    </row>
+    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>65</v>
       </c>
@@ -5722,11 +6133,14 @@
       <c r="T137" s="6"/>
       <c r="U137" s="7"/>
       <c r="V137" s="8"/>
-      <c r="W137" s="7"/>
+      <c r="W137" s="6"/>
       <c r="X137" s="7"/>
-      <c r="Y137" s="7"/>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y137" s="8"/>
+      <c r="Z137" s="7"/>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7"/>
+    </row>
+    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>64</v>
       </c>
@@ -5751,11 +6165,14 @@
       <c r="T138" s="6"/>
       <c r="U138" s="7"/>
       <c r="V138" s="8"/>
-      <c r="W138" s="7"/>
+      <c r="W138" s="6"/>
       <c r="X138" s="7"/>
-      <c r="Y138" s="7"/>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y138" s="8"/>
+      <c r="Z138" s="7"/>
+      <c r="AA138" s="7"/>
+      <c r="AB138" s="7"/>
+    </row>
+    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>63</v>
       </c>
@@ -5780,11 +6197,14 @@
       <c r="T139" s="6"/>
       <c r="U139" s="7"/>
       <c r="V139" s="8"/>
-      <c r="W139" s="7"/>
+      <c r="W139" s="6"/>
       <c r="X139" s="7"/>
-      <c r="Y139" s="7"/>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y139" s="8"/>
+      <c r="Z139" s="7"/>
+      <c r="AA139" s="7"/>
+      <c r="AB139" s="7"/>
+    </row>
+    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>62</v>
       </c>
@@ -5809,11 +6229,14 @@
       <c r="T140" s="6"/>
       <c r="U140" s="7"/>
       <c r="V140" s="8"/>
-      <c r="W140" s="7"/>
+      <c r="W140" s="6"/>
       <c r="X140" s="7"/>
-      <c r="Y140" s="7"/>
-    </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y140" s="8"/>
+      <c r="Z140" s="7"/>
+      <c r="AA140" s="7"/>
+      <c r="AB140" s="7"/>
+    </row>
+    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>61</v>
       </c>
@@ -5838,11 +6261,14 @@
       <c r="T141" s="6"/>
       <c r="U141" s="7"/>
       <c r="V141" s="8"/>
-      <c r="W141" s="7"/>
+      <c r="W141" s="6"/>
       <c r="X141" s="7"/>
-      <c r="Y141" s="7"/>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y141" s="8"/>
+      <c r="Z141" s="7"/>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7"/>
+    </row>
+    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>60</v>
       </c>
@@ -5867,11 +6293,14 @@
       <c r="T142" s="6"/>
       <c r="U142" s="7"/>
       <c r="V142" s="8"/>
-      <c r="W142" s="7"/>
+      <c r="W142" s="6"/>
       <c r="X142" s="7"/>
-      <c r="Y142" s="7"/>
-    </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y142" s="8"/>
+      <c r="Z142" s="7"/>
+      <c r="AA142" s="7"/>
+      <c r="AB142" s="7"/>
+    </row>
+    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>59</v>
       </c>
@@ -5896,11 +6325,14 @@
       <c r="T143" s="6"/>
       <c r="U143" s="7"/>
       <c r="V143" s="8"/>
-      <c r="W143" s="7"/>
+      <c r="W143" s="6"/>
       <c r="X143" s="7"/>
-      <c r="Y143" s="7"/>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y143" s="8"/>
+      <c r="Z143" s="7"/>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7"/>
+    </row>
+    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>58</v>
       </c>
@@ -5925,11 +6357,14 @@
       <c r="T144" s="6"/>
       <c r="U144" s="7"/>
       <c r="V144" s="8"/>
-      <c r="W144" s="7"/>
+      <c r="W144" s="6"/>
       <c r="X144" s="7"/>
-      <c r="Y144" s="7"/>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y144" s="8"/>
+      <c r="Z144" s="7"/>
+      <c r="AA144" s="7"/>
+      <c r="AB144" s="7"/>
+    </row>
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>57</v>
       </c>
@@ -5954,11 +6389,14 @@
       <c r="T145" s="6"/>
       <c r="U145" s="7"/>
       <c r="V145" s="8"/>
-      <c r="W145" s="7"/>
+      <c r="W145" s="6"/>
       <c r="X145" s="7"/>
-      <c r="Y145" s="7"/>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y145" s="8"/>
+      <c r="Z145" s="7"/>
+      <c r="AA145" s="7"/>
+      <c r="AB145" s="7"/>
+    </row>
+    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>56</v>
       </c>
@@ -5983,11 +6421,14 @@
       <c r="T146" s="6"/>
       <c r="U146" s="7"/>
       <c r="V146" s="8"/>
-      <c r="W146" s="7"/>
+      <c r="W146" s="6"/>
       <c r="X146" s="7"/>
-      <c r="Y146" s="7"/>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y146" s="8"/>
+      <c r="Z146" s="7"/>
+      <c r="AA146" s="7"/>
+      <c r="AB146" s="7"/>
+    </row>
+    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>55</v>
       </c>
@@ -6012,11 +6453,14 @@
       <c r="T147" s="6"/>
       <c r="U147" s="7"/>
       <c r="V147" s="8"/>
-      <c r="W147" s="7"/>
+      <c r="W147" s="6"/>
       <c r="X147" s="7"/>
-      <c r="Y147" s="7"/>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y147" s="8"/>
+      <c r="Z147" s="7"/>
+      <c r="AA147" s="7"/>
+      <c r="AB147" s="7"/>
+    </row>
+    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>54</v>
       </c>
@@ -6041,11 +6485,14 @@
       <c r="T148" s="6"/>
       <c r="U148" s="7"/>
       <c r="V148" s="8"/>
-      <c r="W148" s="7"/>
+      <c r="W148" s="6"/>
       <c r="X148" s="7"/>
-      <c r="Y148" s="7"/>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y148" s="8"/>
+      <c r="Z148" s="7"/>
+      <c r="AA148" s="7"/>
+      <c r="AB148" s="7"/>
+    </row>
+    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>53</v>
       </c>
@@ -6070,11 +6517,14 @@
       <c r="T149" s="6"/>
       <c r="U149" s="7"/>
       <c r="V149" s="8"/>
-      <c r="W149" s="7"/>
+      <c r="W149" s="6"/>
       <c r="X149" s="7"/>
-      <c r="Y149" s="7"/>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y149" s="8"/>
+      <c r="Z149" s="7"/>
+      <c r="AA149" s="7"/>
+      <c r="AB149" s="7"/>
+    </row>
+    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>52</v>
       </c>
@@ -6099,11 +6549,14 @@
       <c r="T150" s="6"/>
       <c r="U150" s="7"/>
       <c r="V150" s="8"/>
-      <c r="W150" s="7"/>
+      <c r="W150" s="6"/>
       <c r="X150" s="7"/>
-      <c r="Y150" s="7"/>
-    </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y150" s="8"/>
+      <c r="Z150" s="7"/>
+      <c r="AA150" s="7"/>
+      <c r="AB150" s="7"/>
+    </row>
+    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>51</v>
       </c>
@@ -6128,11 +6581,14 @@
       <c r="T151" s="6"/>
       <c r="U151" s="7"/>
       <c r="V151" s="8"/>
-      <c r="W151" s="7"/>
+      <c r="W151" s="6"/>
       <c r="X151" s="7"/>
-      <c r="Y151" s="7"/>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y151" s="8"/>
+      <c r="Z151" s="7"/>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7"/>
+    </row>
+    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>50</v>
       </c>
@@ -6157,11 +6613,14 @@
       <c r="T152" s="6"/>
       <c r="U152" s="7"/>
       <c r="V152" s="8"/>
-      <c r="W152" s="7"/>
+      <c r="W152" s="6"/>
       <c r="X152" s="7"/>
-      <c r="Y152" s="7"/>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y152" s="8"/>
+      <c r="Z152" s="7"/>
+      <c r="AA152" s="7"/>
+      <c r="AB152" s="7"/>
+    </row>
+    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>49</v>
       </c>
@@ -6186,11 +6645,14 @@
       <c r="T153" s="6"/>
       <c r="U153" s="7"/>
       <c r="V153" s="8"/>
-      <c r="W153" s="7"/>
+      <c r="W153" s="6"/>
       <c r="X153" s="7"/>
-      <c r="Y153" s="7"/>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y153" s="8"/>
+      <c r="Z153" s="7"/>
+      <c r="AA153" s="7"/>
+      <c r="AB153" s="7"/>
+    </row>
+    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>48</v>
       </c>
@@ -6215,11 +6677,14 @@
       <c r="T154" s="6"/>
       <c r="U154" s="7"/>
       <c r="V154" s="8"/>
-      <c r="W154" s="7"/>
+      <c r="W154" s="6"/>
       <c r="X154" s="7"/>
-      <c r="Y154" s="7"/>
-    </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y154" s="8"/>
+      <c r="Z154" s="7"/>
+      <c r="AA154" s="7"/>
+      <c r="AB154" s="7"/>
+    </row>
+    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>47</v>
       </c>
@@ -6244,11 +6709,14 @@
       <c r="T155" s="6"/>
       <c r="U155" s="7"/>
       <c r="V155" s="8"/>
-      <c r="W155" s="7"/>
+      <c r="W155" s="6"/>
       <c r="X155" s="7"/>
-      <c r="Y155" s="7"/>
-    </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y155" s="8"/>
+      <c r="Z155" s="7"/>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7"/>
+    </row>
+    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>46</v>
       </c>
@@ -6273,11 +6741,14 @@
       <c r="T156" s="6"/>
       <c r="U156" s="7"/>
       <c r="V156" s="8"/>
-      <c r="W156" s="7"/>
+      <c r="W156" s="6"/>
       <c r="X156" s="7"/>
-      <c r="Y156" s="7"/>
-    </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y156" s="8"/>
+      <c r="Z156" s="7"/>
+      <c r="AA156" s="7"/>
+      <c r="AB156" s="7"/>
+    </row>
+    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>45</v>
       </c>
@@ -6302,11 +6773,14 @@
       <c r="T157" s="6"/>
       <c r="U157" s="7"/>
       <c r="V157" s="8"/>
-      <c r="W157" s="7"/>
+      <c r="W157" s="6"/>
       <c r="X157" s="7"/>
-      <c r="Y157" s="7"/>
-    </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y157" s="8"/>
+      <c r="Z157" s="7"/>
+      <c r="AA157" s="7"/>
+      <c r="AB157" s="7"/>
+    </row>
+    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>44</v>
       </c>
@@ -6331,11 +6805,14 @@
       <c r="T158" s="6"/>
       <c r="U158" s="7"/>
       <c r="V158" s="8"/>
-      <c r="W158" s="7"/>
+      <c r="W158" s="6"/>
       <c r="X158" s="7"/>
-      <c r="Y158" s="7"/>
-    </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y158" s="8"/>
+      <c r="Z158" s="7"/>
+      <c r="AA158" s="7"/>
+      <c r="AB158" s="7"/>
+    </row>
+    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>43</v>
       </c>
@@ -6360,11 +6837,14 @@
       <c r="T159" s="6"/>
       <c r="U159" s="7"/>
       <c r="V159" s="8"/>
-      <c r="W159" s="7"/>
+      <c r="W159" s="6"/>
       <c r="X159" s="7"/>
-      <c r="Y159" s="7"/>
-    </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y159" s="8"/>
+      <c r="Z159" s="7"/>
+      <c r="AA159" s="7"/>
+      <c r="AB159" s="7"/>
+    </row>
+    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>42</v>
       </c>
@@ -6389,11 +6869,14 @@
       <c r="T160" s="6"/>
       <c r="U160" s="7"/>
       <c r="V160" s="8"/>
-      <c r="W160" s="7"/>
+      <c r="W160" s="6"/>
       <c r="X160" s="7"/>
-      <c r="Y160" s="7"/>
-    </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y160" s="8"/>
+      <c r="Z160" s="7"/>
+      <c r="AA160" s="7"/>
+      <c r="AB160" s="7"/>
+    </row>
+    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>41</v>
       </c>
@@ -6418,11 +6901,14 @@
       <c r="T161" s="6"/>
       <c r="U161" s="7"/>
       <c r="V161" s="8"/>
-      <c r="W161" s="7"/>
+      <c r="W161" s="6"/>
       <c r="X161" s="7"/>
-      <c r="Y161" s="7"/>
-    </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y161" s="8"/>
+      <c r="Z161" s="7"/>
+      <c r="AA161" s="7"/>
+      <c r="AB161" s="7"/>
+    </row>
+    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>40</v>
       </c>
@@ -6447,11 +6933,14 @@
       <c r="T162" s="6"/>
       <c r="U162" s="7"/>
       <c r="V162" s="8"/>
-      <c r="W162" s="7"/>
+      <c r="W162" s="6"/>
       <c r="X162" s="7"/>
-      <c r="Y162" s="7"/>
-    </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y162" s="8"/>
+      <c r="Z162" s="7"/>
+      <c r="AA162" s="7"/>
+      <c r="AB162" s="7"/>
+    </row>
+    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>39</v>
       </c>
@@ -6476,11 +6965,14 @@
       <c r="T163" s="6"/>
       <c r="U163" s="7"/>
       <c r="V163" s="8"/>
-      <c r="W163" s="7"/>
+      <c r="W163" s="6"/>
       <c r="X163" s="7"/>
-      <c r="Y163" s="7"/>
-    </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y163" s="8"/>
+      <c r="Z163" s="7"/>
+      <c r="AA163" s="7"/>
+      <c r="AB163" s="7"/>
+    </row>
+    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>38</v>
       </c>
@@ -6505,11 +6997,14 @@
       <c r="T164" s="6"/>
       <c r="U164" s="7"/>
       <c r="V164" s="8"/>
-      <c r="W164" s="7"/>
+      <c r="W164" s="6"/>
       <c r="X164" s="7"/>
-      <c r="Y164" s="7"/>
-    </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y164" s="8"/>
+      <c r="Z164" s="7"/>
+      <c r="AA164" s="7"/>
+      <c r="AB164" s="7"/>
+    </row>
+    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>37</v>
       </c>
@@ -6534,11 +7029,14 @@
       <c r="T165" s="6"/>
       <c r="U165" s="7"/>
       <c r="V165" s="8"/>
-      <c r="W165" s="7"/>
+      <c r="W165" s="6"/>
       <c r="X165" s="7"/>
-      <c r="Y165" s="7"/>
-    </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y165" s="8"/>
+      <c r="Z165" s="7"/>
+      <c r="AA165" s="7"/>
+      <c r="AB165" s="7"/>
+    </row>
+    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>36</v>
       </c>
@@ -6563,11 +7061,14 @@
       <c r="T166" s="6"/>
       <c r="U166" s="7"/>
       <c r="V166" s="8"/>
-      <c r="W166" s="7"/>
+      <c r="W166" s="6"/>
       <c r="X166" s="7"/>
-      <c r="Y166" s="7"/>
-    </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y166" s="8"/>
+      <c r="Z166" s="7"/>
+      <c r="AA166" s="7"/>
+      <c r="AB166" s="7"/>
+    </row>
+    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>35</v>
       </c>
@@ -6592,11 +7093,14 @@
       <c r="T167" s="6"/>
       <c r="U167" s="7"/>
       <c r="V167" s="8"/>
-      <c r="W167" s="7"/>
+      <c r="W167" s="6"/>
       <c r="X167" s="7"/>
-      <c r="Y167" s="7"/>
-    </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y167" s="8"/>
+      <c r="Z167" s="7"/>
+      <c r="AA167" s="7"/>
+      <c r="AB167" s="7"/>
+    </row>
+    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>34</v>
       </c>
@@ -6621,11 +7125,14 @@
       <c r="T168" s="6"/>
       <c r="U168" s="7"/>
       <c r="V168" s="8"/>
-      <c r="W168" s="7"/>
+      <c r="W168" s="6"/>
       <c r="X168" s="7"/>
-      <c r="Y168" s="7"/>
-    </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y168" s="8"/>
+      <c r="Z168" s="7"/>
+      <c r="AA168" s="7"/>
+      <c r="AB168" s="7"/>
+    </row>
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>33</v>
       </c>
@@ -6650,11 +7157,14 @@
       <c r="T169" s="6"/>
       <c r="U169" s="7"/>
       <c r="V169" s="8"/>
-      <c r="W169" s="7"/>
+      <c r="W169" s="6"/>
       <c r="X169" s="7"/>
-      <c r="Y169" s="7"/>
-    </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y169" s="8"/>
+      <c r="Z169" s="7"/>
+      <c r="AA169" s="7"/>
+      <c r="AB169" s="7"/>
+    </row>
+    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>32</v>
       </c>
@@ -6679,11 +7189,14 @@
       <c r="T170" s="6"/>
       <c r="U170" s="7"/>
       <c r="V170" s="8"/>
-      <c r="W170" s="7"/>
+      <c r="W170" s="6"/>
       <c r="X170" s="7"/>
-      <c r="Y170" s="7"/>
-    </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y170" s="8"/>
+      <c r="Z170" s="7"/>
+      <c r="AA170" s="7"/>
+      <c r="AB170" s="7"/>
+    </row>
+    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>31</v>
       </c>
@@ -6708,11 +7221,14 @@
       <c r="T171" s="6"/>
       <c r="U171" s="7"/>
       <c r="V171" s="8"/>
-      <c r="W171" s="7"/>
+      <c r="W171" s="6"/>
       <c r="X171" s="7"/>
-      <c r="Y171" s="7"/>
-    </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y171" s="8"/>
+      <c r="Z171" s="7"/>
+      <c r="AA171" s="7"/>
+      <c r="AB171" s="7"/>
+    </row>
+    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>30</v>
       </c>
@@ -6737,11 +7253,14 @@
       <c r="T172" s="6"/>
       <c r="U172" s="7"/>
       <c r="V172" s="8"/>
-      <c r="W172" s="7"/>
+      <c r="W172" s="6"/>
       <c r="X172" s="7"/>
-      <c r="Y172" s="7"/>
-    </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y172" s="8"/>
+      <c r="Z172" s="7"/>
+      <c r="AA172" s="7"/>
+      <c r="AB172" s="7"/>
+    </row>
+    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>29</v>
       </c>
@@ -6766,11 +7285,14 @@
       <c r="T173" s="6"/>
       <c r="U173" s="7"/>
       <c r="V173" s="8"/>
-      <c r="W173" s="7"/>
+      <c r="W173" s="6"/>
       <c r="X173" s="7"/>
-      <c r="Y173" s="7"/>
-    </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y173" s="8"/>
+      <c r="Z173" s="7"/>
+      <c r="AA173" s="7"/>
+      <c r="AB173" s="7"/>
+    </row>
+    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>28</v>
       </c>
@@ -6792,14 +7314,17 @@
       <c r="Q174" s="15"/>
       <c r="R174" s="15"/>
       <c r="S174" s="15"/>
-      <c r="T174" s="6"/>
-      <c r="U174" s="7"/>
-      <c r="V174" s="8"/>
-      <c r="W174" s="7"/>
+      <c r="T174" s="11"/>
+      <c r="U174" s="15"/>
+      <c r="V174" s="9"/>
+      <c r="W174" s="6"/>
       <c r="X174" s="7"/>
-      <c r="Y174" s="7"/>
-    </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y174" s="8"/>
+      <c r="Z174" s="7"/>
+      <c r="AA174" s="7"/>
+      <c r="AB174" s="7"/>
+    </row>
+    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>27</v>
       </c>
@@ -6824,11 +7349,14 @@
       <c r="T175" s="6"/>
       <c r="U175" s="7"/>
       <c r="V175" s="8"/>
-      <c r="W175" s="7"/>
+      <c r="W175" s="6"/>
       <c r="X175" s="7"/>
-      <c r="Y175" s="7"/>
-    </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y175" s="8"/>
+      <c r="Z175" s="7"/>
+      <c r="AA175" s="7"/>
+      <c r="AB175" s="7"/>
+    </row>
+    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>26</v>
       </c>
@@ -6853,11 +7381,14 @@
       <c r="T176" s="6"/>
       <c r="U176" s="7"/>
       <c r="V176" s="8"/>
-      <c r="W176" s="7"/>
+      <c r="W176" s="6"/>
       <c r="X176" s="7"/>
-      <c r="Y176" s="7"/>
-    </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y176" s="8"/>
+      <c r="Z176" s="7"/>
+      <c r="AA176" s="7"/>
+      <c r="AB176" s="7"/>
+    </row>
+    <row r="177" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>25</v>
       </c>
@@ -6882,11 +7413,14 @@
       <c r="T177" s="6"/>
       <c r="U177" s="7"/>
       <c r="V177" s="8"/>
-      <c r="W177" s="7"/>
+      <c r="W177" s="6"/>
       <c r="X177" s="7"/>
-      <c r="Y177" s="7"/>
-    </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y177" s="8"/>
+      <c r="Z177" s="7"/>
+      <c r="AA177" s="7"/>
+      <c r="AB177" s="7"/>
+    </row>
+    <row r="178" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>24</v>
       </c>
@@ -6911,11 +7445,14 @@
       <c r="T178" s="6"/>
       <c r="U178" s="7"/>
       <c r="V178" s="8"/>
-      <c r="W178" s="7"/>
+      <c r="W178" s="6"/>
       <c r="X178" s="7"/>
-      <c r="Y178" s="7"/>
-    </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y178" s="8"/>
+      <c r="Z178" s="7"/>
+      <c r="AA178" s="7"/>
+      <c r="AB178" s="7"/>
+    </row>
+    <row r="179" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>23</v>
       </c>
@@ -6940,11 +7477,14 @@
       <c r="T179" s="6"/>
       <c r="U179" s="7"/>
       <c r="V179" s="8"/>
-      <c r="W179" s="7"/>
+      <c r="W179" s="6"/>
       <c r="X179" s="7"/>
-      <c r="Y179" s="7"/>
-    </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y179" s="8"/>
+      <c r="Z179" s="7"/>
+      <c r="AA179" s="7"/>
+      <c r="AB179" s="7"/>
+    </row>
+    <row r="180" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>22</v>
       </c>
@@ -6963,17 +7503,26 @@
       <c r="N180" s="6"/>
       <c r="O180" s="7"/>
       <c r="P180" s="8"/>
-      <c r="Q180" s="7"/>
-      <c r="R180" s="7"/>
-      <c r="S180" s="7"/>
+      <c r="Q180" s="7">
+        <v>4</v>
+      </c>
+      <c r="R180" s="7">
+        <v>1</v>
+      </c>
+      <c r="S180" s="7">
+        <v>3</v>
+      </c>
       <c r="T180" s="6"/>
       <c r="U180" s="7"/>
       <c r="V180" s="8"/>
-      <c r="W180" s="7"/>
+      <c r="W180" s="6"/>
       <c r="X180" s="7"/>
-      <c r="Y180" s="7"/>
-    </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y180" s="8"/>
+      <c r="Z180" s="7"/>
+      <c r="AA180" s="7"/>
+      <c r="AB180" s="7"/>
+    </row>
+    <row r="181" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>21</v>
       </c>
@@ -7004,11 +7553,14 @@
       <c r="T181" s="6"/>
       <c r="U181" s="7"/>
       <c r="V181" s="8"/>
-      <c r="W181" s="7"/>
+      <c r="W181" s="6"/>
       <c r="X181" s="7"/>
-      <c r="Y181" s="7"/>
-    </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y181" s="8"/>
+      <c r="Z181" s="7"/>
+      <c r="AA181" s="7"/>
+      <c r="AB181" s="7"/>
+    </row>
+    <row r="182" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>20</v>
       </c>
@@ -7036,20 +7588,23 @@
       <c r="Q182" s="7"/>
       <c r="R182" s="7"/>
       <c r="S182" s="7"/>
-      <c r="T182" s="12">
+      <c r="T182" s="6"/>
+      <c r="U182" s="7"/>
+      <c r="V182" s="8"/>
+      <c r="W182" s="12">
         <v>2</v>
       </c>
-      <c r="U182" s="13">
+      <c r="X182" s="13">
         <v>3</v>
       </c>
-      <c r="V182" s="14">
+      <c r="Y182" s="14">
         <v>3</v>
       </c>
-      <c r="W182" s="13"/>
-      <c r="X182" s="13"/>
-      <c r="Y182" s="13"/>
-    </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z182" s="13"/>
+      <c r="AA182" s="13"/>
+      <c r="AB182" s="13"/>
+    </row>
+    <row r="183" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>19</v>
       </c>
@@ -7071,20 +7626,23 @@
       <c r="Q183" s="7"/>
       <c r="R183" s="7"/>
       <c r="S183" s="7"/>
-      <c r="T183" s="6">
+      <c r="T183" s="6"/>
+      <c r="U183" s="7"/>
+      <c r="V183" s="8"/>
+      <c r="W183" s="6">
         <v>5</v>
       </c>
-      <c r="U183" s="7">
+      <c r="X183" s="7">
         <v>0</v>
       </c>
-      <c r="V183" s="8">
+      <c r="Y183" s="8">
         <v>3</v>
       </c>
-      <c r="W183" s="7"/>
-      <c r="X183" s="7"/>
-      <c r="Y183" s="7"/>
-    </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z183" s="7"/>
+      <c r="AA183" s="7"/>
+      <c r="AB183" s="7"/>
+    </row>
+    <row r="184" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>18</v>
       </c>
@@ -7109,23 +7667,32 @@
       <c r="P184" s="8">
         <v>3</v>
       </c>
-      <c r="Q184" s="7"/>
-      <c r="R184" s="7"/>
-      <c r="S184" s="7"/>
-      <c r="T184" s="6">
+      <c r="Q184" s="10">
+        <v>3</v>
+      </c>
+      <c r="R184" s="10">
+        <v>2</v>
+      </c>
+      <c r="S184" s="10">
+        <v>3</v>
+      </c>
+      <c r="T184" s="21"/>
+      <c r="U184" s="10"/>
+      <c r="V184" s="22"/>
+      <c r="W184" s="6">
         <v>4</v>
       </c>
-      <c r="U184" s="7">
+      <c r="X184" s="7">
         <v>1</v>
       </c>
-      <c r="V184" s="8">
+      <c r="Y184" s="8">
         <v>3</v>
       </c>
-      <c r="W184" s="7"/>
-      <c r="X184" s="7"/>
-      <c r="Y184" s="7"/>
-    </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Z184" s="7"/>
+      <c r="AA184" s="7"/>
+      <c r="AB184" s="7"/>
+    </row>
+    <row r="185" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>17</v>
       </c>
@@ -7150,11 +7717,14 @@
       <c r="T185" s="6"/>
       <c r="U185" s="7"/>
       <c r="V185" s="8"/>
-      <c r="W185" s="7"/>
+      <c r="W185" s="6"/>
       <c r="X185" s="7"/>
-      <c r="Y185" s="7"/>
-    </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y185" s="8"/>
+      <c r="Z185" s="7"/>
+      <c r="AA185" s="7"/>
+      <c r="AB185" s="7"/>
+    </row>
+    <row r="186" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>16</v>
       </c>
@@ -7176,26 +7746,29 @@
       <c r="Q186" s="6"/>
       <c r="R186" s="7"/>
       <c r="S186" s="7"/>
-      <c r="T186" s="6">
+      <c r="T186" s="6"/>
+      <c r="U186" s="7"/>
+      <c r="V186" s="8"/>
+      <c r="W186" s="6">
         <v>3</v>
       </c>
-      <c r="U186" s="7">
+      <c r="X186" s="7">
         <v>2</v>
       </c>
-      <c r="V186" s="8">
+      <c r="Y186" s="8">
         <v>3</v>
       </c>
-      <c r="W186" s="16">
+      <c r="Z186" s="16">
         <v>1</v>
       </c>
-      <c r="X186" s="16">
+      <c r="AA186" s="16">
         <v>4</v>
       </c>
-      <c r="Y186" s="16">
+      <c r="AB186" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>15</v>
       </c>
@@ -7226,17 +7799,20 @@
       <c r="T187" s="6"/>
       <c r="U187" s="7"/>
       <c r="V187" s="8"/>
-      <c r="W187" s="7">
+      <c r="W187" s="6"/>
+      <c r="X187" s="7"/>
+      <c r="Y187" s="8"/>
+      <c r="Z187" s="7">
         <v>5</v>
       </c>
-      <c r="X187" s="7">
+      <c r="AA187" s="7">
         <v>0</v>
       </c>
-      <c r="Y187" s="7">
+      <c r="AB187" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>14</v>
       </c>
@@ -7273,17 +7849,20 @@
       <c r="T188" s="6"/>
       <c r="U188" s="7"/>
       <c r="V188" s="8"/>
-      <c r="W188" s="7">
+      <c r="W188" s="6"/>
+      <c r="X188" s="7"/>
+      <c r="Y188" s="8"/>
+      <c r="Z188" s="7">
         <v>4</v>
       </c>
-      <c r="X188" s="7">
+      <c r="AA188" s="7">
         <v>1</v>
       </c>
-      <c r="Y188" s="7">
+      <c r="AB188" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>13</v>
       </c>
@@ -7305,14 +7884,17 @@
       <c r="Q189" s="6"/>
       <c r="R189" s="7"/>
       <c r="S189" s="7"/>
-      <c r="T189" s="12"/>
-      <c r="U189" s="13"/>
-      <c r="V189" s="14"/>
-      <c r="W189" s="13"/>
+      <c r="T189" s="6"/>
+      <c r="U189" s="7"/>
+      <c r="V189" s="8"/>
+      <c r="W189" s="12"/>
       <c r="X189" s="13"/>
-      <c r="Y189" s="13"/>
-    </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y189" s="14"/>
+      <c r="Z189" s="13"/>
+      <c r="AA189" s="13"/>
+      <c r="AB189" s="13"/>
+    </row>
+    <row r="190" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>12</v>
       </c>
@@ -7346,29 +7928,32 @@
       <c r="S190" s="7">
         <v>3</v>
       </c>
-      <c r="T190" s="17">
+      <c r="T190" s="6"/>
+      <c r="U190" s="7"/>
+      <c r="V190" s="8"/>
+      <c r="W190" s="17">
         <v>1</v>
       </c>
-      <c r="U190" s="18">
+      <c r="X190" s="18">
         <v>4</v>
       </c>
-      <c r="V190" s="19">
+      <c r="Y190" s="19">
         <v>4</v>
       </c>
-      <c r="W190" s="18">
+      <c r="Z190" s="18">
         <v>3</v>
       </c>
-      <c r="X190" s="18">
+      <c r="AA190" s="18">
         <v>2</v>
       </c>
-      <c r="Y190" s="18">
+      <c r="AB190" s="18">
         <v>3</v>
       </c>
-      <c r="AC190" t="s">
+      <c r="AF190" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>11</v>
       </c>
@@ -7390,14 +7975,23 @@
       <c r="Q191" s="6"/>
       <c r="R191" s="7"/>
       <c r="S191" s="7"/>
-      <c r="T191" s="6"/>
-      <c r="U191" s="7"/>
-      <c r="V191" s="8"/>
-      <c r="W191" s="7"/>
+      <c r="T191" s="12">
+        <v>1</v>
+      </c>
+      <c r="U191" s="13">
+        <v>4</v>
+      </c>
+      <c r="V191" s="14">
+        <v>6</v>
+      </c>
+      <c r="W191" s="6"/>
       <c r="X191" s="7"/>
-      <c r="Y191" s="7"/>
-    </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Y191" s="8"/>
+      <c r="Z191" s="7"/>
+      <c r="AA191" s="7"/>
+      <c r="AB191" s="7"/>
+    </row>
+    <row r="192" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>10</v>
       </c>
@@ -7417,11 +8011,14 @@
       <c r="T192" s="6"/>
       <c r="U192" s="7"/>
       <c r="V192" s="8"/>
-      <c r="W192" s="7"/>
+      <c r="W192" s="6"/>
       <c r="X192" s="7"/>
-      <c r="Y192" s="7"/>
-    </row>
-    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y192" s="8"/>
+      <c r="Z192" s="7"/>
+      <c r="AA192" s="7"/>
+      <c r="AB192" s="7"/>
+    </row>
+    <row r="193" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>9</v>
       </c>
@@ -7452,14 +8049,17 @@
       <c r="S193" s="20">
         <v>1</v>
       </c>
-      <c r="T193" s="6"/>
-      <c r="U193" s="7"/>
-      <c r="V193" s="8"/>
-      <c r="W193" s="7"/>
+      <c r="T193" s="12"/>
+      <c r="U193" s="13"/>
+      <c r="V193" s="14"/>
+      <c r="W193" s="6"/>
       <c r="X193" s="7"/>
-      <c r="Y193" s="7"/>
-    </row>
-    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y193" s="8"/>
+      <c r="Z193" s="7"/>
+      <c r="AA193" s="7"/>
+      <c r="AB193" s="7"/>
+    </row>
+    <row r="194" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>8</v>
       </c>
@@ -7487,20 +8087,23 @@
       <c r="Q194" s="12"/>
       <c r="R194" s="16"/>
       <c r="S194" s="13"/>
-      <c r="T194" s="6"/>
-      <c r="U194" s="7"/>
-      <c r="V194" s="8"/>
-      <c r="W194" s="7">
+      <c r="T194" s="12"/>
+      <c r="U194" s="16"/>
+      <c r="V194" s="14"/>
+      <c r="W194" s="6"/>
+      <c r="X194" s="7"/>
+      <c r="Y194" s="8"/>
+      <c r="Z194" s="7">
         <v>2</v>
       </c>
-      <c r="X194" s="7">
+      <c r="AA194" s="7">
         <v>3</v>
       </c>
-      <c r="Y194" s="7">
+      <c r="AB194" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>7</v>
       </c>
@@ -7528,14 +8131,23 @@
       <c r="S195" s="13">
         <v>0</v>
       </c>
-      <c r="T195" s="6"/>
-      <c r="U195" s="7"/>
-      <c r="V195" s="8"/>
-      <c r="W195" s="7"/>
+      <c r="T195" s="12">
+        <v>2</v>
+      </c>
+      <c r="U195" s="13">
+        <v>3</v>
+      </c>
+      <c r="V195" s="14">
+        <v>5</v>
+      </c>
+      <c r="W195" s="6"/>
       <c r="X195" s="7"/>
-      <c r="Y195" s="7"/>
-    </row>
-    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y195" s="8"/>
+      <c r="Z195" s="7"/>
+      <c r="AA195" s="7"/>
+      <c r="AB195" s="7"/>
+    </row>
+    <row r="196" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>6</v>
       </c>
@@ -7563,20 +8175,23 @@
       <c r="S196" s="18">
         <v>3</v>
       </c>
-      <c r="T196" s="12">
+      <c r="T196" s="17"/>
+      <c r="U196" s="18"/>
+      <c r="V196" s="19"/>
+      <c r="W196" s="12">
         <v>2</v>
       </c>
-      <c r="U196" s="13">
+      <c r="X196" s="13">
         <v>3</v>
       </c>
-      <c r="V196" s="14">
+      <c r="Y196" s="14">
         <v>2</v>
       </c>
-      <c r="W196" s="13"/>
-      <c r="X196" s="13"/>
-      <c r="Y196" s="13"/>
-    </row>
-    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z196" s="13"/>
+      <c r="AA196" s="13"/>
+      <c r="AB196" s="13"/>
+    </row>
+    <row r="197" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>5</v>
       </c>
@@ -7614,11 +8229,14 @@
       <c r="T197" s="6"/>
       <c r="U197" s="7"/>
       <c r="V197" s="8"/>
-      <c r="W197" s="7"/>
+      <c r="W197" s="6"/>
       <c r="X197" s="7"/>
-      <c r="Y197" s="7"/>
-    </row>
-    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y197" s="8"/>
+      <c r="Z197" s="7"/>
+      <c r="AA197" s="7"/>
+      <c r="AB197" s="7"/>
+    </row>
+    <row r="198" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>4</v>
       </c>
@@ -7652,20 +8270,29 @@
       <c r="Q198" s="12"/>
       <c r="R198" s="13"/>
       <c r="S198" s="13"/>
-      <c r="T198" s="11"/>
-      <c r="U198" s="7"/>
-      <c r="V198" s="8"/>
-      <c r="W198" s="7">
+      <c r="T198" s="12">
         <v>3</v>
       </c>
-      <c r="X198" s="7">
+      <c r="U198" s="13">
         <v>2</v>
       </c>
-      <c r="Y198" s="7">
+      <c r="V198" s="14">
+        <v>4</v>
+      </c>
+      <c r="W198" s="11"/>
+      <c r="X198" s="7"/>
+      <c r="Y198" s="8"/>
+      <c r="Z198" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA198" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB198" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>3</v>
       </c>
@@ -7705,20 +8332,23 @@
       <c r="S199" s="13">
         <v>1</v>
       </c>
-      <c r="T199" s="12">
+      <c r="T199" s="12"/>
+      <c r="U199" s="13"/>
+      <c r="V199" s="14"/>
+      <c r="W199" s="12">
         <v>3</v>
       </c>
-      <c r="U199" s="13">
+      <c r="X199" s="13">
         <v>2</v>
       </c>
-      <c r="V199" s="14">
+      <c r="Y199" s="14">
         <v>1</v>
       </c>
-      <c r="W199" s="13"/>
-      <c r="X199" s="13"/>
-      <c r="Y199" s="13"/>
-    </row>
-    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z199" s="13"/>
+      <c r="AA199" s="13"/>
+      <c r="AB199" s="13"/>
+    </row>
+    <row r="200" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2</v>
       </c>
@@ -7759,19 +8389,28 @@
         <v>1</v>
       </c>
       <c r="V200" s="14">
-        <v>1</v>
-      </c>
-      <c r="W200" s="13">
+        <v>3</v>
+      </c>
+      <c r="W200" s="12">
         <v>4</v>
       </c>
       <c r="X200" s="13">
         <v>1</v>
       </c>
-      <c r="Y200" s="13">
+      <c r="Y200" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z200" s="13">
+        <v>4</v>
+      </c>
+      <c r="AA200" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB200" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1</v>
       </c>
@@ -7817,29 +8456,38 @@
       <c r="U201" s="13">
         <v>0</v>
       </c>
-      <c r="V201" s="14">
-        <v>1</v>
-      </c>
-      <c r="W201" s="13">
+      <c r="V201" s="23">
+        <v>2</v>
+      </c>
+      <c r="W201" s="12">
         <v>5</v>
       </c>
       <c r="X201" s="13">
         <v>0</v>
       </c>
-      <c r="Y201" s="13">
+      <c r="Y201" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z201" s="13">
+        <v>5</v>
+      </c>
+      <c r="AA201" s="13">
         <v>0</v>
       </c>
-      <c r="Z201" s="16">
+      <c r="AB201" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC201" s="16">
         <v>4</v>
       </c>
-      <c r="AA201" s="16">
+      <c r="AD201" s="16">
         <v>0</v>
       </c>
-      <c r="AB201" s="16">
+      <c r="AE201" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>0</v>
       </c>
@@ -7894,7 +8542,7 @@
       <c r="R202" s="7">
         <v>5</v>
       </c>
-      <c r="S202" s="8">
+      <c r="S202" s="7">
         <v>3</v>
       </c>
       <c r="T202" s="6">
@@ -7904,7 +8552,7 @@
         <v>5</v>
       </c>
       <c r="V202" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="W202" s="6">
         <v>0</v>
@@ -7922,26 +8570,47 @@
         <v>5</v>
       </c>
       <c r="AB202" s="8">
+        <v>4</v>
+      </c>
+      <c r="AC202" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD202" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AE202" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q204" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="T204" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q205" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="T205" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q206" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="T206" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Q207" t="s">
+        <v>12</v>
+      </c>
+      <c r="T207" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
search for math approach
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="13">
   <si>
     <t>floor</t>
   </si>
@@ -70,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,23 +92,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -145,15 +137,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -197,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,18 +220,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2106,10 +2097,10 @@
   <dimension ref="A1:AB209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O169" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y100" sqref="Y100"/>
+      <selection pane="bottomRight" activeCell="AA178" sqref="AA178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,6 +4084,15 @@
       <c r="N98" s="6"/>
       <c r="O98" s="7"/>
       <c r="P98" s="8"/>
+      <c r="X98" s="30">
+        <v>13</v>
+      </c>
+      <c r="Y98" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z98" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99">
@@ -4113,6 +4113,9 @@
       <c r="N99" s="6"/>
       <c r="O99" s="7"/>
       <c r="P99" s="8"/>
+      <c r="Y99" s="28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -4133,13 +4136,13 @@
       <c r="N100" s="6"/>
       <c r="O100" s="7"/>
       <c r="P100" s="8"/>
-      <c r="X100" s="32">
-        <v>12</v>
-      </c>
-      <c r="Y100" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z100" s="34">
+      <c r="X100" s="30">
+        <v>12</v>
+      </c>
+      <c r="Y100" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z100" s="32">
         <v>2</v>
       </c>
     </row>
@@ -4208,13 +4211,13 @@
       <c r="N103" s="6"/>
       <c r="O103" s="7"/>
       <c r="P103" s="8"/>
-      <c r="X103" s="32">
+      <c r="X103" s="30">
         <v>11</v>
       </c>
-      <c r="Y103" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z103" s="34">
+      <c r="Y103" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z103" s="32">
         <v>3</v>
       </c>
     </row>
@@ -4306,13 +4309,13 @@
       <c r="N107" s="6"/>
       <c r="O107" s="7"/>
       <c r="P107" s="8"/>
-      <c r="X107" s="32">
+      <c r="X107" s="30">
         <v>10</v>
       </c>
-      <c r="Y107" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z107" s="34">
+      <c r="Y107" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z107" s="32">
         <v>4</v>
       </c>
     </row>
@@ -4427,13 +4430,13 @@
       <c r="N112" s="6"/>
       <c r="O112" s="7"/>
       <c r="P112" s="8"/>
-      <c r="X112" s="32">
+      <c r="X112" s="30">
         <v>9</v>
       </c>
-      <c r="Y112" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z112" s="34">
+      <c r="Y112" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z112" s="32">
         <v>5</v>
       </c>
     </row>
@@ -4571,13 +4574,13 @@
       <c r="N118" s="6"/>
       <c r="O118" s="7"/>
       <c r="P118" s="8"/>
-      <c r="X118" s="32">
+      <c r="X118" s="30">
         <v>8</v>
       </c>
-      <c r="Y118" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z118" s="34">
+      <c r="Y118" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z118" s="32">
         <v>6</v>
       </c>
     </row>
@@ -4738,13 +4741,13 @@
       <c r="N125" s="6"/>
       <c r="O125" s="7"/>
       <c r="P125" s="8"/>
-      <c r="X125" s="32">
+      <c r="X125" s="30">
         <v>7</v>
       </c>
-      <c r="Y125" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z125" s="34">
+      <c r="Y125" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z125" s="32">
         <v>7</v>
       </c>
     </row>
@@ -4928,13 +4931,13 @@
       <c r="N133" s="6"/>
       <c r="O133" s="7"/>
       <c r="P133" s="8"/>
-      <c r="X133" s="32">
+      <c r="X133" s="30">
         <v>6</v>
       </c>
-      <c r="Y133" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z133" s="34">
+      <c r="Y133" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z133" s="32">
         <v>8</v>
       </c>
     </row>
@@ -5141,13 +5144,13 @@
       <c r="N142" s="6"/>
       <c r="O142" s="7"/>
       <c r="P142" s="8"/>
-      <c r="X142" s="32">
+      <c r="X142" s="30">
         <v>5</v>
       </c>
-      <c r="Y142" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z142" s="34">
+      <c r="Y142" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z142" s="32">
         <v>9</v>
       </c>
     </row>
@@ -5377,13 +5380,13 @@
       <c r="N152" s="6"/>
       <c r="O152" s="7"/>
       <c r="P152" s="8"/>
-      <c r="X152" s="32">
+      <c r="X152" s="30">
         <v>4</v>
       </c>
-      <c r="Y152" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z152" s="34">
+      <c r="Y152" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z152" s="32">
         <v>10</v>
       </c>
     </row>
@@ -5636,13 +5639,13 @@
       <c r="N163" s="6"/>
       <c r="O163" s="7"/>
       <c r="P163" s="8"/>
-      <c r="X163" s="32">
+      <c r="X163" s="30">
         <v>3</v>
       </c>
-      <c r="Y163" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z163" s="34">
+      <c r="Y163" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z163" s="32">
         <v>11</v>
       </c>
     </row>
@@ -5849,13 +5852,13 @@
       <c r="N172" s="6"/>
       <c r="O172" s="7"/>
       <c r="P172" s="8"/>
-      <c r="U172" s="29">
+      <c r="U172" s="44">
         <v>5</v>
       </c>
-      <c r="V172" s="29">
+      <c r="V172" s="45">
         <v>3</v>
       </c>
-      <c r="W172" s="29">
+      <c r="W172" s="46">
         <v>0</v>
       </c>
       <c r="Y172" s="28" t="s">
@@ -5881,13 +5884,13 @@
       <c r="N173" s="6"/>
       <c r="O173" s="7"/>
       <c r="P173" s="8"/>
-      <c r="U173" s="29">
+      <c r="U173" s="43">
         <v>4</v>
       </c>
-      <c r="V173" s="29">
+      <c r="V173" s="41">
         <v>3</v>
       </c>
-      <c r="W173" s="29">
+      <c r="W173" s="42">
         <v>1</v>
       </c>
       <c r="Y173" s="28" t="s">
@@ -5939,22 +5942,22 @@
       <c r="N175" s="6"/>
       <c r="O175" s="7"/>
       <c r="P175" s="8"/>
-      <c r="U175" s="29">
+      <c r="U175" s="43">
         <v>3</v>
       </c>
-      <c r="V175" s="29">
+      <c r="V175" s="41">
         <v>3</v>
       </c>
-      <c r="W175" s="29">
+      <c r="W175" s="42">
         <v>2</v>
       </c>
-      <c r="X175" s="38">
+      <c r="X175" s="35">
         <v>2</v>
       </c>
-      <c r="Y175" s="39">
-        <v>1</v>
-      </c>
-      <c r="Z175" s="40">
+      <c r="Y175" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z175" s="37">
         <v>12</v>
       </c>
     </row>
@@ -6009,7 +6012,7 @@
       <c r="N177" s="6"/>
       <c r="O177" s="7"/>
       <c r="P177" s="8"/>
-      <c r="U177">
+      <c r="U177" s="26">
         <v>4</v>
       </c>
       <c r="V177">
@@ -6067,16 +6070,16 @@
       <c r="N179" s="6"/>
       <c r="O179" s="7"/>
       <c r="P179" s="8"/>
-      <c r="U179" s="31">
+      <c r="U179" s="48">
         <v>2</v>
       </c>
-      <c r="V179" s="29">
+      <c r="V179" s="41">
         <v>3</v>
       </c>
-      <c r="W179" s="29">
+      <c r="W179" s="42">
         <v>3</v>
       </c>
-      <c r="X179" s="30"/>
+      <c r="X179" s="29"/>
       <c r="Y179" s="28" t="s">
         <v>12</v>
       </c>
@@ -6190,13 +6193,13 @@
       <c r="N183" s="6"/>
       <c r="O183" s="7"/>
       <c r="P183" s="8"/>
-      <c r="U183">
+      <c r="U183" s="30">
         <v>3</v>
       </c>
-      <c r="V183">
+      <c r="V183" s="31">
         <v>2</v>
       </c>
-      <c r="W183">
+      <c r="W183" s="32">
         <v>2</v>
       </c>
       <c r="Y183" s="28" t="s">
@@ -6312,16 +6315,16 @@
       <c r="N187" s="6"/>
       <c r="O187" s="7"/>
       <c r="P187" s="8"/>
-      <c r="U187" s="35">
-        <v>1</v>
-      </c>
-      <c r="V187" s="36">
+      <c r="U187" s="47">
+        <v>1</v>
+      </c>
+      <c r="V187" s="39">
+        <v>3</v>
+      </c>
+      <c r="W187" s="40">
         <v>4</v>
       </c>
-      <c r="W187" s="37">
-        <v>4</v>
-      </c>
-      <c r="X187" s="30"/>
+      <c r="X187" s="29"/>
       <c r="Y187" s="28" t="s">
         <v>12</v>
       </c>
@@ -6363,13 +6366,13 @@
       <c r="W188">
         <v>0</v>
       </c>
-      <c r="X188" s="32">
-        <v>1</v>
-      </c>
-      <c r="Y188" s="33">
-        <v>1</v>
-      </c>
-      <c r="Z188" s="34">
+      <c r="X188" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y188" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z188" s="32">
         <v>13</v>
       </c>
     </row>
@@ -6450,13 +6453,13 @@
       <c r="K191" s="6"/>
       <c r="L191" s="7"/>
       <c r="M191" s="8"/>
-      <c r="U191">
+      <c r="U191" s="30">
         <v>3</v>
       </c>
-      <c r="V191">
+      <c r="V191" s="31">
         <v>2</v>
       </c>
-      <c r="W191">
+      <c r="W191" s="32">
         <v>2</v>
       </c>
       <c r="Y191" s="28" t="s">
@@ -6613,13 +6616,13 @@
       <c r="Q195" s="14"/>
       <c r="R195" s="14"/>
       <c r="S195" s="14"/>
-      <c r="U195" s="16">
+      <c r="U195" s="38">
         <v>2</v>
       </c>
-      <c r="V195" s="16">
+      <c r="V195" s="33">
         <v>2</v>
       </c>
-      <c r="W195" s="16">
+      <c r="W195" s="34">
         <v>3</v>
       </c>
       <c r="Y195" s="28" t="s">

</xml_diff>

<commit_message>
visualise floors and recursion
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>floor</t>
   </si>
@@ -65,6 +64,21 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> attempt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eggs</t>
   </si>
 </sst>
 </file>
@@ -113,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,24 +177,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -216,30 +217,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,301 +250,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>98533</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>433552</xdr:colOff>
-      <xdr:row>201</xdr:row>
-      <xdr:rowOff>105102</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Left Bracket 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{753B08FD-D08F-4FFE-A905-50DF7AABA7ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12455744" y="37246033"/>
-          <a:ext cx="176377" cy="1340069"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>580368</xdr:colOff>
-      <xdr:row>198</xdr:row>
-      <xdr:rowOff>105103</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>145831</xdr:colOff>
-      <xdr:row>201</xdr:row>
-      <xdr:rowOff>112985</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Left Bracket 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F233B23E-4062-499B-89AA-37342EA4BA6E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12168023" y="38014603"/>
-          <a:ext cx="176377" cy="579382"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>575113</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>111672</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>140576</xdr:colOff>
-      <xdr:row>198</xdr:row>
-      <xdr:rowOff>28902</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Left Bracket 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFEB2A9C-A0A2-49F0-98D9-5CC9594112C2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12162768" y="37259172"/>
-          <a:ext cx="176377" cy="679230"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>313669</xdr:colOff>
-      <xdr:row>196</xdr:row>
-      <xdr:rowOff>111672</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>490046</xdr:colOff>
-      <xdr:row>198</xdr:row>
-      <xdr:rowOff>30216</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Left Bracket 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E7CED9F-58E5-4363-98C7-2CA0D775CAE5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11901324" y="37640172"/>
-          <a:ext cx="176377" cy="299544"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>314982</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>106417</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>491359</xdr:colOff>
-      <xdr:row>196</xdr:row>
-      <xdr:rowOff>24961</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Left Bracket 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6A6197-90BD-4CA1-9AFA-2623AE5A302C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11902637" y="37253917"/>
-          <a:ext cx="176377" cy="299544"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBracket">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2094,13 +1794,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB209"/>
+  <dimension ref="A1:AC209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O169" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O184" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA178" sqref="AA178"/>
+      <selection pane="bottomRight" activeCell="AC198" sqref="AC198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,7 +1810,7 @@
     <col min="3" max="4" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2141,11 +1841,38 @@
       <c r="R1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -2164,8 +1891,13 @@
       <c r="N2" s="6"/>
       <c r="O2" s="7"/>
       <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="6"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>199</v>
       </c>
@@ -2184,8 +1916,13 @@
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
       <c r="P3" s="8"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="6"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>198</v>
       </c>
@@ -2204,8 +1941,13 @@
       <c r="N4" s="6"/>
       <c r="O4" s="7"/>
       <c r="P4" s="8"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="6"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="8"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>197</v>
       </c>
@@ -2224,8 +1966,13 @@
       <c r="N5" s="6"/>
       <c r="O5" s="7"/>
       <c r="P5" s="8"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="6"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="8"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>196</v>
       </c>
@@ -2244,8 +1991,13 @@
       <c r="N6" s="6"/>
       <c r="O6" s="7"/>
       <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="6"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="8"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>195</v>
       </c>
@@ -2264,8 +2016,13 @@
       <c r="N7" s="6"/>
       <c r="O7" s="7"/>
       <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="6"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="8"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>194</v>
       </c>
@@ -2284,8 +2041,13 @@
       <c r="N8" s="6"/>
       <c r="O8" s="7"/>
       <c r="P8" s="8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="6"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>193</v>
       </c>
@@ -2304,8 +2066,13 @@
       <c r="N9" s="6"/>
       <c r="O9" s="7"/>
       <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="6"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>192</v>
       </c>
@@ -2324,8 +2091,13 @@
       <c r="N10" s="6"/>
       <c r="O10" s="7"/>
       <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="6"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="8"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>191</v>
       </c>
@@ -2344,8 +2116,13 @@
       <c r="N11" s="6"/>
       <c r="O11" s="7"/>
       <c r="P11" s="8"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="6"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="8"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>190</v>
       </c>
@@ -2364,8 +2141,13 @@
       <c r="N12" s="6"/>
       <c r="O12" s="7"/>
       <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="6"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="8"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>189</v>
       </c>
@@ -2384,8 +2166,13 @@
       <c r="N13" s="6"/>
       <c r="O13" s="7"/>
       <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="6"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="8"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>188</v>
       </c>
@@ -2404,8 +2191,13 @@
       <c r="N14" s="6"/>
       <c r="O14" s="7"/>
       <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="6"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>187</v>
       </c>
@@ -2424,8 +2216,13 @@
       <c r="N15" s="6"/>
       <c r="O15" s="7"/>
       <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="6"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>186</v>
       </c>
@@ -2444,8 +2241,13 @@
       <c r="N16" s="6"/>
       <c r="O16" s="7"/>
       <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T16" s="6"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>185</v>
       </c>
@@ -2464,8 +2266,13 @@
       <c r="N17" s="6"/>
       <c r="O17" s="7"/>
       <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T17" s="6"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>184</v>
       </c>
@@ -2484,8 +2291,13 @@
       <c r="N18" s="6"/>
       <c r="O18" s="7"/>
       <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T18" s="6"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>183</v>
       </c>
@@ -2504,8 +2316,13 @@
       <c r="N19" s="6"/>
       <c r="O19" s="7"/>
       <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T19" s="6"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>182</v>
       </c>
@@ -2524,8 +2341,13 @@
       <c r="N20" s="6"/>
       <c r="O20" s="7"/>
       <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T20" s="6"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>181</v>
       </c>
@@ -2544,8 +2366,13 @@
       <c r="N21" s="6"/>
       <c r="O21" s="7"/>
       <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T21" s="6"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>180</v>
       </c>
@@ -2564,8 +2391,13 @@
       <c r="N22" s="6"/>
       <c r="O22" s="7"/>
       <c r="P22" s="8"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T22" s="6"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>179</v>
       </c>
@@ -2584,8 +2416,13 @@
       <c r="N23" s="6"/>
       <c r="O23" s="7"/>
       <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T23" s="6"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>178</v>
       </c>
@@ -2604,8 +2441,13 @@
       <c r="N24" s="6"/>
       <c r="O24" s="7"/>
       <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T24" s="6"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>177</v>
       </c>
@@ -2624,8 +2466,13 @@
       <c r="N25" s="6"/>
       <c r="O25" s="7"/>
       <c r="P25" s="8"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T25" s="6"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>176</v>
       </c>
@@ -2644,8 +2491,13 @@
       <c r="N26" s="6"/>
       <c r="O26" s="7"/>
       <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T26" s="6"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="8"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>175</v>
       </c>
@@ -2664,8 +2516,13 @@
       <c r="N27" s="6"/>
       <c r="O27" s="7"/>
       <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T27" s="6"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>174</v>
       </c>
@@ -2684,8 +2541,13 @@
       <c r="N28" s="6"/>
       <c r="O28" s="7"/>
       <c r="P28" s="8"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T28" s="6"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="8"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>173</v>
       </c>
@@ -2704,8 +2566,13 @@
       <c r="N29" s="6"/>
       <c r="O29" s="7"/>
       <c r="P29" s="8"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T29" s="6"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="8"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>172</v>
       </c>
@@ -2724,8 +2591,13 @@
       <c r="N30" s="6"/>
       <c r="O30" s="7"/>
       <c r="P30" s="8"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T30" s="6"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="8"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>171</v>
       </c>
@@ -2744,8 +2616,13 @@
       <c r="N31" s="6"/>
       <c r="O31" s="7"/>
       <c r="P31" s="8"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T31" s="6"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>170</v>
       </c>
@@ -2764,8 +2641,13 @@
       <c r="N32" s="6"/>
       <c r="O32" s="7"/>
       <c r="P32" s="8"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T32" s="6"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>169</v>
       </c>
@@ -2784,8 +2666,13 @@
       <c r="N33" s="6"/>
       <c r="O33" s="7"/>
       <c r="P33" s="8"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T33" s="6"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>168</v>
       </c>
@@ -2804,8 +2691,13 @@
       <c r="N34" s="6"/>
       <c r="O34" s="7"/>
       <c r="P34" s="8"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T34" s="6"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="8"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>167</v>
       </c>
@@ -2824,8 +2716,13 @@
       <c r="N35" s="6"/>
       <c r="O35" s="7"/>
       <c r="P35" s="8"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T35" s="6"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>166</v>
       </c>
@@ -2844,8 +2741,13 @@
       <c r="N36" s="6"/>
       <c r="O36" s="7"/>
       <c r="P36" s="8"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T36" s="6"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="8"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>165</v>
       </c>
@@ -2864,8 +2766,13 @@
       <c r="N37" s="6"/>
       <c r="O37" s="7"/>
       <c r="P37" s="8"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T37" s="6"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="8"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>164</v>
       </c>
@@ -2884,8 +2791,13 @@
       <c r="N38" s="6"/>
       <c r="O38" s="7"/>
       <c r="P38" s="8"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T38" s="6"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>163</v>
       </c>
@@ -2904,8 +2816,13 @@
       <c r="N39" s="6"/>
       <c r="O39" s="7"/>
       <c r="P39" s="8"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T39" s="6"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="8"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>162</v>
       </c>
@@ -2924,8 +2841,13 @@
       <c r="N40" s="6"/>
       <c r="O40" s="7"/>
       <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T40" s="6"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="8"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>161</v>
       </c>
@@ -2944,8 +2866,13 @@
       <c r="N41" s="6"/>
       <c r="O41" s="7"/>
       <c r="P41" s="8"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T41" s="6"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="8"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>160</v>
       </c>
@@ -2964,8 +2891,13 @@
       <c r="N42" s="6"/>
       <c r="O42" s="7"/>
       <c r="P42" s="8"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T42" s="6"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="8"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>159</v>
       </c>
@@ -2984,8 +2916,13 @@
       <c r="N43" s="6"/>
       <c r="O43" s="7"/>
       <c r="P43" s="8"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T43" s="6"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="7"/>
+      <c r="X43" s="8"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>158</v>
       </c>
@@ -3004,8 +2941,13 @@
       <c r="N44" s="6"/>
       <c r="O44" s="7"/>
       <c r="P44" s="8"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T44" s="6"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="8"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>157</v>
       </c>
@@ -3024,8 +2966,13 @@
       <c r="N45" s="6"/>
       <c r="O45" s="7"/>
       <c r="P45" s="8"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T45" s="6"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="8"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>156</v>
       </c>
@@ -3044,8 +2991,13 @@
       <c r="N46" s="6"/>
       <c r="O46" s="7"/>
       <c r="P46" s="8"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T46" s="6"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="8"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>155</v>
       </c>
@@ -3064,8 +3016,13 @@
       <c r="N47" s="6"/>
       <c r="O47" s="7"/>
       <c r="P47" s="8"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T47" s="6"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="8"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>154</v>
       </c>
@@ -3084,8 +3041,13 @@
       <c r="N48" s="6"/>
       <c r="O48" s="7"/>
       <c r="P48" s="8"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T48" s="6"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="8"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>153</v>
       </c>
@@ -3104,8 +3066,13 @@
       <c r="N49" s="6"/>
       <c r="O49" s="7"/>
       <c r="P49" s="8"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T49" s="6"/>
+      <c r="U49" s="7"/>
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="8"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>152</v>
       </c>
@@ -3124,8 +3091,13 @@
       <c r="N50" s="6"/>
       <c r="O50" s="7"/>
       <c r="P50" s="8"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T50" s="6"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="8"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>151</v>
       </c>
@@ -3144,8 +3116,13 @@
       <c r="N51" s="6"/>
       <c r="O51" s="7"/>
       <c r="P51" s="8"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T51" s="6"/>
+      <c r="U51" s="7"/>
+      <c r="V51" s="7"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="8"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>150</v>
       </c>
@@ -3164,8 +3141,13 @@
       <c r="N52" s="6"/>
       <c r="O52" s="7"/>
       <c r="P52" s="8"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T52" s="6"/>
+      <c r="U52" s="7"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="8"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>149</v>
       </c>
@@ -3184,8 +3166,13 @@
       <c r="N53" s="6"/>
       <c r="O53" s="7"/>
       <c r="P53" s="8"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T53" s="6"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="8"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>148</v>
       </c>
@@ -3204,8 +3191,13 @@
       <c r="N54" s="6"/>
       <c r="O54" s="7"/>
       <c r="P54" s="8"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T54" s="6"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="8"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>147</v>
       </c>
@@ -3224,8 +3216,13 @@
       <c r="N55" s="6"/>
       <c r="O55" s="7"/>
       <c r="P55" s="8"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T55" s="6"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="8"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>146</v>
       </c>
@@ -3244,8 +3241,13 @@
       <c r="N56" s="6"/>
       <c r="O56" s="7"/>
       <c r="P56" s="8"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T56" s="6"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="8"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>145</v>
       </c>
@@ -3264,8 +3266,13 @@
       <c r="N57" s="6"/>
       <c r="O57" s="7"/>
       <c r="P57" s="8"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T57" s="6"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="8"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>144</v>
       </c>
@@ -3284,8 +3291,13 @@
       <c r="N58" s="6"/>
       <c r="O58" s="7"/>
       <c r="P58" s="8"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T58" s="6"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="8"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>143</v>
       </c>
@@ -3304,8 +3316,13 @@
       <c r="N59" s="6"/>
       <c r="O59" s="7"/>
       <c r="P59" s="8"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T59" s="6"/>
+      <c r="U59" s="7"/>
+      <c r="V59" s="7"/>
+      <c r="W59" s="7"/>
+      <c r="X59" s="8"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>142</v>
       </c>
@@ -3324,8 +3341,13 @@
       <c r="N60" s="6"/>
       <c r="O60" s="7"/>
       <c r="P60" s="8"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T60" s="6"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="8"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>141</v>
       </c>
@@ -3344,8 +3366,13 @@
       <c r="N61" s="6"/>
       <c r="O61" s="7"/>
       <c r="P61" s="8"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T61" s="6"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="8"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>140</v>
       </c>
@@ -3364,8 +3391,13 @@
       <c r="N62" s="6"/>
       <c r="O62" s="7"/>
       <c r="P62" s="8"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T62" s="6"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="8"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>139</v>
       </c>
@@ -3384,8 +3416,13 @@
       <c r="N63" s="6"/>
       <c r="O63" s="7"/>
       <c r="P63" s="8"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T63" s="6"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="8"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>138</v>
       </c>
@@ -3404,8 +3441,13 @@
       <c r="N64" s="6"/>
       <c r="O64" s="7"/>
       <c r="P64" s="8"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T64" s="6"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="8"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>137</v>
       </c>
@@ -3424,8 +3466,13 @@
       <c r="N65" s="6"/>
       <c r="O65" s="7"/>
       <c r="P65" s="8"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T65" s="6"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="8"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>136</v>
       </c>
@@ -3444,8 +3491,13 @@
       <c r="N66" s="6"/>
       <c r="O66" s="7"/>
       <c r="P66" s="8"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T66" s="6"/>
+      <c r="U66" s="7"/>
+      <c r="V66" s="7"/>
+      <c r="W66" s="7"/>
+      <c r="X66" s="8"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>135</v>
       </c>
@@ -3464,8 +3516,13 @@
       <c r="N67" s="6"/>
       <c r="O67" s="7"/>
       <c r="P67" s="8"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T67" s="6"/>
+      <c r="U67" s="7"/>
+      <c r="V67" s="7"/>
+      <c r="W67" s="7"/>
+      <c r="X67" s="8"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>134</v>
       </c>
@@ -3484,8 +3541,13 @@
       <c r="N68" s="6"/>
       <c r="O68" s="7"/>
       <c r="P68" s="8"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T68" s="6"/>
+      <c r="U68" s="7"/>
+      <c r="V68" s="7"/>
+      <c r="W68" s="7"/>
+      <c r="X68" s="8"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>133</v>
       </c>
@@ -3504,8 +3566,13 @@
       <c r="N69" s="6"/>
       <c r="O69" s="7"/>
       <c r="P69" s="8"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T69" s="6"/>
+      <c r="U69" s="7"/>
+      <c r="V69" s="7"/>
+      <c r="W69" s="7"/>
+      <c r="X69" s="8"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>132</v>
       </c>
@@ -3524,8 +3591,13 @@
       <c r="N70" s="6"/>
       <c r="O70" s="7"/>
       <c r="P70" s="8"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T70" s="6"/>
+      <c r="U70" s="7"/>
+      <c r="V70" s="7"/>
+      <c r="W70" s="7"/>
+      <c r="X70" s="8"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>131</v>
       </c>
@@ -3544,8 +3616,13 @@
       <c r="N71" s="6"/>
       <c r="O71" s="7"/>
       <c r="P71" s="8"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T71" s="6"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="8"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>130</v>
       </c>
@@ -3564,8 +3641,13 @@
       <c r="N72" s="6"/>
       <c r="O72" s="7"/>
       <c r="P72" s="8"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T72" s="6"/>
+      <c r="U72" s="7"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="7"/>
+      <c r="X72" s="8"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>129</v>
       </c>
@@ -3584,8 +3666,13 @@
       <c r="N73" s="6"/>
       <c r="O73" s="7"/>
       <c r="P73" s="8"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T73" s="6"/>
+      <c r="U73" s="7"/>
+      <c r="V73" s="7"/>
+      <c r="W73" s="7"/>
+      <c r="X73" s="8"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>128</v>
       </c>
@@ -3604,8 +3691,13 @@
       <c r="N74" s="6"/>
       <c r="O74" s="7"/>
       <c r="P74" s="8"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T74" s="6"/>
+      <c r="U74" s="7"/>
+      <c r="V74" s="7"/>
+      <c r="W74" s="7"/>
+      <c r="X74" s="8"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>127</v>
       </c>
@@ -3624,8 +3716,13 @@
       <c r="N75" s="6"/>
       <c r="O75" s="7"/>
       <c r="P75" s="8"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T75" s="6"/>
+      <c r="U75" s="7"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="8"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>126</v>
       </c>
@@ -3644,8 +3741,13 @@
       <c r="N76" s="6"/>
       <c r="O76" s="7"/>
       <c r="P76" s="8"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T76" s="6"/>
+      <c r="U76" s="7"/>
+      <c r="V76" s="7"/>
+      <c r="W76" s="7"/>
+      <c r="X76" s="8"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>125</v>
       </c>
@@ -3664,8 +3766,13 @@
       <c r="N77" s="6"/>
       <c r="O77" s="7"/>
       <c r="P77" s="8"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T77" s="6"/>
+      <c r="U77" s="7"/>
+      <c r="V77" s="7"/>
+      <c r="W77" s="7"/>
+      <c r="X77" s="8"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>124</v>
       </c>
@@ -3684,8 +3791,13 @@
       <c r="N78" s="6"/>
       <c r="O78" s="7"/>
       <c r="P78" s="8"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T78" s="6"/>
+      <c r="U78" s="7"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="7"/>
+      <c r="X78" s="8"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>123</v>
       </c>
@@ -3704,8 +3816,13 @@
       <c r="N79" s="6"/>
       <c r="O79" s="7"/>
       <c r="P79" s="8"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T79" s="6"/>
+      <c r="U79" s="7"/>
+      <c r="V79" s="7"/>
+      <c r="W79" s="7"/>
+      <c r="X79" s="8"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>122</v>
       </c>
@@ -3724,8 +3841,13 @@
       <c r="N80" s="6"/>
       <c r="O80" s="7"/>
       <c r="P80" s="8"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T80" s="6"/>
+      <c r="U80" s="7"/>
+      <c r="V80" s="7"/>
+      <c r="W80" s="7"/>
+      <c r="X80" s="8"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>121</v>
       </c>
@@ -3744,8 +3866,13 @@
       <c r="N81" s="6"/>
       <c r="O81" s="7"/>
       <c r="P81" s="8"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T81" s="6"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="8"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>120</v>
       </c>
@@ -3764,8 +3891,13 @@
       <c r="N82" s="6"/>
       <c r="O82" s="7"/>
       <c r="P82" s="8"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T82" s="6"/>
+      <c r="U82" s="7"/>
+      <c r="V82" s="7"/>
+      <c r="W82" s="7"/>
+      <c r="X82" s="8"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>119</v>
       </c>
@@ -3784,8 +3916,13 @@
       <c r="N83" s="6"/>
       <c r="O83" s="7"/>
       <c r="P83" s="8"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T83" s="6"/>
+      <c r="U83" s="7"/>
+      <c r="V83" s="7"/>
+      <c r="W83" s="7"/>
+      <c r="X83" s="8"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>118</v>
       </c>
@@ -3804,8 +3941,13 @@
       <c r="N84" s="6"/>
       <c r="O84" s="7"/>
       <c r="P84" s="8"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T84" s="6"/>
+      <c r="U84" s="7"/>
+      <c r="V84" s="7"/>
+      <c r="W84" s="7"/>
+      <c r="X84" s="8"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>117</v>
       </c>
@@ -3824,8 +3966,15 @@
       <c r="N85" s="6"/>
       <c r="O85" s="7"/>
       <c r="P85" s="8"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T85" s="6"/>
+      <c r="U85" s="7"/>
+      <c r="V85" s="7"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="8"/>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>116</v>
       </c>
@@ -3844,8 +3993,15 @@
       <c r="N86" s="6"/>
       <c r="O86" s="7"/>
       <c r="P86" s="8"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T86" s="6"/>
+      <c r="U86" s="7"/>
+      <c r="V86" s="7"/>
+      <c r="W86" s="7"/>
+      <c r="X86" s="8"/>
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>115</v>
       </c>
@@ -3864,8 +4020,15 @@
       <c r="N87" s="6"/>
       <c r="O87" s="7"/>
       <c r="P87" s="8"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T87" s="6"/>
+      <c r="U87" s="7"/>
+      <c r="V87" s="7"/>
+      <c r="W87" s="7"/>
+      <c r="X87" s="8"/>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>114</v>
       </c>
@@ -3884,8 +4047,15 @@
       <c r="N88" s="6"/>
       <c r="O88" s="7"/>
       <c r="P88" s="8"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T88" s="6"/>
+      <c r="U88" s="7"/>
+      <c r="V88" s="7"/>
+      <c r="W88" s="7"/>
+      <c r="X88" s="8"/>
+      <c r="Y88" s="7"/>
+      <c r="Z88" s="7"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>113</v>
       </c>
@@ -3904,8 +4074,15 @@
       <c r="N89" s="6"/>
       <c r="O89" s="7"/>
       <c r="P89" s="8"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T89" s="6"/>
+      <c r="U89" s="7"/>
+      <c r="V89" s="7"/>
+      <c r="W89" s="7"/>
+      <c r="X89" s="8"/>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>112</v>
       </c>
@@ -3924,8 +4101,15 @@
       <c r="N90" s="6"/>
       <c r="O90" s="7"/>
       <c r="P90" s="8"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T90" s="6"/>
+      <c r="U90" s="7"/>
+      <c r="V90" s="7"/>
+      <c r="W90" s="7"/>
+      <c r="X90" s="8"/>
+      <c r="Y90" s="7"/>
+      <c r="Z90" s="7"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>111</v>
       </c>
@@ -3944,8 +4128,15 @@
       <c r="N91" s="6"/>
       <c r="O91" s="7"/>
       <c r="P91" s="8"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T91" s="6"/>
+      <c r="U91" s="7"/>
+      <c r="V91" s="7"/>
+      <c r="W91" s="7"/>
+      <c r="X91" s="8"/>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>110</v>
       </c>
@@ -3964,8 +4155,15 @@
       <c r="N92" s="6"/>
       <c r="O92" s="7"/>
       <c r="P92" s="8"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T92" s="6"/>
+      <c r="U92" s="7"/>
+      <c r="V92" s="7"/>
+      <c r="W92" s="7"/>
+      <c r="X92" s="8"/>
+      <c r="Y92" s="7"/>
+      <c r="Z92" s="7"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>109</v>
       </c>
@@ -3984,8 +4182,15 @@
       <c r="N93" s="6"/>
       <c r="O93" s="7"/>
       <c r="P93" s="8"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T93" s="6"/>
+      <c r="U93" s="7"/>
+      <c r="V93" s="7"/>
+      <c r="W93" s="7"/>
+      <c r="X93" s="8"/>
+      <c r="Y93" s="7"/>
+      <c r="Z93" s="7"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>108</v>
       </c>
@@ -4004,8 +4209,15 @@
       <c r="N94" s="6"/>
       <c r="O94" s="7"/>
       <c r="P94" s="8"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T94" s="6"/>
+      <c r="U94" s="7"/>
+      <c r="V94" s="7"/>
+      <c r="W94" s="7"/>
+      <c r="X94" s="8"/>
+      <c r="Y94" s="7"/>
+      <c r="Z94" s="7"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>107</v>
       </c>
@@ -4024,8 +4236,15 @@
       <c r="N95" s="6"/>
       <c r="O95" s="7"/>
       <c r="P95" s="8"/>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="T95" s="6"/>
+      <c r="U95" s="7"/>
+      <c r="V95" s="7"/>
+      <c r="W95" s="7"/>
+      <c r="X95" s="8"/>
+      <c r="Y95" s="7"/>
+      <c r="Z95" s="7"/>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>106</v>
       </c>
@@ -4044,6 +4263,13 @@
       <c r="N96" s="6"/>
       <c r="O96" s="7"/>
       <c r="P96" s="8"/>
+      <c r="T96" s="6"/>
+      <c r="U96" s="7"/>
+      <c r="V96" s="7"/>
+      <c r="W96" s="7"/>
+      <c r="X96" s="8"/>
+      <c r="Y96" s="7"/>
+      <c r="Z96" s="7"/>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -4064,6 +4290,13 @@
       <c r="N97" s="6"/>
       <c r="O97" s="7"/>
       <c r="P97" s="8"/>
+      <c r="T97" s="6"/>
+      <c r="U97" s="7"/>
+      <c r="V97" s="7"/>
+      <c r="W97" s="7"/>
+      <c r="X97" s="8"/>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7"/>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98">
@@ -4084,15 +4317,13 @@
       <c r="N98" s="6"/>
       <c r="O98" s="7"/>
       <c r="P98" s="8"/>
-      <c r="X98" s="30">
-        <v>13</v>
-      </c>
-      <c r="Y98" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z98" s="32">
-        <v>1</v>
-      </c>
+      <c r="T98" s="6"/>
+      <c r="U98" s="7"/>
+      <c r="V98" s="7"/>
+      <c r="W98" s="7"/>
+      <c r="X98" s="8"/>
+      <c r="Y98" s="7"/>
+      <c r="Z98" s="7"/>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99">
@@ -4113,9 +4344,13 @@
       <c r="N99" s="6"/>
       <c r="O99" s="7"/>
       <c r="P99" s="8"/>
-      <c r="Y99" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T99" s="6"/>
+      <c r="U99" s="7"/>
+      <c r="V99" s="7"/>
+      <c r="W99" s="7"/>
+      <c r="X99" s="8"/>
+      <c r="Y99" s="38"/>
+      <c r="Z99" s="7"/>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -4136,15 +4371,13 @@
       <c r="N100" s="6"/>
       <c r="O100" s="7"/>
       <c r="P100" s="8"/>
-      <c r="X100" s="30">
-        <v>12</v>
-      </c>
-      <c r="Y100" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z100" s="32">
-        <v>2</v>
-      </c>
+      <c r="T100" s="6"/>
+      <c r="U100" s="7"/>
+      <c r="V100" s="7"/>
+      <c r="W100" s="7"/>
+      <c r="X100" s="8"/>
+      <c r="Y100" s="7"/>
+      <c r="Z100" s="7"/>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -4165,9 +4398,13 @@
       <c r="N101" s="6"/>
       <c r="O101" s="7"/>
       <c r="P101" s="8"/>
-      <c r="Y101" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T101" s="6"/>
+      <c r="U101" s="7"/>
+      <c r="V101" s="7"/>
+      <c r="W101" s="7"/>
+      <c r="X101" s="8"/>
+      <c r="Y101" s="38"/>
+      <c r="Z101" s="7"/>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102">
@@ -4188,9 +4425,13 @@
       <c r="N102" s="6"/>
       <c r="O102" s="7"/>
       <c r="P102" s="8"/>
-      <c r="Y102" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T102" s="6"/>
+      <c r="U102" s="7"/>
+      <c r="V102" s="7"/>
+      <c r="W102" s="7"/>
+      <c r="X102" s="8"/>
+      <c r="Y102" s="38"/>
+      <c r="Z102" s="7"/>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103">
@@ -4211,15 +4452,13 @@
       <c r="N103" s="6"/>
       <c r="O103" s="7"/>
       <c r="P103" s="8"/>
-      <c r="X103" s="30">
-        <v>11</v>
-      </c>
-      <c r="Y103" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z103" s="32">
-        <v>3</v>
-      </c>
+      <c r="T103" s="6"/>
+      <c r="U103" s="7"/>
+      <c r="V103" s="7"/>
+      <c r="W103" s="7"/>
+      <c r="X103" s="8"/>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7"/>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -4240,9 +4479,13 @@
       <c r="N104" s="6"/>
       <c r="O104" s="7"/>
       <c r="P104" s="8"/>
-      <c r="Y104" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T104" s="6"/>
+      <c r="U104" s="7"/>
+      <c r="V104" s="7"/>
+      <c r="W104" s="7"/>
+      <c r="X104" s="8"/>
+      <c r="Y104" s="38"/>
+      <c r="Z104" s="7"/>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -4263,9 +4506,13 @@
       <c r="N105" s="6"/>
       <c r="O105" s="7"/>
       <c r="P105" s="8"/>
-      <c r="Y105" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T105" s="6"/>
+      <c r="U105" s="7"/>
+      <c r="V105" s="7"/>
+      <c r="W105" s="7"/>
+      <c r="X105" s="8"/>
+      <c r="Y105" s="38"/>
+      <c r="Z105" s="7"/>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -4286,9 +4533,13 @@
       <c r="N106" s="6"/>
       <c r="O106" s="7"/>
       <c r="P106" s="8"/>
-      <c r="Y106" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T106" s="6"/>
+      <c r="U106" s="7"/>
+      <c r="V106" s="7"/>
+      <c r="W106" s="7"/>
+      <c r="X106" s="8"/>
+      <c r="Y106" s="38"/>
+      <c r="Z106" s="7"/>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -4309,15 +4560,13 @@
       <c r="N107" s="6"/>
       <c r="O107" s="7"/>
       <c r="P107" s="8"/>
-      <c r="X107" s="30">
-        <v>10</v>
-      </c>
-      <c r="Y107" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z107" s="32">
-        <v>4</v>
-      </c>
+      <c r="T107" s="6"/>
+      <c r="U107" s="7"/>
+      <c r="V107" s="7"/>
+      <c r="W107" s="7"/>
+      <c r="X107" s="8"/>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7"/>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108">
@@ -4338,9 +4587,13 @@
       <c r="N108" s="6"/>
       <c r="O108" s="7"/>
       <c r="P108" s="8"/>
-      <c r="Y108" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T108" s="6"/>
+      <c r="U108" s="7"/>
+      <c r="V108" s="7"/>
+      <c r="W108" s="7"/>
+      <c r="X108" s="8"/>
+      <c r="Y108" s="38"/>
+      <c r="Z108" s="7"/>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109">
@@ -4361,9 +4614,13 @@
       <c r="N109" s="6"/>
       <c r="O109" s="7"/>
       <c r="P109" s="8"/>
-      <c r="Y109" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T109" s="6"/>
+      <c r="U109" s="7"/>
+      <c r="V109" s="7"/>
+      <c r="W109" s="7"/>
+      <c r="X109" s="8"/>
+      <c r="Y109" s="38"/>
+      <c r="Z109" s="7"/>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110">
@@ -4384,9 +4641,13 @@
       <c r="N110" s="6"/>
       <c r="O110" s="7"/>
       <c r="P110" s="8"/>
-      <c r="Y110" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T110" s="6"/>
+      <c r="U110" s="7"/>
+      <c r="V110" s="7"/>
+      <c r="W110" s="7"/>
+      <c r="X110" s="8"/>
+      <c r="Y110" s="38"/>
+      <c r="Z110" s="7"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -4407,9 +4668,13 @@
       <c r="N111" s="6"/>
       <c r="O111" s="7"/>
       <c r="P111" s="8"/>
-      <c r="Y111" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T111" s="6"/>
+      <c r="U111" s="7"/>
+      <c r="V111" s="7"/>
+      <c r="W111" s="7"/>
+      <c r="X111" s="8"/>
+      <c r="Y111" s="38"/>
+      <c r="Z111" s="7"/>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -4430,15 +4695,13 @@
       <c r="N112" s="6"/>
       <c r="O112" s="7"/>
       <c r="P112" s="8"/>
-      <c r="X112" s="30">
-        <v>9</v>
-      </c>
-      <c r="Y112" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z112" s="32">
-        <v>5</v>
-      </c>
+      <c r="T112" s="6"/>
+      <c r="U112" s="7"/>
+      <c r="V112" s="7"/>
+      <c r="W112" s="7"/>
+      <c r="X112" s="8"/>
+      <c r="Y112" s="7"/>
+      <c r="Z112" s="7"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A113">
@@ -4459,9 +4722,13 @@
       <c r="N113" s="6"/>
       <c r="O113" s="7"/>
       <c r="P113" s="8"/>
-      <c r="Y113" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T113" s="6"/>
+      <c r="U113" s="7"/>
+      <c r="V113" s="7"/>
+      <c r="W113" s="7"/>
+      <c r="X113" s="8"/>
+      <c r="Y113" s="38"/>
+      <c r="Z113" s="7"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A114">
@@ -4482,9 +4749,13 @@
       <c r="N114" s="6"/>
       <c r="O114" s="7"/>
       <c r="P114" s="8"/>
-      <c r="Y114" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T114" s="6"/>
+      <c r="U114" s="7"/>
+      <c r="V114" s="7"/>
+      <c r="W114" s="7"/>
+      <c r="X114" s="8"/>
+      <c r="Y114" s="38"/>
+      <c r="Z114" s="7"/>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A115">
@@ -4505,9 +4776,13 @@
       <c r="N115" s="6"/>
       <c r="O115" s="7"/>
       <c r="P115" s="8"/>
-      <c r="Y115" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T115" s="6"/>
+      <c r="U115" s="7"/>
+      <c r="V115" s="7"/>
+      <c r="W115" s="7"/>
+      <c r="X115" s="8"/>
+      <c r="Y115" s="38"/>
+      <c r="Z115" s="7"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A116">
@@ -4528,9 +4803,13 @@
       <c r="N116" s="6"/>
       <c r="O116" s="7"/>
       <c r="P116" s="8"/>
-      <c r="Y116" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T116" s="6"/>
+      <c r="U116" s="7"/>
+      <c r="V116" s="7"/>
+      <c r="W116" s="7"/>
+      <c r="X116" s="8"/>
+      <c r="Y116" s="38"/>
+      <c r="Z116" s="7"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A117">
@@ -4551,9 +4830,13 @@
       <c r="N117" s="6"/>
       <c r="O117" s="7"/>
       <c r="P117" s="8"/>
-      <c r="Y117" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T117" s="6"/>
+      <c r="U117" s="7"/>
+      <c r="V117" s="7"/>
+      <c r="W117" s="7"/>
+      <c r="X117" s="8"/>
+      <c r="Y117" s="38"/>
+      <c r="Z117" s="7"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A118">
@@ -4574,15 +4857,13 @@
       <c r="N118" s="6"/>
       <c r="O118" s="7"/>
       <c r="P118" s="8"/>
-      <c r="X118" s="30">
-        <v>8</v>
-      </c>
-      <c r="Y118" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z118" s="32">
-        <v>6</v>
-      </c>
+      <c r="T118" s="6"/>
+      <c r="U118" s="7"/>
+      <c r="V118" s="7"/>
+      <c r="W118" s="7"/>
+      <c r="X118" s="8"/>
+      <c r="Y118" s="7"/>
+      <c r="Z118" s="7"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -4603,9 +4884,13 @@
       <c r="N119" s="6"/>
       <c r="O119" s="7"/>
       <c r="P119" s="8"/>
-      <c r="Y119" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T119" s="6"/>
+      <c r="U119" s="7"/>
+      <c r="V119" s="7"/>
+      <c r="W119" s="7"/>
+      <c r="X119" s="8"/>
+      <c r="Y119" s="38"/>
+      <c r="Z119" s="7"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -4626,9 +4911,13 @@
       <c r="N120" s="6"/>
       <c r="O120" s="7"/>
       <c r="P120" s="8"/>
-      <c r="Y120" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T120" s="6"/>
+      <c r="U120" s="7"/>
+      <c r="V120" s="7"/>
+      <c r="W120" s="7"/>
+      <c r="X120" s="8"/>
+      <c r="Y120" s="38"/>
+      <c r="Z120" s="7"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -4649,9 +4938,13 @@
       <c r="N121" s="6"/>
       <c r="O121" s="7"/>
       <c r="P121" s="8"/>
-      <c r="Y121" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T121" s="6"/>
+      <c r="U121" s="7"/>
+      <c r="V121" s="7"/>
+      <c r="W121" s="7"/>
+      <c r="X121" s="8"/>
+      <c r="Y121" s="38"/>
+      <c r="Z121" s="7"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -4672,9 +4965,13 @@
       <c r="N122" s="6"/>
       <c r="O122" s="7"/>
       <c r="P122" s="8"/>
-      <c r="Y122" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T122" s="6"/>
+      <c r="U122" s="7"/>
+      <c r="V122" s="7"/>
+      <c r="W122" s="7"/>
+      <c r="X122" s="8"/>
+      <c r="Y122" s="38"/>
+      <c r="Z122" s="7"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A123">
@@ -4695,9 +4992,13 @@
       <c r="N123" s="6"/>
       <c r="O123" s="7"/>
       <c r="P123" s="8"/>
-      <c r="Y123" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T123" s="6"/>
+      <c r="U123" s="7"/>
+      <c r="V123" s="7"/>
+      <c r="W123" s="7"/>
+      <c r="X123" s="8"/>
+      <c r="Y123" s="38"/>
+      <c r="Z123" s="7"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A124">
@@ -4718,9 +5019,13 @@
       <c r="N124" s="6"/>
       <c r="O124" s="7"/>
       <c r="P124" s="8"/>
-      <c r="Y124" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T124" s="6"/>
+      <c r="U124" s="7"/>
+      <c r="V124" s="7"/>
+      <c r="W124" s="7"/>
+      <c r="X124" s="8"/>
+      <c r="Y124" s="38"/>
+      <c r="Z124" s="7"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A125">
@@ -4741,15 +5046,13 @@
       <c r="N125" s="6"/>
       <c r="O125" s="7"/>
       <c r="P125" s="8"/>
-      <c r="X125" s="30">
-        <v>7</v>
-      </c>
-      <c r="Y125" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z125" s="32">
-        <v>7</v>
-      </c>
+      <c r="T125" s="6"/>
+      <c r="U125" s="7"/>
+      <c r="V125" s="7"/>
+      <c r="W125" s="7"/>
+      <c r="X125" s="8"/>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -4770,9 +5073,13 @@
       <c r="N126" s="6"/>
       <c r="O126" s="7"/>
       <c r="P126" s="8"/>
-      <c r="Y126" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T126" s="6"/>
+      <c r="U126" s="7"/>
+      <c r="V126" s="7"/>
+      <c r="W126" s="7"/>
+      <c r="X126" s="8"/>
+      <c r="Y126" s="38"/>
+      <c r="Z126" s="7"/>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A127">
@@ -4793,9 +5100,13 @@
       <c r="N127" s="6"/>
       <c r="O127" s="7"/>
       <c r="P127" s="8"/>
-      <c r="Y127" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T127" s="6"/>
+      <c r="U127" s="7"/>
+      <c r="V127" s="7"/>
+      <c r="W127" s="7"/>
+      <c r="X127" s="8"/>
+      <c r="Y127" s="38"/>
+      <c r="Z127" s="7"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -4816,9 +5127,13 @@
       <c r="N128" s="6"/>
       <c r="O128" s="7"/>
       <c r="P128" s="8"/>
-      <c r="Y128" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T128" s="6"/>
+      <c r="U128" s="7"/>
+      <c r="V128" s="7"/>
+      <c r="W128" s="7"/>
+      <c r="X128" s="8"/>
+      <c r="Y128" s="38"/>
+      <c r="Z128" s="7"/>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A129">
@@ -4839,9 +5154,13 @@
       <c r="N129" s="6"/>
       <c r="O129" s="7"/>
       <c r="P129" s="8"/>
-      <c r="Y129" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T129" s="6"/>
+      <c r="U129" s="7"/>
+      <c r="V129" s="7"/>
+      <c r="W129" s="7"/>
+      <c r="X129" s="8"/>
+      <c r="Y129" s="38"/>
+      <c r="Z129" s="7"/>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -4862,9 +5181,13 @@
       <c r="N130" s="6"/>
       <c r="O130" s="7"/>
       <c r="P130" s="8"/>
-      <c r="Y130" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T130" s="6"/>
+      <c r="U130" s="7"/>
+      <c r="V130" s="7"/>
+      <c r="W130" s="7"/>
+      <c r="X130" s="8"/>
+      <c r="Y130" s="38"/>
+      <c r="Z130" s="7"/>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A131">
@@ -4885,9 +5208,13 @@
       <c r="N131" s="6"/>
       <c r="O131" s="7"/>
       <c r="P131" s="8"/>
-      <c r="Y131" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T131" s="6"/>
+      <c r="U131" s="7"/>
+      <c r="V131" s="7"/>
+      <c r="W131" s="7"/>
+      <c r="X131" s="8"/>
+      <c r="Y131" s="38"/>
+      <c r="Z131" s="7"/>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A132">
@@ -4908,9 +5235,13 @@
       <c r="N132" s="6"/>
       <c r="O132" s="7"/>
       <c r="P132" s="8"/>
-      <c r="Y132" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T132" s="6"/>
+      <c r="U132" s="7"/>
+      <c r="V132" s="7"/>
+      <c r="W132" s="7"/>
+      <c r="X132" s="8"/>
+      <c r="Y132" s="38"/>
+      <c r="Z132" s="7"/>
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A133">
@@ -4931,15 +5262,13 @@
       <c r="N133" s="6"/>
       <c r="O133" s="7"/>
       <c r="P133" s="8"/>
-      <c r="X133" s="30">
-        <v>6</v>
-      </c>
-      <c r="Y133" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z133" s="32">
-        <v>8</v>
-      </c>
+      <c r="T133" s="6"/>
+      <c r="U133" s="7"/>
+      <c r="V133" s="7"/>
+      <c r="W133" s="7"/>
+      <c r="X133" s="8"/>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7"/>
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A134">
@@ -4960,9 +5289,13 @@
       <c r="N134" s="6"/>
       <c r="O134" s="7"/>
       <c r="P134" s="8"/>
-      <c r="Y134" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T134" s="6"/>
+      <c r="U134" s="7"/>
+      <c r="V134" s="7"/>
+      <c r="W134" s="7"/>
+      <c r="X134" s="8"/>
+      <c r="Y134" s="38"/>
+      <c r="Z134" s="7"/>
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -4983,9 +5316,13 @@
       <c r="N135" s="6"/>
       <c r="O135" s="7"/>
       <c r="P135" s="8"/>
-      <c r="Y135" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T135" s="6"/>
+      <c r="U135" s="7"/>
+      <c r="V135" s="7"/>
+      <c r="W135" s="7"/>
+      <c r="X135" s="8"/>
+      <c r="Y135" s="38"/>
+      <c r="Z135" s="7"/>
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A136">
@@ -5006,9 +5343,13 @@
       <c r="N136" s="6"/>
       <c r="O136" s="7"/>
       <c r="P136" s="8"/>
-      <c r="Y136" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T136" s="6"/>
+      <c r="U136" s="7"/>
+      <c r="V136" s="7"/>
+      <c r="W136" s="7"/>
+      <c r="X136" s="8"/>
+      <c r="Y136" s="38"/>
+      <c r="Z136" s="7"/>
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A137">
@@ -5029,9 +5370,13 @@
       <c r="N137" s="6"/>
       <c r="O137" s="7"/>
       <c r="P137" s="8"/>
-      <c r="Y137" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T137" s="6"/>
+      <c r="U137" s="7"/>
+      <c r="V137" s="7"/>
+      <c r="W137" s="7"/>
+      <c r="X137" s="8"/>
+      <c r="Y137" s="38"/>
+      <c r="Z137" s="7"/>
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A138">
@@ -5052,9 +5397,13 @@
       <c r="N138" s="6"/>
       <c r="O138" s="7"/>
       <c r="P138" s="8"/>
-      <c r="Y138" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T138" s="6"/>
+      <c r="U138" s="7"/>
+      <c r="V138" s="7"/>
+      <c r="W138" s="7"/>
+      <c r="X138" s="8"/>
+      <c r="Y138" s="38"/>
+      <c r="Z138" s="7"/>
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A139">
@@ -5075,9 +5424,13 @@
       <c r="N139" s="6"/>
       <c r="O139" s="7"/>
       <c r="P139" s="8"/>
-      <c r="Y139" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T139" s="6"/>
+      <c r="U139" s="7"/>
+      <c r="V139" s="7"/>
+      <c r="W139" s="7"/>
+      <c r="X139" s="8"/>
+      <c r="Y139" s="38"/>
+      <c r="Z139" s="7"/>
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A140">
@@ -5098,9 +5451,13 @@
       <c r="N140" s="6"/>
       <c r="O140" s="7"/>
       <c r="P140" s="8"/>
-      <c r="Y140" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T140" s="6"/>
+      <c r="U140" s="7"/>
+      <c r="V140" s="7"/>
+      <c r="W140" s="7"/>
+      <c r="X140" s="8"/>
+      <c r="Y140" s="38"/>
+      <c r="Z140" s="7"/>
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A141">
@@ -5121,9 +5478,13 @@
       <c r="N141" s="6"/>
       <c r="O141" s="7"/>
       <c r="P141" s="8"/>
-      <c r="Y141" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T141" s="6"/>
+      <c r="U141" s="7"/>
+      <c r="V141" s="7"/>
+      <c r="W141" s="7"/>
+      <c r="X141" s="8"/>
+      <c r="Y141" s="38"/>
+      <c r="Z141" s="7"/>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A142">
@@ -5144,15 +5505,13 @@
       <c r="N142" s="6"/>
       <c r="O142" s="7"/>
       <c r="P142" s="8"/>
-      <c r="X142" s="30">
-        <v>5</v>
-      </c>
-      <c r="Y142" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z142" s="32">
-        <v>9</v>
-      </c>
+      <c r="T142" s="6"/>
+      <c r="U142" s="7"/>
+      <c r="V142" s="7"/>
+      <c r="W142" s="7"/>
+      <c r="X142" s="8"/>
+      <c r="Y142" s="7"/>
+      <c r="Z142" s="7"/>
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A143">
@@ -5173,9 +5532,13 @@
       <c r="N143" s="6"/>
       <c r="O143" s="7"/>
       <c r="P143" s="8"/>
-      <c r="Y143" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T143" s="6"/>
+      <c r="U143" s="7"/>
+      <c r="V143" s="7"/>
+      <c r="W143" s="7"/>
+      <c r="X143" s="8"/>
+      <c r="Y143" s="38"/>
+      <c r="Z143" s="7"/>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A144">
@@ -5196,9 +5559,13 @@
       <c r="N144" s="6"/>
       <c r="O144" s="7"/>
       <c r="P144" s="8"/>
-      <c r="Y144" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T144" s="6"/>
+      <c r="U144" s="7"/>
+      <c r="V144" s="7"/>
+      <c r="W144" s="7"/>
+      <c r="X144" s="8"/>
+      <c r="Y144" s="38"/>
+      <c r="Z144" s="7"/>
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A145">
@@ -5219,9 +5586,13 @@
       <c r="N145" s="6"/>
       <c r="O145" s="7"/>
       <c r="P145" s="8"/>
-      <c r="Y145" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T145" s="6"/>
+      <c r="U145" s="7"/>
+      <c r="V145" s="7"/>
+      <c r="W145" s="7"/>
+      <c r="X145" s="8"/>
+      <c r="Y145" s="38"/>
+      <c r="Z145" s="7"/>
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A146">
@@ -5242,9 +5613,13 @@
       <c r="N146" s="6"/>
       <c r="O146" s="7"/>
       <c r="P146" s="8"/>
-      <c r="Y146" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T146" s="6"/>
+      <c r="U146" s="7"/>
+      <c r="V146" s="7"/>
+      <c r="W146" s="7"/>
+      <c r="X146" s="8"/>
+      <c r="Y146" s="38"/>
+      <c r="Z146" s="7"/>
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A147">
@@ -5265,9 +5640,13 @@
       <c r="N147" s="6"/>
       <c r="O147" s="7"/>
       <c r="P147" s="8"/>
-      <c r="Y147" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T147" s="6"/>
+      <c r="U147" s="7"/>
+      <c r="V147" s="7"/>
+      <c r="W147" s="7"/>
+      <c r="X147" s="8"/>
+      <c r="Y147" s="38"/>
+      <c r="Z147" s="7"/>
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A148">
@@ -5288,9 +5667,13 @@
       <c r="N148" s="6"/>
       <c r="O148" s="7"/>
       <c r="P148" s="8"/>
-      <c r="Y148" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T148" s="6"/>
+      <c r="U148" s="7"/>
+      <c r="V148" s="7"/>
+      <c r="W148" s="7"/>
+      <c r="X148" s="8"/>
+      <c r="Y148" s="38"/>
+      <c r="Z148" s="7"/>
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A149">
@@ -5311,9 +5694,13 @@
       <c r="N149" s="6"/>
       <c r="O149" s="7"/>
       <c r="P149" s="8"/>
-      <c r="Y149" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T149" s="6"/>
+      <c r="U149" s="7"/>
+      <c r="V149" s="7"/>
+      <c r="W149" s="7"/>
+      <c r="X149" s="8"/>
+      <c r="Y149" s="38"/>
+      <c r="Z149" s="7"/>
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A150">
@@ -5334,9 +5721,13 @@
       <c r="N150" s="6"/>
       <c r="O150" s="7"/>
       <c r="P150" s="8"/>
-      <c r="Y150" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T150" s="6"/>
+      <c r="U150" s="7"/>
+      <c r="V150" s="7"/>
+      <c r="W150" s="7"/>
+      <c r="X150" s="8"/>
+      <c r="Y150" s="38"/>
+      <c r="Z150" s="7"/>
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A151">
@@ -5357,9 +5748,13 @@
       <c r="N151" s="6"/>
       <c r="O151" s="7"/>
       <c r="P151" s="8"/>
-      <c r="Y151" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T151" s="6"/>
+      <c r="U151" s="7"/>
+      <c r="V151" s="7"/>
+      <c r="W151" s="7"/>
+      <c r="X151" s="8"/>
+      <c r="Y151" s="38"/>
+      <c r="Z151" s="7"/>
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A152">
@@ -5380,15 +5775,13 @@
       <c r="N152" s="6"/>
       <c r="O152" s="7"/>
       <c r="P152" s="8"/>
-      <c r="X152" s="30">
-        <v>4</v>
-      </c>
-      <c r="Y152" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z152" s="32">
-        <v>10</v>
-      </c>
+      <c r="T152" s="6"/>
+      <c r="U152" s="7"/>
+      <c r="V152" s="7"/>
+      <c r="W152" s="7"/>
+      <c r="X152" s="8"/>
+      <c r="Y152" s="7"/>
+      <c r="Z152" s="7"/>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A153">
@@ -5409,9 +5802,13 @@
       <c r="N153" s="6"/>
       <c r="O153" s="7"/>
       <c r="P153" s="8"/>
-      <c r="Y153" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T153" s="6"/>
+      <c r="U153" s="7"/>
+      <c r="V153" s="7"/>
+      <c r="W153" s="7"/>
+      <c r="X153" s="8"/>
+      <c r="Y153" s="38"/>
+      <c r="Z153" s="7"/>
     </row>
     <row r="154" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A154">
@@ -5432,9 +5829,13 @@
       <c r="N154" s="6"/>
       <c r="O154" s="7"/>
       <c r="P154" s="8"/>
-      <c r="Y154" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T154" s="6"/>
+      <c r="U154" s="7"/>
+      <c r="V154" s="7"/>
+      <c r="W154" s="7"/>
+      <c r="X154" s="8"/>
+      <c r="Y154" s="38"/>
+      <c r="Z154" s="7"/>
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A155">
@@ -5455,9 +5856,13 @@
       <c r="N155" s="6"/>
       <c r="O155" s="7"/>
       <c r="P155" s="8"/>
-      <c r="Y155" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T155" s="6"/>
+      <c r="U155" s="7"/>
+      <c r="V155" s="7"/>
+      <c r="W155" s="7"/>
+      <c r="X155" s="8"/>
+      <c r="Y155" s="38"/>
+      <c r="Z155" s="7"/>
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A156">
@@ -5478,9 +5883,13 @@
       <c r="N156" s="6"/>
       <c r="O156" s="7"/>
       <c r="P156" s="8"/>
-      <c r="Y156" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T156" s="6"/>
+      <c r="U156" s="7"/>
+      <c r="V156" s="7"/>
+      <c r="W156" s="7"/>
+      <c r="X156" s="8"/>
+      <c r="Y156" s="38"/>
+      <c r="Z156" s="7"/>
     </row>
     <row r="157" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A157">
@@ -5501,9 +5910,13 @@
       <c r="N157" s="6"/>
       <c r="O157" s="7"/>
       <c r="P157" s="8"/>
-      <c r="Y157" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T157" s="6"/>
+      <c r="U157" s="7"/>
+      <c r="V157" s="7"/>
+      <c r="W157" s="7"/>
+      <c r="X157" s="8"/>
+      <c r="Y157" s="38"/>
+      <c r="Z157" s="7"/>
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A158">
@@ -5524,9 +5937,13 @@
       <c r="N158" s="6"/>
       <c r="O158" s="7"/>
       <c r="P158" s="8"/>
-      <c r="Y158" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T158" s="6"/>
+      <c r="U158" s="7"/>
+      <c r="V158" s="7"/>
+      <c r="W158" s="7"/>
+      <c r="X158" s="8"/>
+      <c r="Y158" s="38"/>
+      <c r="Z158" s="7"/>
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A159">
@@ -5547,9 +5964,13 @@
       <c r="N159" s="6"/>
       <c r="O159" s="7"/>
       <c r="P159" s="8"/>
-      <c r="Y159" s="28" t="s">
-        <v>12</v>
-      </c>
+      <c r="T159" s="6"/>
+      <c r="U159" s="7"/>
+      <c r="V159" s="7"/>
+      <c r="W159" s="7"/>
+      <c r="X159" s="8"/>
+      <c r="Y159" s="38"/>
+      <c r="Z159" s="7"/>
     </row>
     <row r="160" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A160">
@@ -5570,11 +5991,15 @@
       <c r="N160" s="6"/>
       <c r="O160" s="7"/>
       <c r="P160" s="8"/>
-      <c r="Y160" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T160" s="6"/>
+      <c r="U160" s="7"/>
+      <c r="V160" s="7"/>
+      <c r="W160" s="7"/>
+      <c r="X160" s="8"/>
+      <c r="Y160" s="38"/>
+      <c r="Z160" s="7"/>
+    </row>
+    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>41</v>
       </c>
@@ -5593,11 +6018,15 @@
       <c r="N161" s="6"/>
       <c r="O161" s="7"/>
       <c r="P161" s="8"/>
-      <c r="Y161" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T161" s="6"/>
+      <c r="U161" s="7"/>
+      <c r="V161" s="7"/>
+      <c r="W161" s="7"/>
+      <c r="X161" s="8"/>
+      <c r="Y161" s="38"/>
+      <c r="Z161" s="7"/>
+    </row>
+    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>40</v>
       </c>
@@ -5616,11 +6045,15 @@
       <c r="N162" s="6"/>
       <c r="O162" s="7"/>
       <c r="P162" s="8"/>
-      <c r="Y162" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T162" s="6"/>
+      <c r="U162" s="7"/>
+      <c r="V162" s="7"/>
+      <c r="W162" s="7"/>
+      <c r="X162" s="8"/>
+      <c r="Y162" s="38"/>
+      <c r="Z162" s="7"/>
+    </row>
+    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>39</v>
       </c>
@@ -5639,17 +6072,15 @@
       <c r="N163" s="6"/>
       <c r="O163" s="7"/>
       <c r="P163" s="8"/>
-      <c r="X163" s="30">
-        <v>3</v>
-      </c>
-      <c r="Y163" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z163" s="32">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T163" s="6"/>
+      <c r="U163" s="7"/>
+      <c r="V163" s="7"/>
+      <c r="W163" s="7"/>
+      <c r="X163" s="8"/>
+      <c r="Y163" s="7"/>
+      <c r="Z163" s="7"/>
+    </row>
+    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>38</v>
       </c>
@@ -5668,11 +6099,15 @@
       <c r="N164" s="6"/>
       <c r="O164" s="7"/>
       <c r="P164" s="8"/>
-      <c r="Y164" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T164" s="6"/>
+      <c r="U164" s="7"/>
+      <c r="V164" s="7"/>
+      <c r="W164" s="7"/>
+      <c r="X164" s="8"/>
+      <c r="Y164" s="38"/>
+      <c r="Z164" s="7"/>
+    </row>
+    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>37</v>
       </c>
@@ -5691,11 +6126,15 @@
       <c r="N165" s="6"/>
       <c r="O165" s="7"/>
       <c r="P165" s="8"/>
-      <c r="Y165" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T165" s="6"/>
+      <c r="U165" s="7"/>
+      <c r="V165" s="7"/>
+      <c r="W165" s="7"/>
+      <c r="X165" s="8"/>
+      <c r="Y165" s="38"/>
+      <c r="Z165" s="7"/>
+    </row>
+    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>36</v>
       </c>
@@ -5714,11 +6153,14 @@
       <c r="N166" s="6"/>
       <c r="O166" s="7"/>
       <c r="P166" s="8"/>
-      <c r="Y166" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T166" s="6"/>
+      <c r="U166" s="7"/>
+      <c r="V166" s="7"/>
+      <c r="W166" s="7"/>
+      <c r="X166" s="8"/>
+      <c r="AC166" s="9"/>
+    </row>
+    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>35</v>
       </c>
@@ -5737,11 +6179,14 @@
       <c r="N167" s="6"/>
       <c r="O167" s="7"/>
       <c r="P167" s="8"/>
-      <c r="Y167" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T167" s="6"/>
+      <c r="U167" s="7"/>
+      <c r="V167" s="7"/>
+      <c r="W167" s="7"/>
+      <c r="X167" s="8"/>
+      <c r="AC167" s="9"/>
+    </row>
+    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>34</v>
       </c>
@@ -5760,11 +6205,14 @@
       <c r="N168" s="6"/>
       <c r="O168" s="7"/>
       <c r="P168" s="8"/>
-      <c r="Y168" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T168" s="6"/>
+      <c r="U168" s="7"/>
+      <c r="V168" s="7"/>
+      <c r="W168" s="7"/>
+      <c r="X168" s="8"/>
+      <c r="AC168" s="9"/>
+    </row>
+    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>33</v>
       </c>
@@ -5783,11 +6231,14 @@
       <c r="N169" s="6"/>
       <c r="O169" s="7"/>
       <c r="P169" s="8"/>
-      <c r="Y169" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T169" s="6"/>
+      <c r="U169" s="7"/>
+      <c r="V169" s="7"/>
+      <c r="W169" s="7"/>
+      <c r="X169" s="8"/>
+      <c r="AC169" s="9"/>
+    </row>
+    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>32</v>
       </c>
@@ -5806,11 +6257,14 @@
       <c r="N170" s="6"/>
       <c r="O170" s="7"/>
       <c r="P170" s="8"/>
-      <c r="Y170" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T170" s="6"/>
+      <c r="U170" s="7"/>
+      <c r="V170" s="7"/>
+      <c r="W170" s="7"/>
+      <c r="X170" s="8"/>
+      <c r="AC170" s="9"/>
+    </row>
+    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>31</v>
       </c>
@@ -5829,11 +6283,14 @@
       <c r="N171" s="6"/>
       <c r="O171" s="7"/>
       <c r="P171" s="8"/>
-      <c r="Y171" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T171" s="6"/>
+      <c r="U171" s="7"/>
+      <c r="V171" s="7"/>
+      <c r="W171" s="7"/>
+      <c r="X171" s="8"/>
+      <c r="AC171" s="9"/>
+    </row>
+    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>30</v>
       </c>
@@ -5852,20 +6309,22 @@
       <c r="N172" s="6"/>
       <c r="O172" s="7"/>
       <c r="P172" s="8"/>
-      <c r="U172" s="44">
+      <c r="T172" s="6">
+        <v>1</v>
+      </c>
+      <c r="U172" s="34">
         <v>5</v>
       </c>
-      <c r="V172" s="45">
+      <c r="V172" s="35">
         <v>3</v>
       </c>
-      <c r="W172" s="46">
+      <c r="W172" s="35">
         <v>0</v>
       </c>
-      <c r="Y172" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X172" s="8"/>
+      <c r="AC172" s="9"/>
+    </row>
+    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>29</v>
       </c>
@@ -5884,20 +6343,22 @@
       <c r="N173" s="6"/>
       <c r="O173" s="7"/>
       <c r="P173" s="8"/>
-      <c r="U173" s="43">
+      <c r="T173" s="6">
+        <v>1</v>
+      </c>
+      <c r="U173" s="33">
         <v>4</v>
       </c>
-      <c r="V173" s="41">
+      <c r="V173" s="32">
         <v>3</v>
       </c>
-      <c r="W173" s="42">
+      <c r="W173" s="32">
         <v>1</v>
       </c>
-      <c r="Y173" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X173" s="8"/>
+      <c r="AC173" s="9"/>
+    </row>
+    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>28</v>
       </c>
@@ -5916,14 +6377,16 @@
       <c r="N174" s="6"/>
       <c r="O174" s="7"/>
       <c r="P174" s="8"/>
-      <c r="V174" s="28" t="s">
+      <c r="T174" s="6"/>
+      <c r="U174" s="7"/>
+      <c r="V174" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y174" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W174" s="7"/>
+      <c r="X174" s="8"/>
+      <c r="AC174" s="9"/>
+    </row>
+    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>27</v>
       </c>
@@ -5942,26 +6405,22 @@
       <c r="N175" s="6"/>
       <c r="O175" s="7"/>
       <c r="P175" s="8"/>
-      <c r="U175" s="43">
+      <c r="T175" s="6">
+        <v>1</v>
+      </c>
+      <c r="U175" s="33">
         <v>3</v>
       </c>
-      <c r="V175" s="41">
+      <c r="V175" s="32">
         <v>3</v>
       </c>
-      <c r="W175" s="42">
+      <c r="W175" s="32">
         <v>2</v>
       </c>
-      <c r="X175" s="35">
-        <v>2</v>
-      </c>
-      <c r="Y175" s="36">
-        <v>1</v>
-      </c>
-      <c r="Z175" s="37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X175" s="40"/>
+      <c r="AC175" s="9"/>
+    </row>
+    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>26</v>
       </c>
@@ -5980,20 +6439,24 @@
       <c r="N176" s="6"/>
       <c r="O176" s="7"/>
       <c r="P176" s="8"/>
-      <c r="U176">
+      <c r="T176" s="6">
+        <v>2</v>
+      </c>
+      <c r="U176" s="7">
         <v>5</v>
       </c>
-      <c r="V176">
+      <c r="V176" s="7">
         <v>2</v>
       </c>
-      <c r="W176">
+      <c r="W176" s="7">
         <v>0</v>
       </c>
-      <c r="Y176" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X176" s="21">
+        <v>3</v>
+      </c>
+      <c r="AC176" s="9"/>
+    </row>
+    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>25</v>
       </c>
@@ -6012,20 +6475,24 @@
       <c r="N177" s="6"/>
       <c r="O177" s="7"/>
       <c r="P177" s="8"/>
-      <c r="U177" s="26">
+      <c r="T177" s="6">
+        <v>2</v>
+      </c>
+      <c r="U177" s="39">
         <v>4</v>
       </c>
-      <c r="V177">
+      <c r="V177" s="7">
         <v>2</v>
       </c>
-      <c r="W177">
+      <c r="W177" s="7">
         <v>1</v>
       </c>
-      <c r="Y177" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X177" s="21">
+        <v>3</v>
+      </c>
+      <c r="AC177" s="9"/>
+    </row>
+    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>24</v>
       </c>
@@ -6044,14 +6511,16 @@
       <c r="N178" s="6"/>
       <c r="O178" s="7"/>
       <c r="P178" s="8"/>
-      <c r="V178" s="28" t="s">
+      <c r="T178" s="6"/>
+      <c r="U178" s="7"/>
+      <c r="V178" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y178" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W178" s="7"/>
+      <c r="X178" s="8"/>
+      <c r="AC178" s="9"/>
+    </row>
+    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>23</v>
       </c>
@@ -6070,21 +6539,24 @@
       <c r="N179" s="6"/>
       <c r="O179" s="7"/>
       <c r="P179" s="8"/>
-      <c r="U179" s="48">
+      <c r="T179" s="6">
+        <v>1</v>
+      </c>
+      <c r="U179" s="37">
         <v>2</v>
       </c>
-      <c r="V179" s="41">
+      <c r="V179" s="32">
         <v>3</v>
       </c>
-      <c r="W179" s="42">
+      <c r="W179" s="32">
         <v>3</v>
       </c>
-      <c r="X179" s="29"/>
-      <c r="Y179" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X179" s="41">
+        <v>1</v>
+      </c>
+      <c r="AC179" s="9"/>
+    </row>
+    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>22</v>
       </c>
@@ -6103,20 +6575,24 @@
       <c r="N180" s="6"/>
       <c r="O180" s="7"/>
       <c r="P180" s="8"/>
-      <c r="U180">
+      <c r="T180" s="6">
+        <v>2</v>
+      </c>
+      <c r="U180" s="7">
         <v>5</v>
       </c>
-      <c r="V180">
+      <c r="V180" s="7">
         <v>2</v>
       </c>
-      <c r="W180">
+      <c r="W180" s="7">
         <v>0</v>
       </c>
-      <c r="Y180" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X180" s="21">
+        <v>3</v>
+      </c>
+      <c r="AC180" s="9"/>
+    </row>
+    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>21</v>
       </c>
@@ -6135,20 +6611,36 @@
       <c r="N181" s="6"/>
       <c r="O181" s="7"/>
       <c r="P181" s="8"/>
-      <c r="U181">
+      <c r="T181" s="6">
+        <v>2</v>
+      </c>
+      <c r="U181" s="7">
         <v>4</v>
       </c>
-      <c r="V181">
+      <c r="V181" s="7">
         <v>2</v>
       </c>
-      <c r="W181">
+      <c r="W181" s="7">
         <v>1</v>
       </c>
-      <c r="Y181" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X181" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y181" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z181" s="7">
+        <v>30</v>
+      </c>
+      <c r="AA181" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB181" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC181" s="9"/>
+    </row>
+    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>20</v>
       </c>
@@ -6167,14 +6659,28 @@
       <c r="N182" s="6"/>
       <c r="O182" s="7"/>
       <c r="P182" s="8"/>
-      <c r="V182" s="28" t="s">
+      <c r="T182" s="6"/>
+      <c r="U182" s="7"/>
+      <c r="V182" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y182" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W182" s="7"/>
+      <c r="X182" s="8"/>
+      <c r="Y182" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z182" s="7">
+        <v>29</v>
+      </c>
+      <c r="AA182" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB182" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC182" s="9"/>
+    </row>
+    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>19</v>
       </c>
@@ -6193,20 +6699,36 @@
       <c r="N183" s="6"/>
       <c r="O183" s="7"/>
       <c r="P183" s="8"/>
-      <c r="U183" s="30">
+      <c r="T183" s="6">
+        <v>2</v>
+      </c>
+      <c r="U183" s="27">
         <v>3</v>
       </c>
-      <c r="V183" s="31">
+      <c r="V183" s="28">
         <v>2</v>
       </c>
-      <c r="W183" s="32">
+      <c r="W183" s="28">
         <v>2</v>
       </c>
-      <c r="Y183" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X183" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y183" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z183" s="7">
+        <v>27</v>
+      </c>
+      <c r="AA183" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB183" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC183" s="9"/>
+    </row>
+    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>18</v>
       </c>
@@ -6225,20 +6747,36 @@
       <c r="N184" s="6"/>
       <c r="O184" s="7"/>
       <c r="P184" s="8"/>
-      <c r="U184">
+      <c r="T184" s="10">
+        <v>3</v>
+      </c>
+      <c r="U184" s="7">
         <v>5</v>
       </c>
-      <c r="V184">
+      <c r="V184" s="7">
         <v>1</v>
       </c>
-      <c r="W184">
+      <c r="W184" s="7">
         <v>0</v>
       </c>
-      <c r="Y184" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X184" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y184" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z184" s="7">
+        <v>26</v>
+      </c>
+      <c r="AA184" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB184" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC184" s="9"/>
+    </row>
+    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>17</v>
       </c>
@@ -6257,20 +6795,36 @@
       <c r="N185" s="6"/>
       <c r="O185" s="7"/>
       <c r="P185" s="8"/>
-      <c r="U185">
+      <c r="T185" s="10">
+        <v>3</v>
+      </c>
+      <c r="U185" s="7">
         <v>4</v>
       </c>
-      <c r="V185">
+      <c r="V185" s="7">
         <v>1</v>
       </c>
-      <c r="W185">
+      <c r="W185" s="7">
         <v>1</v>
       </c>
-      <c r="Y185" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X185" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y185" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z185" s="7">
+        <v>25</v>
+      </c>
+      <c r="AA185" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB185" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC185" s="9"/>
+    </row>
+    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>16</v>
       </c>
@@ -6289,14 +6843,28 @@
       <c r="N186" s="6"/>
       <c r="O186" s="7"/>
       <c r="P186" s="8"/>
-      <c r="V186" s="28" t="s">
+      <c r="T186" s="6"/>
+      <c r="U186" s="7"/>
+      <c r="V186" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y186" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W186" s="7"/>
+      <c r="X186" s="8"/>
+      <c r="Y186" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z186" s="7">
+        <v>23</v>
+      </c>
+      <c r="AA186" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB186" s="7">
+        <v>4</v>
+      </c>
+      <c r="AC186" s="9"/>
+    </row>
+    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>15</v>
       </c>
@@ -6315,21 +6883,35 @@
       <c r="N187" s="6"/>
       <c r="O187" s="7"/>
       <c r="P187" s="8"/>
-      <c r="U187" s="47">
+      <c r="T187" s="6">
         <v>1</v>
       </c>
-      <c r="V187" s="39">
+      <c r="U187" s="36">
+        <v>1</v>
+      </c>
+      <c r="V187" s="31">
         <v>3</v>
       </c>
-      <c r="W187" s="40">
+      <c r="W187" s="31">
         <v>4</v>
       </c>
-      <c r="X187" s="29"/>
-      <c r="Y187" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X187" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y187" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z187" s="7">
+        <v>22</v>
+      </c>
+      <c r="AA187" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB187" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>14</v>
       </c>
@@ -6357,26 +6939,35 @@
       <c r="Q188" s="14"/>
       <c r="R188" s="14"/>
       <c r="S188" s="14"/>
-      <c r="U188">
+      <c r="T188" s="6">
+        <v>2</v>
+      </c>
+      <c r="U188" s="7">
         <v>5</v>
       </c>
-      <c r="V188">
+      <c r="V188" s="7">
         <v>2</v>
       </c>
-      <c r="W188">
+      <c r="W188" s="7">
         <v>0</v>
       </c>
-      <c r="X188" s="30">
-        <v>1</v>
-      </c>
-      <c r="Y188" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z188" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X188" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y188" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z188" s="7">
+        <v>21</v>
+      </c>
+      <c r="AA188" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB188" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>13</v>
       </c>
@@ -6395,20 +6986,35 @@
       <c r="N189" s="6"/>
       <c r="O189" s="7"/>
       <c r="P189" s="8"/>
-      <c r="U189">
+      <c r="T189" s="6">
+        <v>2</v>
+      </c>
+      <c r="U189" s="7">
         <v>4</v>
       </c>
-      <c r="V189">
+      <c r="V189" s="7">
         <v>2</v>
       </c>
-      <c r="W189">
+      <c r="W189" s="7">
         <v>1</v>
       </c>
-      <c r="Y189" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X189" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y189" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z189" s="7">
+        <v>19</v>
+      </c>
+      <c r="AA189" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB189" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>12</v>
       </c>
@@ -6430,14 +7036,27 @@
       <c r="Q190" s="26"/>
       <c r="R190" s="26"/>
       <c r="S190" s="26"/>
-      <c r="V190" s="28" t="s">
+      <c r="T190" s="6"/>
+      <c r="U190" s="7"/>
+      <c r="V190" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y190" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W190" s="7"/>
+      <c r="X190" s="8"/>
+      <c r="Y190" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z190" s="7">
+        <v>18</v>
+      </c>
+      <c r="AA190" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB190" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>11</v>
       </c>
@@ -6453,20 +7072,35 @@
       <c r="K191" s="6"/>
       <c r="L191" s="7"/>
       <c r="M191" s="8"/>
-      <c r="U191" s="30">
+      <c r="T191" s="6">
+        <v>2</v>
+      </c>
+      <c r="U191" s="27">
         <v>3</v>
       </c>
-      <c r="V191" s="31">
+      <c r="V191" s="28">
         <v>2</v>
       </c>
-      <c r="W191" s="32">
+      <c r="W191" s="28">
         <v>2</v>
       </c>
-      <c r="Y191" s="28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X191" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y191" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z191" s="7">
+        <v>17</v>
+      </c>
+      <c r="AA191" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB191" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>10</v>
       </c>
@@ -6488,17 +7122,32 @@
       <c r="Q192" s="16"/>
       <c r="R192" s="16"/>
       <c r="S192" s="16"/>
-      <c r="U192">
+      <c r="T192" s="10">
+        <v>3</v>
+      </c>
+      <c r="U192" s="7">
         <v>5</v>
       </c>
-      <c r="V192">
+      <c r="V192" s="7">
         <v>1</v>
       </c>
-      <c r="W192">
+      <c r="W192" s="7">
         <v>0</v>
       </c>
-      <c r="Y192" s="28" t="s">
-        <v>12</v>
+      <c r="X192" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y192" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z192" s="7">
+        <v>15</v>
+      </c>
+      <c r="AA192" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB192" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:28" x14ac:dyDescent="0.25">
@@ -6520,18 +7169,32 @@
       <c r="N193" s="10"/>
       <c r="O193" s="11"/>
       <c r="P193" s="8"/>
-      <c r="T193" s="14"/>
-      <c r="U193">
+      <c r="T193" s="10">
+        <v>3</v>
+      </c>
+      <c r="U193" s="7">
         <v>4</v>
       </c>
-      <c r="V193">
+      <c r="V193" s="7">
         <v>1</v>
       </c>
-      <c r="W193">
+      <c r="W193" s="7">
         <v>1</v>
       </c>
-      <c r="Y193" s="28" t="s">
-        <v>12</v>
+      <c r="X193" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y193" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z193" s="7">
+        <v>14</v>
+      </c>
+      <c r="AA193" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB193" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:28" x14ac:dyDescent="0.25">
@@ -6574,12 +7237,24 @@
       <c r="Q194" s="14"/>
       <c r="R194" s="14"/>
       <c r="S194" s="14"/>
-      <c r="T194" s="14"/>
-      <c r="V194" s="28" t="s">
+      <c r="T194" s="10"/>
+      <c r="U194" s="7"/>
+      <c r="V194" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="Y194" s="28" t="s">
-        <v>12</v>
+      <c r="W194" s="7"/>
+      <c r="X194" s="8"/>
+      <c r="Y194" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z194" s="7">
+        <v>13</v>
+      </c>
+      <c r="AA194" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB194" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:28" x14ac:dyDescent="0.25">
@@ -6616,17 +7291,32 @@
       <c r="Q195" s="14"/>
       <c r="R195" s="14"/>
       <c r="S195" s="14"/>
-      <c r="U195" s="38">
+      <c r="T195" s="6">
         <v>2</v>
       </c>
-      <c r="V195" s="33">
+      <c r="U195" s="30">
         <v>2</v>
       </c>
-      <c r="W195" s="34">
+      <c r="V195" s="29">
+        <v>2</v>
+      </c>
+      <c r="W195" s="29">
         <v>3</v>
       </c>
-      <c r="Y195" s="28" t="s">
-        <v>12</v>
+      <c r="X195" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y195" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z195" s="7">
+        <v>11</v>
+      </c>
+      <c r="AA195" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB195" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:28" x14ac:dyDescent="0.25">
@@ -6646,11 +7336,32 @@
       <c r="L196" s="7"/>
       <c r="M196" s="8"/>
       <c r="P196" s="8"/>
-      <c r="V196" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y196" s="28" t="s">
-        <v>12</v>
+      <c r="T196" s="10">
+        <v>3</v>
+      </c>
+      <c r="U196" s="7">
+        <v>5</v>
+      </c>
+      <c r="V196" s="7">
+        <v>1</v>
+      </c>
+      <c r="W196" s="7">
+        <v>0</v>
+      </c>
+      <c r="X196" s="21">
+        <v>3</v>
+      </c>
+      <c r="Y196" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z196" s="7">
+        <v>10</v>
+      </c>
+      <c r="AA196" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB196" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="197" spans="1:28" x14ac:dyDescent="0.25">
@@ -6677,23 +7388,33 @@
       <c r="M197" s="8"/>
       <c r="P197" s="8"/>
       <c r="R197" s="14"/>
-      <c r="T197" s="14"/>
-      <c r="U197">
+      <c r="T197" s="10">
+        <v>3</v>
+      </c>
+      <c r="U197" s="7">
         <v>4</v>
       </c>
-      <c r="V197">
+      <c r="V197" s="7">
         <v>1</v>
       </c>
-      <c r="W197">
+      <c r="W197" s="7">
         <v>1</v>
       </c>
-      <c r="X197" s="14"/>
-      <c r="Y197" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z197" s="16"/>
-      <c r="AA197" s="16"/>
-      <c r="AB197" s="16"/>
+      <c r="X197" s="12">
+        <v>3</v>
+      </c>
+      <c r="Y197" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z197" s="7">
+        <v>9</v>
+      </c>
+      <c r="AA197" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB197" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="198" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A198">
@@ -6741,13 +7462,24 @@
       <c r="Q198" s="9"/>
       <c r="R198" s="9"/>
       <c r="S198" s="9"/>
-      <c r="T198" s="14"/>
-      <c r="V198" s="28" t="s">
+      <c r="T198" s="10"/>
+      <c r="U198" s="7"/>
+      <c r="V198" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="X198" s="14"/>
-      <c r="Y198" s="28" t="s">
-        <v>12</v>
+      <c r="W198" s="7"/>
+      <c r="X198" s="12"/>
+      <c r="Y198" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z198" s="7">
+        <v>7</v>
+      </c>
+      <c r="AA198" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB198" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:28" x14ac:dyDescent="0.25">
@@ -6782,23 +7514,33 @@
       <c r="Q199" s="14"/>
       <c r="R199" s="14"/>
       <c r="S199" s="14"/>
-      <c r="T199" s="14"/>
-      <c r="U199" s="16">
+      <c r="T199" s="10">
         <v>3</v>
       </c>
-      <c r="V199" s="16">
+      <c r="U199" s="18">
+        <v>3</v>
+      </c>
+      <c r="V199" s="18">
         <v>1</v>
       </c>
-      <c r="W199" s="16">
+      <c r="W199" s="18">
         <v>2</v>
       </c>
-      <c r="X199" s="15"/>
-      <c r="Y199" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z199" s="27"/>
-      <c r="AA199" s="15"/>
-      <c r="AB199" s="15"/>
+      <c r="X199" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y199" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z199" s="7">
+        <v>6</v>
+      </c>
+      <c r="AA199" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB199" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="200" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A200">
@@ -6832,14 +7574,24 @@
       <c r="Q200" s="14"/>
       <c r="R200" s="14"/>
       <c r="S200" s="14"/>
-      <c r="T200" s="14"/>
-      <c r="U200" s="16"/>
-      <c r="V200" s="28" t="s">
+      <c r="T200" s="10"/>
+      <c r="U200" s="18"/>
+      <c r="V200" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="W200" s="16"/>
-      <c r="Y200" s="28" t="s">
-        <v>12</v>
+      <c r="W200" s="18"/>
+      <c r="X200" s="8"/>
+      <c r="Y200" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z200" s="7">
+        <v>5</v>
+      </c>
+      <c r="AA200" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB200" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:28" x14ac:dyDescent="0.25">
@@ -6871,14 +7623,24 @@
       <c r="L201" s="7"/>
       <c r="M201" s="8"/>
       <c r="P201" s="8"/>
-      <c r="T201" s="16"/>
-      <c r="U201" s="16"/>
-      <c r="V201" s="28" t="s">
+      <c r="T201" s="17"/>
+      <c r="U201" s="18"/>
+      <c r="V201" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="W201" s="16"/>
-      <c r="Y201" s="28" t="s">
-        <v>12</v>
+      <c r="W201" s="18"/>
+      <c r="X201" s="8"/>
+      <c r="Y201" s="7">
+        <v>3</v>
+      </c>
+      <c r="Z201" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA201" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB201" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:28" x14ac:dyDescent="0.25">
@@ -6949,15 +7711,27 @@
       <c r="W202" s="9">
         <v>5</v>
       </c>
-      <c r="X202" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y202" s="9">
-        <v>2</v>
-      </c>
-      <c r="Z202" s="9">
-        <v>14</v>
-      </c>
+      <c r="X202" s="9"/>
+      <c r="Y202" s="7"/>
+      <c r="Z202" s="7"/>
+      <c r="AA202" s="7"/>
+      <c r="AB202" s="7"/>
+    </row>
+    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y203" s="7"/>
+      <c r="Z203" s="7"/>
+      <c r="AA203" s="7"/>
+      <c r="AB203" s="7"/>
+    </row>
+    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y204" s="7"/>
+      <c r="Z204" s="7"/>
+      <c r="AA204" s="7"/>
+      <c r="AB204" s="7"/>
+    </row>
+    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y205" s="9"/>
+      <c r="Z205" s="9"/>
     </row>
     <row r="206" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N206" t="s">
@@ -6980,8 +7754,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="Y166:AC186">
+    <sortCondition descending="1" ref="AC166:AC186"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
count number of occurrences at each recursion levl
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -630,7 +630,7 @@
   <dimension ref="A1:O188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,10 +984,10 @@
   <dimension ref="A1:AT209"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AG177" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL187" sqref="AL187"/>
+      <selection pane="bottomRight" activeCell="AM143" sqref="AM143:AN143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working version, optimized(get_floor()) and naive (get_floor_v1()) solution function
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1048,11 +1048,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT209"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AG177" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AG181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AM143" sqref="AM143:AN143"/>
+      <selection pane="bottomRight" activeCell="AM196" sqref="AM196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
search for efficient calculation of sums at each level
</commit_message>
<xml_diff>
--- a/solutions/fabergè_easter_eggs_crush_test.xlsx
+++ b/solutions/fabergè_easter_eggs_crush_test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="22">
   <si>
     <t>floor</t>
   </si>
@@ -89,6 +89,9 @@
   <si>
     <t>no. sub levels</t>
   </si>
+  <si>
+    <t>level 2 =</t>
+  </si>
 </sst>
 </file>
 
@@ -97,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -291,6 +302,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,1182 +618,1493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L188"/>
+  <dimension ref="A1:Y188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="6" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="5" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="11" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="54">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="54">
         <v>1.5</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
       <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
-      <c r="G1" s="36">
-        <v>1</v>
-      </c>
-      <c r="H1" s="31">
+      <c r="F1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="L1" s="36">
+        <v>1</v>
+      </c>
+      <c r="M1" s="31">
         <v>6</v>
       </c>
-      <c r="I1" s="31">
+      <c r="N1" s="31">
         <v>5</v>
       </c>
-      <c r="J1" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="54">
+      <c r="O1" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B2" s="54">
         <v>1.4</v>
       </c>
-      <c r="B2" s="54">
+      <c r="D2" s="54">
         <v>2.4</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55"/>
-      <c r="G2" s="36">
-        <v>1</v>
-      </c>
-      <c r="H2" s="31">
+      <c r="F2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="J2" s="55"/>
+      <c r="L2" s="36">
+        <v>1</v>
+      </c>
+      <c r="M2" s="31">
         <v>5</v>
       </c>
-      <c r="I2" s="31">
+      <c r="N2" s="31">
         <v>5</v>
       </c>
-      <c r="J2" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
+      <c r="O2" s="43">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="54">
         <v>1.3</v>
       </c>
-      <c r="B3" s="54">
+      <c r="D3" s="54">
         <v>2.4</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="G3" s="6">
-        <v>2</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="F3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="L3" s="6">
+        <v>2</v>
+      </c>
+      <c r="M3" s="7">
         <v>6</v>
       </c>
-      <c r="I3" s="7">
-        <v>4</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54">
+      <c r="N3" s="7">
+        <v>4</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="54"/>
+      <c r="D4" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C4" s="55">
+      <c r="F4" s="55">
         <v>3.3</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="G4" s="36">
-        <v>1</v>
-      </c>
-      <c r="H4" s="31">
-        <v>4</v>
-      </c>
-      <c r="I4" s="31">
+      <c r="H4" s="54"/>
+      <c r="J4" s="55"/>
+      <c r="L4" s="36">
+        <v>1</v>
+      </c>
+      <c r="M4" s="31">
+        <v>4</v>
+      </c>
+      <c r="N4" s="31">
         <v>5</v>
       </c>
-      <c r="J4" s="43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
+      <c r="O4" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="54">
         <v>1.2</v>
       </c>
-      <c r="B5" s="54">
+      <c r="D5" s="54">
         <v>2.4</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55"/>
-      <c r="G5" s="45">
-        <v>2</v>
-      </c>
-      <c r="H5" s="46">
+      <c r="F5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="J5" s="55"/>
+      <c r="L5" s="45">
+        <v>2</v>
+      </c>
+      <c r="M5" s="46">
         <v>6</v>
       </c>
-      <c r="I5" s="46">
-        <v>4</v>
-      </c>
-      <c r="J5" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54">
+      <c r="N5" s="46">
+        <v>4</v>
+      </c>
+      <c r="O5" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="54"/>
+      <c r="D6" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C6" s="55">
+      <c r="F6" s="55">
         <v>3.3</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="G6" s="45">
-        <v>2</v>
-      </c>
-      <c r="H6" s="46">
+      <c r="H6" s="54"/>
+      <c r="J6" s="55"/>
+      <c r="L6" s="45">
+        <v>2</v>
+      </c>
+      <c r="M6" s="46">
         <v>5</v>
       </c>
-      <c r="I6" s="46">
-        <v>4</v>
-      </c>
-      <c r="J6" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="54">
+      <c r="N6" s="46">
+        <v>4</v>
+      </c>
+      <c r="O6" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="54"/>
+      <c r="D7" s="54">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="55">
+      <c r="F7" s="55">
         <v>3.3</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="G7" s="6">
-        <v>3</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="H7" s="54"/>
+      <c r="J7" s="55"/>
+      <c r="L7" s="6">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7">
         <v>6</v>
       </c>
-      <c r="I7" s="7">
-        <v>3</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
+      <c r="N7" s="7">
+        <v>3</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="54"/>
-      <c r="C8" s="55">
+      <c r="D8" s="54"/>
+      <c r="F8" s="55">
         <v>3.2</v>
       </c>
-      <c r="D8" s="55">
+      <c r="H8" s="55">
         <v>4.2</v>
       </c>
-      <c r="E8" s="55"/>
-      <c r="G8" s="36">
-        <v>1</v>
-      </c>
-      <c r="H8" s="31">
-        <v>3</v>
-      </c>
-      <c r="I8" s="31">
+      <c r="J8" s="55"/>
+      <c r="L8" s="36">
+        <v>1</v>
+      </c>
+      <c r="M8" s="31">
+        <v>3</v>
+      </c>
+      <c r="N8" s="31">
         <v>5</v>
       </c>
-      <c r="J8" s="43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+      <c r="O8" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="54">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B9" s="54">
+      <c r="D9" s="54">
         <v>2.4</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="G9" s="45">
-        <v>2</v>
-      </c>
-      <c r="H9" s="46">
+      <c r="F9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="J9" s="55"/>
+      <c r="L9" s="45">
+        <v>2</v>
+      </c>
+      <c r="M9" s="46">
         <v>6</v>
       </c>
-      <c r="I9" s="46">
-        <v>4</v>
-      </c>
-      <c r="J9" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54">
+      <c r="N9" s="46">
+        <v>4</v>
+      </c>
+      <c r="O9" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="54"/>
+      <c r="D10" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C10" s="55">
+      <c r="F10" s="55">
         <v>3.3</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="G10" s="45">
-        <v>2</v>
-      </c>
-      <c r="H10" s="46">
+      <c r="H10" s="54"/>
+      <c r="J10" s="55"/>
+      <c r="L10" s="45">
+        <v>2</v>
+      </c>
+      <c r="M10" s="46">
         <v>5</v>
       </c>
-      <c r="I10" s="46">
-        <v>4</v>
-      </c>
-      <c r="J10" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54">
+      <c r="N10" s="46">
+        <v>4</v>
+      </c>
+      <c r="O10" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="54"/>
+      <c r="D11" s="54">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" s="55">
+      <c r="F11" s="55">
         <v>3.3</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="G11" s="6">
-        <v>3</v>
-      </c>
-      <c r="H11" s="7">
+      <c r="H11" s="54"/>
+      <c r="J11" s="55"/>
+      <c r="L11" s="6">
+        <v>3</v>
+      </c>
+      <c r="M11" s="7">
         <v>6</v>
       </c>
-      <c r="I11" s="7">
-        <v>3</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="N11" s="7">
+        <v>3</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="56">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <f>SUM(R11:W11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="54"/>
-      <c r="C12" s="55">
+      <c r="D12" s="54"/>
+      <c r="F12" s="55">
         <v>3.2</v>
       </c>
-      <c r="D12" s="55">
+      <c r="H12" s="55">
         <v>4.2</v>
       </c>
-      <c r="E12" s="55"/>
-      <c r="G12" s="45">
-        <v>2</v>
-      </c>
-      <c r="H12" s="46">
-        <v>4</v>
-      </c>
-      <c r="I12" s="46">
-        <v>4</v>
-      </c>
-      <c r="J12" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54">
+      <c r="J12" s="55"/>
+      <c r="L12" s="45">
+        <v>2</v>
+      </c>
+      <c r="M12" s="46">
+        <v>4</v>
+      </c>
+      <c r="N12" s="46">
+        <v>4</v>
+      </c>
+      <c r="O12" s="47">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="56">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
+      <c r="U12">
+        <v>4</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" ref="Y12:Y22" si="0">SUM(R12:W12)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="D13" s="54">
         <v>2.1</v>
       </c>
-      <c r="C13" s="55">
+      <c r="F13" s="55">
         <v>3.3</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="G13" s="48">
-        <v>3</v>
-      </c>
-      <c r="H13" s="49">
+      <c r="H13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="L13" s="48">
+        <v>3</v>
+      </c>
+      <c r="M13" s="49">
         <v>6</v>
       </c>
-      <c r="I13" s="49">
-        <v>3</v>
-      </c>
-      <c r="J13" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="N13" s="49">
+        <v>3</v>
+      </c>
+      <c r="O13" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="56">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>3</v>
+      </c>
+      <c r="T13">
+        <v>6</v>
+      </c>
+      <c r="U13">
+        <v>10</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
-      <c r="C14" s="55">
+      <c r="D14" s="54"/>
+      <c r="F14" s="55">
         <v>3.2</v>
       </c>
-      <c r="D14" s="55">
+      <c r="H14" s="55">
         <v>4.2</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="G14" s="48">
-        <v>3</v>
-      </c>
-      <c r="H14" s="49">
+      <c r="J14" s="55"/>
+      <c r="L14" s="48">
+        <v>3</v>
+      </c>
+      <c r="M14" s="49">
         <v>5</v>
       </c>
-      <c r="I14" s="49">
-        <v>3</v>
-      </c>
-      <c r="J14" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="N14" s="49">
+        <v>3</v>
+      </c>
+      <c r="O14" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="56">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>4</v>
+      </c>
+      <c r="T14">
+        <v>10</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="54"/>
-      <c r="C15" s="55">
+      <c r="D15" s="54"/>
+      <c r="F15" s="55">
         <v>3.1</v>
       </c>
-      <c r="D15" s="55">
+      <c r="H15" s="55">
         <v>4.2</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="G15" s="6">
-        <v>4</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="J15" s="55"/>
+      <c r="L15" s="6">
+        <v>4</v>
+      </c>
+      <c r="M15" s="7">
         <v>6</v>
       </c>
-      <c r="I15" s="7">
-        <v>2</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="N15" s="7">
+        <v>2</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="56">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="54"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55">
+      <c r="D16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="H16" s="55">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E16" s="55">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G16" s="36">
-        <v>1</v>
-      </c>
-      <c r="H16" s="31">
-        <v>2</v>
-      </c>
-      <c r="I16" s="31">
+      <c r="L16" s="36">
+        <v>1</v>
+      </c>
+      <c r="M16" s="31">
+        <v>2</v>
+      </c>
+      <c r="N16" s="31">
         <v>5</v>
       </c>
-      <c r="J16" s="43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
-        <v>1</v>
+      <c r="O16" s="43">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="56"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31</v>
       </c>
       <c r="B17" s="54">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="54">
         <v>2.4</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="55"/>
-      <c r="G17" s="45">
-        <v>2</v>
-      </c>
-      <c r="H17" s="46">
+      <c r="F17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="J17" s="55"/>
+      <c r="L17" s="45">
+        <v>2</v>
+      </c>
+      <c r="M17" s="46">
         <v>6</v>
       </c>
-      <c r="I17" s="46">
-        <v>4</v>
-      </c>
-      <c r="J17" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54">
+      <c r="N17" s="46">
+        <v>4</v>
+      </c>
+      <c r="O17" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="56">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="54">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C18" s="55">
+      <c r="F18" s="55">
         <v>3.3</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
-      <c r="G18" s="45">
-        <v>2</v>
-      </c>
-      <c r="H18" s="46">
+      <c r="H18" s="54"/>
+      <c r="J18" s="55"/>
+      <c r="L18" s="45">
+        <v>2</v>
+      </c>
+      <c r="M18" s="46">
         <v>5</v>
       </c>
-      <c r="I18" s="46">
-        <v>4</v>
-      </c>
-      <c r="J18" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54">
+      <c r="N18" s="46">
+        <v>4</v>
+      </c>
+      <c r="O18" s="47">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="56">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>2</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="U18">
+        <v>4</v>
+      </c>
+      <c r="V18">
+        <v>5</v>
+      </c>
+      <c r="W18">
+        <v>6</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="54">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C19" s="55">
+      <c r="F19" s="55">
         <v>3.3</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="G19" s="6">
-        <v>3</v>
-      </c>
-      <c r="H19" s="7">
+      <c r="H19" s="54"/>
+      <c r="J19" s="55"/>
+      <c r="L19" s="6">
+        <v>3</v>
+      </c>
+      <c r="M19" s="7">
         <v>6</v>
       </c>
-      <c r="I19" s="7">
-        <v>3</v>
-      </c>
-      <c r="J19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="N19" s="7">
+        <v>3</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="56">
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+      <c r="T19">
+        <v>6</v>
+      </c>
+      <c r="U19">
+        <v>10</v>
+      </c>
+      <c r="V19">
+        <v>15</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="54"/>
-      <c r="C20" s="55">
+      <c r="D20" s="54"/>
+      <c r="F20" s="55">
         <v>3.2</v>
       </c>
-      <c r="D20" s="55">
+      <c r="H20" s="55">
         <v>4.2</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="G20" s="45">
-        <v>2</v>
-      </c>
-      <c r="H20" s="46">
-        <v>4</v>
-      </c>
-      <c r="I20" s="46">
-        <v>4</v>
-      </c>
-      <c r="J20" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54">
+      <c r="J20" s="55"/>
+      <c r="L20" s="45">
+        <v>2</v>
+      </c>
+      <c r="M20" s="46">
+        <v>4</v>
+      </c>
+      <c r="N20" s="46">
+        <v>4</v>
+      </c>
+      <c r="O20" s="47">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="56">
+        <v>4</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>4</v>
+      </c>
+      <c r="T20">
+        <v>10</v>
+      </c>
+      <c r="U20">
+        <v>20</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" s="54">
         <v>2.1</v>
       </c>
-      <c r="C21" s="55">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="55">
         <v>3.3</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="G21" s="48">
-        <v>3</v>
-      </c>
-      <c r="H21" s="49">
+      <c r="H21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="L21" s="48">
+        <v>3</v>
+      </c>
+      <c r="M21" s="49">
         <v>6</v>
       </c>
-      <c r="I21" s="49">
-        <v>3</v>
-      </c>
-      <c r="J21" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="N21" s="49">
+        <v>3</v>
+      </c>
+      <c r="O21" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="56">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <v>15</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="54"/>
-      <c r="C22" s="55">
+      <c r="D22" s="54"/>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="55">
         <v>3.2</v>
       </c>
-      <c r="D22" s="55">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="55">
         <v>4.2</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="G22" s="48">
-        <v>3</v>
-      </c>
-      <c r="H22" s="49">
+      <c r="J22" s="55"/>
+      <c r="L22" s="48">
+        <v>3</v>
+      </c>
+      <c r="M22" s="49">
         <v>5</v>
       </c>
-      <c r="I22" s="49">
-        <v>3</v>
-      </c>
-      <c r="J22" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="N22" s="49">
+        <v>3</v>
+      </c>
+      <c r="O22" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="56">
+        <v>6</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>6</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="54"/>
-      <c r="C23" s="55">
+      <c r="D23" s="54"/>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" s="55">
         <v>3.1</v>
       </c>
-      <c r="D23" s="55">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="55">
         <v>4.2</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="G23" s="6">
-        <v>4</v>
-      </c>
-      <c r="H23" s="7">
+      <c r="J23" s="55"/>
+      <c r="L23" s="6">
+        <v>4</v>
+      </c>
+      <c r="M23" s="7">
         <v>6</v>
       </c>
-      <c r="I23" s="7">
-        <v>2</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="N23" s="7">
+        <v>2</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55">
+      <c r="D24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" s="55">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E24" s="55">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G24" s="45">
-        <v>2</v>
-      </c>
-      <c r="H24" s="46">
-        <v>3</v>
-      </c>
-      <c r="I24" s="46">
-        <v>4</v>
-      </c>
-      <c r="J24" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="55">
-        <v>2</v>
-      </c>
-      <c r="C25" s="55">
+      <c r="L24" s="45">
+        <v>2</v>
+      </c>
+      <c r="M24" s="46">
+        <v>3</v>
+      </c>
+      <c r="N24" s="46">
+        <v>4</v>
+      </c>
+      <c r="O24" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25" s="55">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="55">
         <v>3.3</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="G25" s="48">
-        <v>3</v>
-      </c>
-      <c r="H25" s="49">
+      <c r="H25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="L25" s="48">
+        <v>3</v>
+      </c>
+      <c r="M25" s="49">
         <v>6</v>
       </c>
-      <c r="I25" s="49">
-        <v>3</v>
-      </c>
-      <c r="J25" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55">
+      <c r="N25" s="49">
+        <v>3</v>
+      </c>
+      <c r="O25" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="55">
         <v>3.2</v>
       </c>
-      <c r="D26" s="55">
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="55">
         <v>4.2</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="G26" s="48">
-        <v>3</v>
-      </c>
-      <c r="H26" s="49">
+      <c r="J26" s="55"/>
+      <c r="L26" s="48">
+        <v>3</v>
+      </c>
+      <c r="M26" s="49">
         <v>5</v>
       </c>
-      <c r="I26" s="49">
-        <v>3</v>
-      </c>
-      <c r="J26" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55">
+      <c r="N26" s="49">
+        <v>3</v>
+      </c>
+      <c r="O26" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" s="55">
         <v>3.1</v>
       </c>
-      <c r="D27" s="55">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" s="55">
         <v>4.2</v>
       </c>
-      <c r="E27" s="55"/>
-      <c r="G27" s="6">
-        <v>4</v>
-      </c>
-      <c r="H27" s="7">
+      <c r="J27" s="55"/>
+      <c r="L27" s="6">
+        <v>4</v>
+      </c>
+      <c r="M27" s="7">
         <v>6</v>
       </c>
-      <c r="I27" s="7">
-        <v>2</v>
-      </c>
-      <c r="J27" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55">
+      <c r="N27" s="7">
+        <v>2</v>
+      </c>
+      <c r="O27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" s="55">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E28" s="55">
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G28" s="48">
-        <v>3</v>
-      </c>
-      <c r="H28" s="49">
-        <v>4</v>
-      </c>
-      <c r="I28" s="49">
-        <v>3</v>
-      </c>
-      <c r="J28" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55">
-        <v>3</v>
-      </c>
-      <c r="D29" s="55">
+      <c r="L28" s="48">
+        <v>3</v>
+      </c>
+      <c r="M28" s="49">
+        <v>4</v>
+      </c>
+      <c r="N28" s="49">
+        <v>3</v>
+      </c>
+      <c r="O28" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29" s="55">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="55">
         <v>4.2</v>
       </c>
-      <c r="E29" s="55"/>
-      <c r="G29" s="51">
-        <v>4</v>
-      </c>
-      <c r="H29" s="52">
+      <c r="J29" s="55"/>
+      <c r="L29" s="51">
+        <v>4</v>
+      </c>
+      <c r="M29" s="52">
         <v>6</v>
       </c>
-      <c r="I29" s="52">
-        <v>2</v>
-      </c>
-      <c r="J29" s="53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55">
+      <c r="N29" s="52">
+        <v>2</v>
+      </c>
+      <c r="O29" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30" s="55">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E30" s="55">
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G30" s="51">
-        <v>4</v>
-      </c>
-      <c r="H30" s="52">
+      <c r="L30" s="51">
+        <v>4</v>
+      </c>
+      <c r="M30" s="52">
         <v>5</v>
       </c>
-      <c r="I30" s="52">
-        <v>2</v>
-      </c>
-      <c r="J30" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55">
-        <v>4</v>
-      </c>
-      <c r="E31" s="55">
+      <c r="N30" s="52">
+        <v>2</v>
+      </c>
+      <c r="O30" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31" s="55">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="55">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G31" s="6">
+      <c r="L31" s="6">
         <v>5</v>
       </c>
-      <c r="H31" s="7">
+      <c r="M31" s="7">
         <v>6</v>
       </c>
-      <c r="I31" s="7">
-        <v>1</v>
-      </c>
-      <c r="J31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="55">
+      <c r="N31" s="7">
+        <v>1</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" s="55">
         <v>5</v>
       </c>
-      <c r="G32" s="36">
-        <v>1</v>
-      </c>
-      <c r="H32" s="31">
-        <v>1</v>
-      </c>
-      <c r="I32" s="31">
+      <c r="L32" s="36">
+        <v>1</v>
+      </c>
+      <c r="M32" s="31">
+        <v>1</v>
+      </c>
+      <c r="N32" s="31">
         <v>5</v>
       </c>
-      <c r="J32" s="43">
+      <c r="O32" s="43">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G33" s="45">
-        <v>2</v>
-      </c>
-      <c r="H33" s="46">
+    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="45">
+        <v>2</v>
+      </c>
+      <c r="M33" s="46">
         <v>6</v>
       </c>
-      <c r="I33" s="46">
-        <v>4</v>
-      </c>
-      <c r="J33" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G34" s="45">
-        <v>2</v>
-      </c>
-      <c r="H34" s="46">
+      <c r="N33" s="46">
+        <v>4</v>
+      </c>
+      <c r="O33" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L34" s="45">
+        <v>2</v>
+      </c>
+      <c r="M34" s="46">
         <v>5</v>
       </c>
-      <c r="I34" s="46">
-        <v>4</v>
-      </c>
-      <c r="J34" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G35" s="6">
-        <v>3</v>
-      </c>
-      <c r="H35" s="7">
+      <c r="N34" s="46">
+        <v>4</v>
+      </c>
+      <c r="O34" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L35" s="6">
+        <v>3</v>
+      </c>
+      <c r="M35" s="7">
         <v>6</v>
       </c>
-      <c r="I35" s="7">
-        <v>3</v>
-      </c>
-      <c r="J35" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="45">
-        <v>2</v>
-      </c>
-      <c r="H36" s="46">
-        <v>4</v>
-      </c>
-      <c r="I36" s="46">
-        <v>4</v>
-      </c>
-      <c r="J36" s="47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G37" s="48">
-        <v>3</v>
-      </c>
-      <c r="H37" s="49">
+      <c r="N35" s="7">
+        <v>3</v>
+      </c>
+      <c r="O35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L36" s="45">
+        <v>2</v>
+      </c>
+      <c r="M36" s="46">
+        <v>4</v>
+      </c>
+      <c r="N36" s="46">
+        <v>4</v>
+      </c>
+      <c r="O36" s="47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L37" s="48">
+        <v>3</v>
+      </c>
+      <c r="M37" s="49">
         <v>6</v>
       </c>
-      <c r="I37" s="49">
-        <v>3</v>
-      </c>
-      <c r="J37" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G38" s="48">
-        <v>3</v>
-      </c>
-      <c r="H38" s="49">
+      <c r="N37" s="49">
+        <v>3</v>
+      </c>
+      <c r="O37" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L38" s="48">
+        <v>3</v>
+      </c>
+      <c r="M38" s="49">
         <v>5</v>
       </c>
-      <c r="I38" s="49">
-        <v>3</v>
-      </c>
-      <c r="J38" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G39" s="6">
-        <v>2</v>
-      </c>
-      <c r="H39" s="7">
+      <c r="N38" s="49">
+        <v>3</v>
+      </c>
+      <c r="O38" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L39" s="6">
+        <v>2</v>
+      </c>
+      <c r="M39" s="7">
         <v>6</v>
       </c>
-      <c r="I39" s="7">
-        <v>2</v>
-      </c>
-      <c r="J39" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="45">
-        <v>2</v>
-      </c>
-      <c r="H40" s="46">
-        <v>3</v>
-      </c>
-      <c r="I40" s="46">
-        <v>4</v>
-      </c>
-      <c r="J40" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G41" s="48">
-        <v>3</v>
-      </c>
-      <c r="H41" s="49">
+      <c r="N39" s="7">
+        <v>2</v>
+      </c>
+      <c r="O39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L40" s="45">
+        <v>2</v>
+      </c>
+      <c r="M40" s="46">
+        <v>3</v>
+      </c>
+      <c r="N40" s="46">
+        <v>4</v>
+      </c>
+      <c r="O40" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L41" s="48">
+        <v>3</v>
+      </c>
+      <c r="M41" s="49">
         <v>6</v>
       </c>
-      <c r="I41" s="49">
-        <v>3</v>
-      </c>
-      <c r="J41" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G42" s="48">
-        <v>3</v>
-      </c>
-      <c r="H42" s="49">
+      <c r="N41" s="49">
+        <v>3</v>
+      </c>
+      <c r="O41" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L42" s="48">
+        <v>3</v>
+      </c>
+      <c r="M42" s="49">
         <v>5</v>
       </c>
-      <c r="I42" s="49">
-        <v>3</v>
-      </c>
-      <c r="J42" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G43" s="6">
-        <v>4</v>
-      </c>
-      <c r="H43" s="7">
+      <c r="N42" s="49">
+        <v>3</v>
+      </c>
+      <c r="O42" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L43" s="6">
+        <v>4</v>
+      </c>
+      <c r="M43" s="7">
         <v>6</v>
       </c>
-      <c r="I43" s="7">
-        <v>2</v>
-      </c>
-      <c r="J43" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G44" s="48">
-        <v>3</v>
-      </c>
-      <c r="H44" s="49">
-        <v>4</v>
-      </c>
-      <c r="I44" s="49">
-        <v>3</v>
-      </c>
-      <c r="J44" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G45" s="51">
-        <v>4</v>
-      </c>
-      <c r="H45" s="52">
+      <c r="N43" s="7">
+        <v>2</v>
+      </c>
+      <c r="O43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L44" s="48">
+        <v>3</v>
+      </c>
+      <c r="M44" s="49">
+        <v>4</v>
+      </c>
+      <c r="N44" s="49">
+        <v>3</v>
+      </c>
+      <c r="O44" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L45" s="51">
+        <v>4</v>
+      </c>
+      <c r="M45" s="52">
         <v>6</v>
       </c>
-      <c r="I45" s="52">
-        <v>2</v>
-      </c>
-      <c r="J45" s="53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G46" s="51">
-        <v>4</v>
-      </c>
-      <c r="H46" s="52">
+      <c r="N45" s="52">
+        <v>2</v>
+      </c>
+      <c r="O45" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L46" s="51">
+        <v>4</v>
+      </c>
+      <c r="M46" s="52">
         <v>5</v>
       </c>
-      <c r="I46" s="52">
-        <v>2</v>
-      </c>
-      <c r="J46" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G47" s="6">
+      <c r="N46" s="52">
+        <v>2</v>
+      </c>
+      <c r="O46" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L47" s="6">
         <v>5</v>
       </c>
-      <c r="H47" s="7">
+      <c r="M47" s="7">
         <v>6</v>
       </c>
-      <c r="I47" s="7">
-        <v>1</v>
-      </c>
-      <c r="J47" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G48" s="45">
-        <v>2</v>
-      </c>
-      <c r="H48" s="46">
-        <v>2</v>
-      </c>
-      <c r="I48" s="46">
-        <v>4</v>
-      </c>
-      <c r="J48" s="47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G49" s="48">
-        <v>3</v>
-      </c>
-      <c r="H49" s="49">
+      <c r="N47" s="7">
+        <v>1</v>
+      </c>
+      <c r="O47" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L48" s="45">
+        <v>2</v>
+      </c>
+      <c r="M48" s="46">
+        <v>2</v>
+      </c>
+      <c r="N48" s="46">
+        <v>4</v>
+      </c>
+      <c r="O48" s="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L49" s="48">
+        <v>3</v>
+      </c>
+      <c r="M49" s="49">
         <v>6</v>
       </c>
-      <c r="I49" s="49">
-        <v>3</v>
-      </c>
-      <c r="J49" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G50" s="48">
-        <v>3</v>
-      </c>
-      <c r="H50" s="49">
+      <c r="N49" s="49">
+        <v>3</v>
+      </c>
+      <c r="O49" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L50" s="48">
+        <v>3</v>
+      </c>
+      <c r="M50" s="49">
         <v>5</v>
       </c>
-      <c r="I50" s="49">
-        <v>3</v>
-      </c>
-      <c r="J50" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G51" s="6">
-        <v>4</v>
-      </c>
-      <c r="H51" s="7">
+      <c r="N50" s="49">
+        <v>3</v>
+      </c>
+      <c r="O50" s="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L51" s="6">
+        <v>4</v>
+      </c>
+      <c r="M51" s="7">
         <v>6</v>
       </c>
-      <c r="I51" s="7">
-        <v>2</v>
-      </c>
-      <c r="J51" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G52" s="48">
-        <v>3</v>
-      </c>
-      <c r="H52" s="49">
-        <v>4</v>
-      </c>
-      <c r="I52" s="49">
-        <v>3</v>
-      </c>
-      <c r="J52" s="50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G53" s="51">
-        <v>4</v>
-      </c>
-      <c r="H53" s="52">
+      <c r="N51" s="7">
+        <v>2</v>
+      </c>
+      <c r="O51" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L52" s="48">
+        <v>3</v>
+      </c>
+      <c r="M52" s="49">
+        <v>4</v>
+      </c>
+      <c r="N52" s="49">
+        <v>3</v>
+      </c>
+      <c r="O52" s="50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L53" s="51">
+        <v>4</v>
+      </c>
+      <c r="M53" s="52">
         <v>6</v>
       </c>
-      <c r="I53" s="52">
-        <v>2</v>
-      </c>
-      <c r="J53" s="53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G54" s="51">
-        <v>4</v>
-      </c>
-      <c r="H54" s="52">
+      <c r="N53" s="52">
+        <v>2</v>
+      </c>
+      <c r="O53" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L54" s="51">
+        <v>4</v>
+      </c>
+      <c r="M54" s="52">
         <v>5</v>
       </c>
-      <c r="I54" s="52">
-        <v>2</v>
-      </c>
-      <c r="J54" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G55" s="6">
+      <c r="N54" s="52">
+        <v>2</v>
+      </c>
+      <c r="O54" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L55" s="6">
         <v>5</v>
       </c>
-      <c r="H55" s="7">
+      <c r="M55" s="7">
         <v>6</v>
       </c>
-      <c r="I55" s="7">
-        <v>1</v>
-      </c>
-      <c r="J55" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G56" s="48">
-        <v>3</v>
-      </c>
-      <c r="H56" s="49">
-        <v>3</v>
-      </c>
-      <c r="I56" s="49">
-        <v>3</v>
-      </c>
-      <c r="J56" s="50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G57" s="51">
-        <v>4</v>
-      </c>
-      <c r="H57" s="52">
+      <c r="N55" s="7">
+        <v>1</v>
+      </c>
+      <c r="O55" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L56" s="48">
+        <v>3</v>
+      </c>
+      <c r="M56" s="49">
+        <v>3</v>
+      </c>
+      <c r="N56" s="49">
+        <v>3</v>
+      </c>
+      <c r="O56" s="50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L57" s="51">
+        <v>4</v>
+      </c>
+      <c r="M57" s="52">
         <v>6</v>
       </c>
-      <c r="I57" s="52">
-        <v>2</v>
-      </c>
-      <c r="J57" s="53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G58" s="51">
-        <v>4</v>
-      </c>
-      <c r="H58" s="52">
+      <c r="N57" s="52">
+        <v>2</v>
+      </c>
+      <c r="O57" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L58" s="51">
+        <v>4</v>
+      </c>
+      <c r="M58" s="52">
         <v>5</v>
       </c>
-      <c r="I58" s="52">
-        <v>2</v>
-      </c>
-      <c r="J58" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G59" s="6">
+      <c r="N58" s="52">
+        <v>2</v>
+      </c>
+      <c r="O58" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L59" s="6">
         <v>5</v>
       </c>
-      <c r="H59" s="7">
+      <c r="M59" s="7">
         <v>6</v>
       </c>
-      <c r="I59" s="7">
-        <v>1</v>
-      </c>
-      <c r="J59" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G60" s="51">
-        <v>4</v>
-      </c>
-      <c r="H60" s="52">
-        <v>4</v>
-      </c>
-      <c r="I60" s="52">
-        <v>2</v>
-      </c>
-      <c r="J60" s="53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G61" s="6">
+      <c r="N59" s="7">
+        <v>1</v>
+      </c>
+      <c r="O59" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L60" s="51">
+        <v>4</v>
+      </c>
+      <c r="M60" s="52">
+        <v>4</v>
+      </c>
+      <c r="N60" s="52">
+        <v>2</v>
+      </c>
+      <c r="O60" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L61" s="6">
         <v>5</v>
       </c>
-      <c r="H61" s="7">
+      <c r="M61" s="7">
         <v>6</v>
       </c>
-      <c r="I61" s="7">
-        <v>1</v>
-      </c>
-      <c r="J61" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G62" s="6">
+      <c r="N61" s="7">
+        <v>1</v>
+      </c>
+      <c r="O61" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L62" s="6">
         <v>5</v>
       </c>
-      <c r="H62" s="7">
+      <c r="M62" s="7">
         <v>5</v>
       </c>
-      <c r="I62" s="7">
-        <v>1</v>
-      </c>
-      <c r="J62" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G63" s="6">
-        <v>0</v>
-      </c>
-      <c r="H63" s="7">
-        <v>0</v>
-      </c>
-      <c r="I63" s="7">
+      <c r="N62" s="7">
+        <v>1</v>
+      </c>
+      <c r="O62" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L63" s="6">
+        <v>0</v>
+      </c>
+      <c r="M63" s="7">
+        <v>0</v>
+      </c>
+      <c r="N63" s="7">
         <v>5</v>
       </c>
-      <c r="J63" s="8">
+      <c r="O63" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L188" s="2"/>
+    <row r="188" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q188" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>